<commit_message>
Added the requested information for test case 83
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111PHILIPSXXXX/Philips/VuePACS-SignPlugin/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111PHILIPSXXXX/Philips/VuePACS-SignPlugin/1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.philips.com/sites/HCISIntegration260/Integration Project Docs/EAMER/Italy/FSE 2.0/Accreditamento/file da sottomettere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE52BFD0-DB17-4D96-B339-AAF8336BD1BA}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CB7C22D-675F-40F0-B654-C37BF000EE54}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="885">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4612,6 +4612,9 @@
   </si>
   <si>
     <t>Il Sistema non prevede il campo opzionale "documentationOf"</t>
+  </si>
+  <si>
+    <t>Non riceviamo alcun errore dal servizio</t>
   </si>
 </sst>
 </file>
@@ -5033,29 +5036,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -5073,6 +5053,29 @@
     </xf>
     <xf numFmtId="11" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7531,10 +7534,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B220" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B265" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A222" sqref="A222"/>
+      <selection pane="bottomRight" activeCell="B266" sqref="B266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -7573,11 +7576,11 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="43" t="s">
         <v>833</v>
       </c>
       <c r="D2" s="44"/>
@@ -7598,11 +7601,11 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="51" t="s">
         <v>830</v>
       </c>
       <c r="D3" s="44"/>
@@ -7623,9 +7626,9 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="43" t="s">
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="51" t="s">
         <v>831</v>
       </c>
       <c r="D4" s="44"/>
@@ -7647,9 +7650,9 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43" t="s">
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51" t="s">
         <v>832</v>
       </c>
       <c r="D5" s="44"/>
@@ -7670,8 +7673,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -14094,32 +14097,32 @@
       <c r="E195" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="F195" s="46">
+      <c r="F195" s="33">
         <v>45063</v>
       </c>
-      <c r="G195" s="47" t="s">
+      <c r="G195" s="34" t="s">
         <v>834</v>
       </c>
-      <c r="H195" s="47" t="s">
+      <c r="H195" s="34" t="s">
         <v>835</v>
       </c>
-      <c r="I195" s="47" t="s">
+      <c r="I195" s="34" t="s">
         <v>836</v>
       </c>
-      <c r="J195" s="48" t="s">
+      <c r="J195" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="K195" s="48"/>
-      <c r="L195" s="48"/>
-      <c r="M195" s="48"/>
-      <c r="N195" s="48"/>
-      <c r="O195" s="48"/>
-      <c r="P195" s="48"/>
-      <c r="Q195" s="48" t="s">
+      <c r="K195" s="35"/>
+      <c r="L195" s="35"/>
+      <c r="M195" s="35"/>
+      <c r="N195" s="35"/>
+      <c r="O195" s="35"/>
+      <c r="P195" s="35"/>
+      <c r="Q195" s="35" t="s">
         <v>827</v>
       </c>
-      <c r="R195" s="49"/>
-      <c r="S195" s="50"/>
+      <c r="R195" s="36"/>
+      <c r="S195" s="37"/>
       <c r="T195" s="28" t="s">
         <v>48</v>
       </c>
@@ -14140,24 +14143,24 @@
       <c r="E196" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="F196" s="46"/>
-      <c r="G196" s="47"/>
-      <c r="H196" s="47"/>
-      <c r="I196" s="47"/>
-      <c r="J196" s="48" t="s">
+      <c r="F196" s="33"/>
+      <c r="G196" s="34"/>
+      <c r="H196" s="34"/>
+      <c r="I196" s="34"/>
+      <c r="J196" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K196" s="48" t="s">
+      <c r="K196" s="35" t="s">
         <v>837</v>
       </c>
-      <c r="L196" s="48"/>
-      <c r="M196" s="48"/>
-      <c r="N196" s="48"/>
-      <c r="O196" s="48"/>
-      <c r="P196" s="48"/>
-      <c r="Q196" s="48"/>
-      <c r="R196" s="49"/>
-      <c r="S196" s="50"/>
+      <c r="L196" s="35"/>
+      <c r="M196" s="35"/>
+      <c r="N196" s="35"/>
+      <c r="O196" s="35"/>
+      <c r="P196" s="35"/>
+      <c r="Q196" s="35"/>
+      <c r="R196" s="36"/>
+      <c r="S196" s="37"/>
       <c r="T196" s="28" t="s">
         <v>48</v>
       </c>
@@ -14178,24 +14181,24 @@
       <c r="E197" s="22" t="s">
         <v>428</v>
       </c>
-      <c r="F197" s="46"/>
-      <c r="G197" s="47"/>
-      <c r="H197" s="47"/>
-      <c r="I197" s="47"/>
-      <c r="J197" s="48" t="s">
+      <c r="F197" s="33"/>
+      <c r="G197" s="34"/>
+      <c r="H197" s="34"/>
+      <c r="I197" s="34"/>
+      <c r="J197" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K197" s="48" t="s">
+      <c r="K197" s="35" t="s">
         <v>838</v>
       </c>
-      <c r="L197" s="48"/>
-      <c r="M197" s="48"/>
-      <c r="N197" s="48"/>
-      <c r="O197" s="48"/>
-      <c r="P197" s="48"/>
-      <c r="Q197" s="48"/>
-      <c r="R197" s="49"/>
-      <c r="S197" s="50"/>
+      <c r="L197" s="35"/>
+      <c r="M197" s="35"/>
+      <c r="N197" s="35"/>
+      <c r="O197" s="35"/>
+      <c r="P197" s="35"/>
+      <c r="Q197" s="35"/>
+      <c r="R197" s="36"/>
+      <c r="S197" s="37"/>
       <c r="T197" s="28" t="s">
         <v>48</v>
       </c>
@@ -14216,24 +14219,24 @@
       <c r="E198" s="22" t="s">
         <v>430</v>
       </c>
-      <c r="F198" s="46"/>
-      <c r="G198" s="47"/>
-      <c r="H198" s="47"/>
-      <c r="I198" s="47"/>
-      <c r="J198" s="48" t="s">
+      <c r="F198" s="33"/>
+      <c r="G198" s="34"/>
+      <c r="H198" s="34"/>
+      <c r="I198" s="34"/>
+      <c r="J198" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K198" s="48" t="s">
+      <c r="K198" s="35" t="s">
         <v>839</v>
       </c>
-      <c r="L198" s="48"/>
-      <c r="M198" s="48"/>
-      <c r="N198" s="48"/>
-      <c r="O198" s="48"/>
-      <c r="P198" s="48"/>
-      <c r="Q198" s="48"/>
-      <c r="R198" s="49"/>
-      <c r="S198" s="50"/>
+      <c r="L198" s="35"/>
+      <c r="M198" s="35"/>
+      <c r="N198" s="35"/>
+      <c r="O198" s="35"/>
+      <c r="P198" s="35"/>
+      <c r="Q198" s="35"/>
+      <c r="R198" s="36"/>
+      <c r="S198" s="37"/>
       <c r="T198" s="28" t="s">
         <v>48</v>
       </c>
@@ -14764,42 +14767,42 @@
       <c r="E214" s="22" t="s">
         <v>462</v>
       </c>
-      <c r="F214" s="46">
+      <c r="F214" s="33">
         <v>45063</v>
       </c>
-      <c r="G214" s="47" t="s">
+      <c r="G214" s="34" t="s">
         <v>840</v>
       </c>
-      <c r="H214" s="47" t="s">
+      <c r="H214" s="34" t="s">
         <v>841</v>
       </c>
-      <c r="I214" s="47" t="s">
+      <c r="I214" s="34" t="s">
         <v>842</v>
       </c>
-      <c r="J214" s="48" t="s">
+      <c r="J214" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="K214" s="48"/>
-      <c r="L214" s="48" t="s">
+      <c r="K214" s="35"/>
+      <c r="L214" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="M214" s="48" t="s">
+      <c r="M214" s="35" t="s">
         <v>843</v>
       </c>
-      <c r="N214" s="48" t="s">
+      <c r="N214" s="35" t="s">
         <v>844</v>
       </c>
-      <c r="O214" s="48" t="s">
+      <c r="O214" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="P214" s="48" t="s">
+      <c r="P214" s="35" t="s">
         <v>845</v>
       </c>
-      <c r="Q214" s="48" t="s">
+      <c r="Q214" s="35" t="s">
         <v>827</v>
       </c>
-      <c r="R214" s="49"/>
-      <c r="S214" s="50" t="s">
+      <c r="R214" s="36"/>
+      <c r="S214" s="37" t="s">
         <v>846</v>
       </c>
       <c r="T214" s="28" t="s">
@@ -15060,24 +15063,24 @@
       <c r="E222" s="22" t="s">
         <v>478</v>
       </c>
-      <c r="F222" s="46"/>
-      <c r="G222" s="47"/>
-      <c r="H222" s="47"/>
-      <c r="I222" s="47"/>
-      <c r="J222" s="48" t="s">
+      <c r="F222" s="33"/>
+      <c r="G222" s="34"/>
+      <c r="H222" s="34"/>
+      <c r="I222" s="34"/>
+      <c r="J222" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K222" s="48" t="s">
+      <c r="K222" s="35" t="s">
         <v>847</v>
       </c>
-      <c r="L222" s="48"/>
-      <c r="M222" s="48"/>
-      <c r="N222" s="48"/>
-      <c r="O222" s="48"/>
-      <c r="P222" s="48"/>
-      <c r="Q222" s="48"/>
-      <c r="R222" s="49"/>
-      <c r="S222" s="50"/>
+      <c r="L222" s="35"/>
+      <c r="M222" s="35"/>
+      <c r="N222" s="35"/>
+      <c r="O222" s="35"/>
+      <c r="P222" s="35"/>
+      <c r="Q222" s="35"/>
+      <c r="R222" s="36"/>
+      <c r="S222" s="37"/>
       <c r="T222" s="28" t="s">
         <v>51</v>
       </c>
@@ -15342,32 +15345,32 @@
       <c r="E230" s="22" t="s">
         <v>488</v>
       </c>
-      <c r="F230" s="46">
+      <c r="F230" s="33">
         <v>45063</v>
       </c>
-      <c r="G230" s="47" t="s">
+      <c r="G230" s="34" t="s">
         <v>848</v>
       </c>
-      <c r="H230" s="47"/>
-      <c r="I230" s="47"/>
-      <c r="J230" s="48" t="s">
+      <c r="H230" s="34"/>
+      <c r="I230" s="34"/>
+      <c r="J230" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="K230" s="48"/>
-      <c r="L230" s="48"/>
-      <c r="M230" s="48"/>
-      <c r="N230" s="48"/>
-      <c r="O230" s="48" t="s">
+      <c r="K230" s="35"/>
+      <c r="L230" s="35"/>
+      <c r="M230" s="35"/>
+      <c r="N230" s="35"/>
+      <c r="O230" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="P230" s="48" t="s">
+      <c r="P230" s="35" t="s">
         <v>849</v>
       </c>
-      <c r="Q230" s="48" t="s">
+      <c r="Q230" s="35" t="s">
         <v>827</v>
       </c>
-      <c r="R230" s="49"/>
-      <c r="S230" s="50"/>
+      <c r="R230" s="36"/>
+      <c r="S230" s="37"/>
       <c r="T230" s="28" t="s">
         <v>51</v>
       </c>
@@ -16314,24 +16317,24 @@
       <c r="E258" s="22" t="s">
         <v>544</v>
       </c>
-      <c r="F258" s="46"/>
-      <c r="G258" s="47"/>
-      <c r="H258" s="47"/>
-      <c r="I258" s="47"/>
-      <c r="J258" s="48" t="s">
+      <c r="F258" s="33"/>
+      <c r="G258" s="34"/>
+      <c r="H258" s="34"/>
+      <c r="I258" s="34"/>
+      <c r="J258" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K258" s="48" t="s">
+      <c r="K258" s="35" t="s">
         <v>850</v>
       </c>
-      <c r="L258" s="48"/>
-      <c r="M258" s="48"/>
-      <c r="N258" s="48"/>
-      <c r="O258" s="48"/>
-      <c r="P258" s="48"/>
-      <c r="Q258" s="48"/>
-      <c r="R258" s="49"/>
-      <c r="S258" s="50"/>
+      <c r="L258" s="35"/>
+      <c r="M258" s="35"/>
+      <c r="N258" s="35"/>
+      <c r="O258" s="35"/>
+      <c r="P258" s="35"/>
+      <c r="Q258" s="35"/>
+      <c r="R258" s="36"/>
+      <c r="S258" s="37"/>
       <c r="T258" s="28" t="s">
         <v>51</v>
       </c>
@@ -16352,42 +16355,42 @@
       <c r="E259" s="22" t="s">
         <v>546</v>
       </c>
-      <c r="F259" s="46">
+      <c r="F259" s="33">
         <v>45063</v>
       </c>
-      <c r="G259" s="47" t="s">
+      <c r="G259" s="34" t="s">
         <v>851</v>
       </c>
-      <c r="H259" s="47" t="s">
+      <c r="H259" s="34" t="s">
         <v>852</v>
       </c>
-      <c r="I259" s="47" t="s">
+      <c r="I259" s="34" t="s">
         <v>853</v>
       </c>
-      <c r="J259" s="48" t="s">
+      <c r="J259" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="K259" s="48"/>
-      <c r="L259" s="48" t="s">
+      <c r="K259" s="35"/>
+      <c r="L259" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="M259" s="48" t="s">
+      <c r="M259" s="35" t="s">
         <v>843</v>
       </c>
-      <c r="N259" s="48" t="s">
+      <c r="N259" s="35" t="s">
         <v>854</v>
       </c>
-      <c r="O259" s="48" t="s">
+      <c r="O259" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="P259" s="48" t="s">
+      <c r="P259" s="35" t="s">
         <v>845</v>
       </c>
-      <c r="Q259" s="48" t="s">
+      <c r="Q259" s="35" t="s">
         <v>827</v>
       </c>
-      <c r="R259" s="49"/>
-      <c r="S259" s="50" t="s">
+      <c r="R259" s="36"/>
+      <c r="S259" s="37" t="s">
         <v>855</v>
       </c>
       <c r="T259" s="28" t="s">
@@ -16410,24 +16413,24 @@
       <c r="E260" s="22" t="s">
         <v>548</v>
       </c>
-      <c r="F260" s="46"/>
-      <c r="G260" s="47"/>
-      <c r="H260" s="47"/>
-      <c r="I260" s="47"/>
-      <c r="J260" s="48" t="s">
+      <c r="F260" s="33"/>
+      <c r="G260" s="34"/>
+      <c r="H260" s="34"/>
+      <c r="I260" s="34"/>
+      <c r="J260" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K260" s="48" t="s">
+      <c r="K260" s="35" t="s">
         <v>856</v>
       </c>
-      <c r="L260" s="48"/>
-      <c r="M260" s="48"/>
-      <c r="N260" s="48"/>
-      <c r="O260" s="48"/>
-      <c r="P260" s="48"/>
-      <c r="Q260" s="48"/>
-      <c r="R260" s="49"/>
-      <c r="S260" s="50"/>
+      <c r="L260" s="35"/>
+      <c r="M260" s="35"/>
+      <c r="N260" s="35"/>
+      <c r="O260" s="35"/>
+      <c r="P260" s="35"/>
+      <c r="Q260" s="35"/>
+      <c r="R260" s="36"/>
+      <c r="S260" s="37"/>
       <c r="T260" s="28" t="s">
         <v>51</v>
       </c>
@@ -16448,24 +16451,24 @@
       <c r="E261" s="22" t="s">
         <v>550</v>
       </c>
-      <c r="F261" s="46"/>
-      <c r="G261" s="47"/>
-      <c r="H261" s="47"/>
-      <c r="I261" s="47"/>
-      <c r="J261" s="48" t="s">
+      <c r="F261" s="33"/>
+      <c r="G261" s="34"/>
+      <c r="H261" s="34"/>
+      <c r="I261" s="34"/>
+      <c r="J261" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K261" s="48" t="s">
+      <c r="K261" s="35" t="s">
         <v>857</v>
       </c>
-      <c r="L261" s="48"/>
-      <c r="M261" s="48"/>
-      <c r="N261" s="48"/>
-      <c r="O261" s="48"/>
-      <c r="P261" s="48"/>
-      <c r="Q261" s="48"/>
-      <c r="R261" s="49"/>
-      <c r="S261" s="50"/>
+      <c r="L261" s="35"/>
+      <c r="M261" s="35"/>
+      <c r="N261" s="35"/>
+      <c r="O261" s="35"/>
+      <c r="P261" s="35"/>
+      <c r="Q261" s="35"/>
+      <c r="R261" s="36"/>
+      <c r="S261" s="37"/>
       <c r="T261" s="28" t="s">
         <v>51</v>
       </c>
@@ -16486,40 +16489,40 @@
       <c r="E262" s="22" t="s">
         <v>552</v>
       </c>
-      <c r="F262" s="46">
+      <c r="F262" s="33">
         <v>45063</v>
       </c>
-      <c r="G262" s="47" t="s">
+      <c r="G262" s="34" t="s">
         <v>858</v>
       </c>
-      <c r="H262" s="47" t="s">
+      <c r="H262" s="34" t="s">
         <v>859</v>
       </c>
-      <c r="I262" s="47" t="s">
+      <c r="I262" s="34" t="s">
         <v>860</v>
       </c>
-      <c r="J262" s="48" t="s">
+      <c r="J262" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="K262" s="48"/>
-      <c r="L262" s="48" t="s">
+      <c r="K262" s="35"/>
+      <c r="L262" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="M262" s="48" t="s">
+      <c r="M262" s="35" t="s">
         <v>843</v>
       </c>
-      <c r="N262" s="48"/>
-      <c r="O262" s="48" t="s">
+      <c r="N262" s="35"/>
+      <c r="O262" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="P262" s="48" t="s">
+      <c r="P262" s="35" t="s">
         <v>845</v>
       </c>
-      <c r="Q262" s="48" t="s">
+      <c r="Q262" s="35" t="s">
         <v>827</v>
       </c>
-      <c r="R262" s="49"/>
-      <c r="S262" s="50"/>
+      <c r="R262" s="36"/>
+      <c r="S262" s="37"/>
       <c r="T262" s="28" t="s">
         <v>51</v>
       </c>
@@ -16540,42 +16543,42 @@
       <c r="E263" s="22" t="s">
         <v>554</v>
       </c>
-      <c r="F263" s="46">
+      <c r="F263" s="33">
         <v>45063</v>
       </c>
-      <c r="G263" s="47" t="s">
+      <c r="G263" s="34" t="s">
         <v>861</v>
       </c>
-      <c r="H263" s="47" t="s">
+      <c r="H263" s="34" t="s">
         <v>862</v>
       </c>
-      <c r="I263" s="47" t="s">
+      <c r="I263" s="34" t="s">
         <v>863</v>
       </c>
-      <c r="J263" s="48" t="s">
+      <c r="J263" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="K263" s="48"/>
-      <c r="L263" s="48" t="s">
+      <c r="K263" s="35"/>
+      <c r="L263" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="M263" s="48" t="s">
+      <c r="M263" s="35" t="s">
         <v>843</v>
       </c>
-      <c r="N263" s="48" t="s">
+      <c r="N263" s="35" t="s">
         <v>864</v>
       </c>
-      <c r="O263" s="48" t="s">
+      <c r="O263" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="P263" s="48" t="s">
+      <c r="P263" s="35" t="s">
         <v>845</v>
       </c>
-      <c r="Q263" s="48" t="s">
+      <c r="Q263" s="35" t="s">
         <v>827</v>
       </c>
-      <c r="R263" s="49"/>
-      <c r="S263" s="50" t="s">
+      <c r="R263" s="36"/>
+      <c r="S263" s="37" t="s">
         <v>865</v>
       </c>
       <c r="T263" s="28" t="s">
@@ -16598,24 +16601,24 @@
       <c r="E264" s="22" t="s">
         <v>556</v>
       </c>
-      <c r="F264" s="46"/>
-      <c r="G264" s="47"/>
-      <c r="H264" s="47"/>
-      <c r="I264" s="47"/>
-      <c r="J264" s="48" t="s">
+      <c r="F264" s="33"/>
+      <c r="G264" s="34"/>
+      <c r="H264" s="34"/>
+      <c r="I264" s="34"/>
+      <c r="J264" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K264" s="48" t="s">
+      <c r="K264" s="35" t="s">
         <v>866</v>
       </c>
-      <c r="L264" s="48"/>
-      <c r="M264" s="48"/>
-      <c r="N264" s="48"/>
-      <c r="O264" s="48"/>
-      <c r="P264" s="48"/>
-      <c r="Q264" s="48"/>
-      <c r="R264" s="49"/>
-      <c r="S264" s="50"/>
+      <c r="L264" s="35"/>
+      <c r="M264" s="35"/>
+      <c r="N264" s="35"/>
+      <c r="O264" s="35"/>
+      <c r="P264" s="35"/>
+      <c r="Q264" s="35"/>
+      <c r="R264" s="36"/>
+      <c r="S264" s="37"/>
       <c r="T264" s="28" t="s">
         <v>51</v>
       </c>
@@ -16636,42 +16639,42 @@
       <c r="E265" s="22" t="s">
         <v>558</v>
       </c>
-      <c r="F265" s="46">
+      <c r="F265" s="33">
         <v>45064</v>
       </c>
-      <c r="G265" s="47" t="s">
+      <c r="G265" s="34" t="s">
         <v>867</v>
       </c>
-      <c r="H265" s="51" t="s">
+      <c r="H265" s="38" t="s">
         <v>868</v>
       </c>
-      <c r="I265" s="47" t="s">
+      <c r="I265" s="34" t="s">
         <v>869</v>
       </c>
-      <c r="J265" s="48" t="s">
+      <c r="J265" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="K265" s="48"/>
-      <c r="L265" s="48" t="s">
+      <c r="K265" s="35"/>
+      <c r="L265" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="M265" s="48" t="s">
+      <c r="M265" s="35" t="s">
         <v>843</v>
       </c>
-      <c r="N265" s="48" t="s">
+      <c r="N265" s="35" t="s">
         <v>870</v>
       </c>
-      <c r="O265" s="48" t="s">
+      <c r="O265" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="P265" s="48" t="s">
+      <c r="P265" s="35" t="s">
         <v>845</v>
       </c>
-      <c r="Q265" s="48" t="s">
+      <c r="Q265" s="35" t="s">
         <v>827</v>
       </c>
-      <c r="R265" s="49"/>
-      <c r="S265" s="50" t="s">
+      <c r="R265" s="36"/>
+      <c r="S265" s="37" t="s">
         <v>855</v>
       </c>
       <c r="T265" s="28" t="s">
@@ -16694,32 +16697,42 @@
       <c r="E266" s="22" t="s">
         <v>560</v>
       </c>
-      <c r="F266" s="46">
+      <c r="F266" s="33">
         <v>45064</v>
       </c>
-      <c r="G266" s="47" t="s">
+      <c r="G266" s="34" t="s">
         <v>871</v>
       </c>
-      <c r="H266" s="47" t="s">
+      <c r="H266" s="34" t="s">
         <v>872</v>
       </c>
-      <c r="I266" s="47" t="s">
+      <c r="I266" s="34" t="s">
         <v>873</v>
       </c>
-      <c r="J266" s="48" t="s">
+      <c r="J266" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="K266" s="48"/>
-      <c r="L266" s="48"/>
-      <c r="M266" s="48"/>
-      <c r="N266" s="48"/>
-      <c r="O266" s="48"/>
-      <c r="P266" s="48"/>
-      <c r="Q266" s="48" t="s">
+      <c r="K266" s="35"/>
+      <c r="L266" s="35" t="s">
+        <v>829</v>
+      </c>
+      <c r="M266" s="35" t="s">
+        <v>829</v>
+      </c>
+      <c r="N266" s="35" t="s">
+        <v>884</v>
+      </c>
+      <c r="O266" s="35" t="s">
+        <v>489</v>
+      </c>
+      <c r="P266" s="35" t="s">
+        <v>845</v>
+      </c>
+      <c r="Q266" s="35" t="s">
         <v>827</v>
       </c>
-      <c r="R266" s="49"/>
-      <c r="S266" s="50"/>
+      <c r="R266" s="36"/>
+      <c r="S266" s="37"/>
       <c r="T266" s="28" t="s">
         <v>51</v>
       </c>
@@ -16740,42 +16753,42 @@
       <c r="E267" s="22" t="s">
         <v>562</v>
       </c>
-      <c r="F267" s="46">
+      <c r="F267" s="33">
         <v>45064</v>
       </c>
-      <c r="G267" s="47" t="s">
+      <c r="G267" s="34" t="s">
         <v>874</v>
       </c>
-      <c r="H267" s="47" t="s">
+      <c r="H267" s="34" t="s">
         <v>875</v>
       </c>
-      <c r="I267" s="47" t="s">
+      <c r="I267" s="34" t="s">
         <v>876</v>
       </c>
-      <c r="J267" s="48" t="s">
+      <c r="J267" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="K267" s="48"/>
-      <c r="L267" s="48" t="s">
+      <c r="K267" s="35"/>
+      <c r="L267" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="M267" s="48" t="s">
+      <c r="M267" s="35" t="s">
         <v>843</v>
       </c>
-      <c r="N267" s="48" t="s">
+      <c r="N267" s="35" t="s">
         <v>877</v>
       </c>
-      <c r="O267" s="48" t="s">
+      <c r="O267" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="P267" s="48" t="s">
+      <c r="P267" s="35" t="s">
         <v>845</v>
       </c>
-      <c r="Q267" s="48" t="s">
+      <c r="Q267" s="35" t="s">
         <v>827</v>
       </c>
-      <c r="R267" s="49"/>
-      <c r="S267" s="50"/>
+      <c r="R267" s="36"/>
+      <c r="S267" s="37"/>
       <c r="T267" s="28" t="s">
         <v>51</v>
       </c>
@@ -16796,24 +16809,24 @@
       <c r="E268" s="22" t="s">
         <v>564</v>
       </c>
-      <c r="F268" s="46"/>
-      <c r="G268" s="47"/>
-      <c r="H268" s="47"/>
-      <c r="I268" s="47"/>
-      <c r="J268" s="48" t="s">
+      <c r="F268" s="33"/>
+      <c r="G268" s="34"/>
+      <c r="H268" s="34"/>
+      <c r="I268" s="34"/>
+      <c r="J268" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K268" s="48" t="s">
+      <c r="K268" s="35" t="s">
         <v>878</v>
       </c>
-      <c r="L268" s="48"/>
-      <c r="M268" s="48"/>
-      <c r="N268" s="48"/>
-      <c r="O268" s="48"/>
-      <c r="P268" s="48"/>
-      <c r="Q268" s="48"/>
-      <c r="R268" s="49"/>
-      <c r="S268" s="50"/>
+      <c r="L268" s="35"/>
+      <c r="M268" s="35"/>
+      <c r="N268" s="35"/>
+      <c r="O268" s="35"/>
+      <c r="P268" s="35"/>
+      <c r="Q268" s="35"/>
+      <c r="R268" s="36"/>
+      <c r="S268" s="37"/>
       <c r="T268" s="28" t="s">
         <v>51</v>
       </c>
@@ -16834,24 +16847,24 @@
       <c r="E269" s="22" t="s">
         <v>566</v>
       </c>
-      <c r="F269" s="46"/>
-      <c r="G269" s="47"/>
-      <c r="H269" s="47"/>
-      <c r="I269" s="47"/>
-      <c r="J269" s="48" t="s">
+      <c r="F269" s="33"/>
+      <c r="G269" s="34"/>
+      <c r="H269" s="34"/>
+      <c r="I269" s="34"/>
+      <c r="J269" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K269" s="48" t="s">
+      <c r="K269" s="35" t="s">
         <v>879</v>
       </c>
-      <c r="L269" s="48"/>
-      <c r="M269" s="48"/>
-      <c r="N269" s="48"/>
-      <c r="O269" s="48"/>
-      <c r="P269" s="48"/>
-      <c r="Q269" s="48"/>
-      <c r="R269" s="49"/>
-      <c r="S269" s="50"/>
+      <c r="L269" s="35"/>
+      <c r="M269" s="35"/>
+      <c r="N269" s="35"/>
+      <c r="O269" s="35"/>
+      <c r="P269" s="35"/>
+      <c r="Q269" s="35"/>
+      <c r="R269" s="36"/>
+      <c r="S269" s="37"/>
       <c r="T269" s="28" t="s">
         <v>51</v>
       </c>
@@ -16872,24 +16885,24 @@
       <c r="E270" s="22" t="s">
         <v>568</v>
       </c>
-      <c r="F270" s="46"/>
-      <c r="G270" s="47"/>
-      <c r="H270" s="47"/>
-      <c r="I270" s="47"/>
-      <c r="J270" s="48" t="s">
+      <c r="F270" s="33"/>
+      <c r="G270" s="34"/>
+      <c r="H270" s="34"/>
+      <c r="I270" s="34"/>
+      <c r="J270" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K270" s="48" t="s">
+      <c r="K270" s="35" t="s">
         <v>880</v>
       </c>
-      <c r="L270" s="48"/>
-      <c r="M270" s="48"/>
-      <c r="N270" s="48"/>
-      <c r="O270" s="48"/>
-      <c r="P270" s="48"/>
-      <c r="Q270" s="48"/>
-      <c r="R270" s="49"/>
-      <c r="S270" s="50"/>
+      <c r="L270" s="35"/>
+      <c r="M270" s="35"/>
+      <c r="N270" s="35"/>
+      <c r="O270" s="35"/>
+      <c r="P270" s="35"/>
+      <c r="Q270" s="35"/>
+      <c r="R270" s="36"/>
+      <c r="S270" s="37"/>
       <c r="T270" s="28" t="s">
         <v>51</v>
       </c>
@@ -16910,24 +16923,24 @@
       <c r="E271" s="22" t="s">
         <v>570</v>
       </c>
-      <c r="F271" s="46"/>
-      <c r="G271" s="47"/>
-      <c r="H271" s="47"/>
-      <c r="I271" s="47"/>
-      <c r="J271" s="48" t="s">
+      <c r="F271" s="33"/>
+      <c r="G271" s="34"/>
+      <c r="H271" s="34"/>
+      <c r="I271" s="34"/>
+      <c r="J271" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K271" s="48" t="s">
+      <c r="K271" s="35" t="s">
         <v>881</v>
       </c>
-      <c r="L271" s="48"/>
-      <c r="M271" s="48"/>
-      <c r="N271" s="48"/>
-      <c r="O271" s="48"/>
-      <c r="P271" s="48"/>
-      <c r="Q271" s="48"/>
-      <c r="R271" s="49"/>
-      <c r="S271" s="50"/>
+      <c r="L271" s="35"/>
+      <c r="M271" s="35"/>
+      <c r="N271" s="35"/>
+      <c r="O271" s="35"/>
+      <c r="P271" s="35"/>
+      <c r="Q271" s="35"/>
+      <c r="R271" s="36"/>
+      <c r="S271" s="37"/>
       <c r="T271" s="28" t="s">
         <v>51</v>
       </c>
@@ -16948,24 +16961,24 @@
       <c r="E272" s="22" t="s">
         <v>572</v>
       </c>
-      <c r="F272" s="46"/>
-      <c r="G272" s="47"/>
-      <c r="H272" s="47"/>
-      <c r="I272" s="47"/>
-      <c r="J272" s="48" t="s">
+      <c r="F272" s="33"/>
+      <c r="G272" s="34"/>
+      <c r="H272" s="34"/>
+      <c r="I272" s="34"/>
+      <c r="J272" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K272" s="48" t="s">
+      <c r="K272" s="35" t="s">
         <v>881</v>
       </c>
-      <c r="L272" s="48"/>
-      <c r="M272" s="48"/>
-      <c r="N272" s="48"/>
-      <c r="O272" s="48"/>
-      <c r="P272" s="48"/>
-      <c r="Q272" s="48"/>
-      <c r="R272" s="49"/>
-      <c r="S272" s="50"/>
+      <c r="L272" s="35"/>
+      <c r="M272" s="35"/>
+      <c r="N272" s="35"/>
+      <c r="O272" s="35"/>
+      <c r="P272" s="35"/>
+      <c r="Q272" s="35"/>
+      <c r="R272" s="36"/>
+      <c r="S272" s="37"/>
       <c r="T272" s="28" t="s">
         <v>51</v>
       </c>
@@ -16986,24 +16999,24 @@
       <c r="E273" s="22" t="s">
         <v>574</v>
       </c>
-      <c r="F273" s="46"/>
-      <c r="G273" s="47"/>
-      <c r="H273" s="47"/>
-      <c r="I273" s="47"/>
-      <c r="J273" s="48" t="s">
+      <c r="F273" s="33"/>
+      <c r="G273" s="34"/>
+      <c r="H273" s="34"/>
+      <c r="I273" s="34"/>
+      <c r="J273" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K273" s="48" t="s">
+      <c r="K273" s="35" t="s">
         <v>881</v>
       </c>
-      <c r="L273" s="48"/>
-      <c r="M273" s="48"/>
-      <c r="N273" s="48"/>
-      <c r="O273" s="48"/>
-      <c r="P273" s="48"/>
-      <c r="Q273" s="48"/>
-      <c r="R273" s="49"/>
-      <c r="S273" s="50"/>
+      <c r="L273" s="35"/>
+      <c r="M273" s="35"/>
+      <c r="N273" s="35"/>
+      <c r="O273" s="35"/>
+      <c r="P273" s="35"/>
+      <c r="Q273" s="35"/>
+      <c r="R273" s="36"/>
+      <c r="S273" s="37"/>
       <c r="T273" s="28" t="s">
         <v>51</v>
       </c>
@@ -17024,24 +17037,24 @@
       <c r="E274" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="F274" s="46"/>
-      <c r="G274" s="47"/>
-      <c r="H274" s="47"/>
-      <c r="I274" s="47"/>
-      <c r="J274" s="48" t="s">
+      <c r="F274" s="33"/>
+      <c r="G274" s="34"/>
+      <c r="H274" s="34"/>
+      <c r="I274" s="34"/>
+      <c r="J274" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K274" s="48" t="s">
+      <c r="K274" s="35" t="s">
         <v>881</v>
       </c>
-      <c r="L274" s="48"/>
-      <c r="M274" s="48"/>
-      <c r="N274" s="48"/>
-      <c r="O274" s="48"/>
-      <c r="P274" s="48"/>
-      <c r="Q274" s="48"/>
-      <c r="R274" s="49"/>
-      <c r="S274" s="50"/>
+      <c r="L274" s="35"/>
+      <c r="M274" s="35"/>
+      <c r="N274" s="35"/>
+      <c r="O274" s="35"/>
+      <c r="P274" s="35"/>
+      <c r="Q274" s="35"/>
+      <c r="R274" s="36"/>
+      <c r="S274" s="37"/>
       <c r="T274" s="28" t="s">
         <v>51</v>
       </c>
@@ -17062,24 +17075,24 @@
       <c r="E275" s="22" t="s">
         <v>578</v>
       </c>
-      <c r="F275" s="46"/>
-      <c r="G275" s="47"/>
-      <c r="H275" s="47"/>
-      <c r="I275" s="47"/>
-      <c r="J275" s="48" t="s">
+      <c r="F275" s="33"/>
+      <c r="G275" s="34"/>
+      <c r="H275" s="34"/>
+      <c r="I275" s="34"/>
+      <c r="J275" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K275" s="48" t="s">
+      <c r="K275" s="35" t="s">
         <v>882</v>
       </c>
-      <c r="L275" s="48"/>
-      <c r="M275" s="48"/>
-      <c r="N275" s="48"/>
-      <c r="O275" s="48"/>
-      <c r="P275" s="48"/>
-      <c r="Q275" s="48"/>
-      <c r="R275" s="49"/>
-      <c r="S275" s="50"/>
+      <c r="L275" s="35"/>
+      <c r="M275" s="35"/>
+      <c r="N275" s="35"/>
+      <c r="O275" s="35"/>
+      <c r="P275" s="35"/>
+      <c r="Q275" s="35"/>
+      <c r="R275" s="36"/>
+      <c r="S275" s="37"/>
       <c r="T275" s="28" t="s">
         <v>51</v>
       </c>
@@ -17100,24 +17113,24 @@
       <c r="E276" s="22" t="s">
         <v>580</v>
       </c>
-      <c r="F276" s="46"/>
-      <c r="G276" s="47"/>
-      <c r="H276" s="47"/>
-      <c r="I276" s="47"/>
-      <c r="J276" s="48" t="s">
+      <c r="F276" s="33"/>
+      <c r="G276" s="34"/>
+      <c r="H276" s="34"/>
+      <c r="I276" s="34"/>
+      <c r="J276" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="K276" s="48" t="s">
+      <c r="K276" s="35" t="s">
         <v>883</v>
       </c>
-      <c r="L276" s="48"/>
-      <c r="M276" s="48"/>
-      <c r="N276" s="48"/>
-      <c r="O276" s="48"/>
-      <c r="P276" s="48"/>
-      <c r="Q276" s="48"/>
-      <c r="R276" s="49"/>
-      <c r="S276" s="50"/>
+      <c r="L276" s="35"/>
+      <c r="M276" s="35"/>
+      <c r="N276" s="35"/>
+      <c r="O276" s="35"/>
+      <c r="P276" s="35"/>
+      <c r="Q276" s="35"/>
+      <c r="R276" s="36"/>
+      <c r="S276" s="37"/>
       <c r="T276" s="28" t="s">
         <v>51</v>
       </c>
@@ -33054,20 +33067,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ContentTypeId="0x01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d">
@@ -33079,14 +33078,47 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{330C73C0-97BE-4E44-9B85-0CBBC432A409}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{330C73C0-97BE-4E44-9B85-0CBBC432A409}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
+    <ds:schemaRef ds:uri="bb0bfb2d-9415-422c-9311-cf5d9d9d5142"/>
+    <ds:schemaRef ds:uri="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12D86236-EAFC-48DB-B351-E7598A8B8AB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2850EEF4-EC69-4F2E-B0CE-8034B61489F3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
+    <ds:schemaRef ds:uri="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -33100,5 +33132,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2850EEF4-EC69-4F2E-B0CE-8034B61489F3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12D86236-EAFC-48DB-B351-E7598A8B8AB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test ID 79 and 83 updated as requested
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111PHILIPSXXXX/Philips/VuePACS-SignPlugin/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111PHILIPSXXXX/Philips/VuePACS-SignPlugin/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.philips.com/sites/HCISIntegration260/Integration Project Docs/EAMER/Italy/FSE 2.0/Accreditamento/file da sottomettere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CB7C22D-675F-40F0-B654-C37BF000EE54}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9530529-A5B9-422E-8FC5-8A415B4E4272}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="880">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4536,15 +4536,6 @@
     <t>Il sistema non prevede il campo opzionale indirizzo del paziente</t>
   </si>
   <si>
-    <t>2023-05-17T17:37:51.713Z</t>
-  </si>
-  <si>
-    <t>4fcd5cc82e88646f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.f46690ec53^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-05-17T16:21:54.999Z</t>
   </si>
   <si>
@@ -4575,15 +4566,6 @@
     <t>title:"Errore semantico.","detail":"[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ]","status":422,"instance":"/validation/error"</t>
   </si>
   <si>
-    <t>2023-05-18T11:04:38.650Z</t>
-  </si>
-  <si>
-    <t>c5d0254874f4a666</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.4d8f935f45^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-05-18T09:40:43.581Z</t>
   </si>
   <si>
@@ -4614,7 +4596,10 @@
     <t>Il Sistema non prevede il campo opzionale "documentationOf"</t>
   </si>
   <si>
-    <t>Non riceviamo alcun errore dal servizio</t>
+    <t>Il sistema non prevede l'assenza del tag  patient\name\given nel CDA2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il sistema genera sempre almeno un tag inFulfillmentOf/order/id, in quanto l'accession number è un prerequisito necessario e obbligatorio per la firma digitale. </t>
   </si>
 </sst>
 </file>
@@ -5372,11 +5357,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="130.08984375" customWidth="1"/>
+    <col min="1" max="1" width="149.1796875" customWidth="1"/>
     <col min="2" max="26" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5385,32 +5372,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.25" customHeight="1">
+    <row r="2" spans="1:1" ht="87">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.25" customHeight="1">
+    <row r="3" spans="1:1" ht="14.5">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="14.25" customHeight="1">
+    <row r="4" spans="1:1" ht="174">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.25" customHeight="1">
+    <row r="5" spans="1:1" ht="29">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.25" customHeight="1">
+    <row r="6" spans="1:1" ht="29">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.25" customHeight="1">
+    <row r="7" spans="1:1" ht="14.5">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -7531,13 +7518,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B265" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B264" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B266" sqref="B266"/>
+      <selection pane="bottomRight" activeCell="A266" sqref="A266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -7791,7 +7779,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="232">
+    <row r="10" spans="1:20" ht="232" hidden="1">
       <c r="A10" s="20">
         <v>194</v>
       </c>
@@ -7825,7 +7813,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="217.5">
+    <row r="11" spans="1:20" ht="217.5" hidden="1">
       <c r="A11" s="20">
         <v>205</v>
       </c>
@@ -7859,7 +7847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="232">
+    <row r="12" spans="1:20" ht="232" hidden="1">
       <c r="A12" s="20">
         <v>210</v>
       </c>
@@ -7893,7 +7881,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="217.5">
+    <row r="13" spans="1:20" ht="217.5" hidden="1">
       <c r="A13" s="20">
         <v>221</v>
       </c>
@@ -7995,7 +7983,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="232">
+    <row r="16" spans="1:20" ht="232" hidden="1">
       <c r="A16" s="20">
         <v>242</v>
       </c>
@@ -8029,7 +8017,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="217.5">
+    <row r="17" spans="1:20" ht="217.5" hidden="1">
       <c r="A17" s="20">
         <v>253</v>
       </c>
@@ -8063,7 +8051,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="232">
+    <row r="18" spans="1:20" ht="232" hidden="1">
       <c r="A18" s="20">
         <v>258</v>
       </c>
@@ -8097,7 +8085,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="217.5">
+    <row r="19" spans="1:20" ht="217.5" hidden="1">
       <c r="A19" s="20">
         <v>269</v>
       </c>
@@ -8131,7 +8119,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="232">
+    <row r="20" spans="1:20" ht="232" hidden="1">
       <c r="A20" s="20">
         <v>274</v>
       </c>
@@ -8165,7 +8153,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="217.5">
+    <row r="21" spans="1:20" ht="217.5" hidden="1">
       <c r="A21" s="20">
         <v>285</v>
       </c>
@@ -8199,7 +8187,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="232">
+    <row r="22" spans="1:20" ht="232" hidden="1">
       <c r="A22" s="20">
         <v>290</v>
       </c>
@@ -8233,7 +8221,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="217.5">
+    <row r="23" spans="1:20" ht="217.5" hidden="1">
       <c r="A23" s="20">
         <v>301</v>
       </c>
@@ -8267,7 +8255,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="232">
+    <row r="24" spans="1:20" ht="232" hidden="1">
       <c r="A24" s="20">
         <v>306</v>
       </c>
@@ -8301,7 +8289,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="217.5">
+    <row r="25" spans="1:20" ht="217.5" hidden="1">
       <c r="A25" s="20">
         <v>317</v>
       </c>
@@ -8335,7 +8323,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="174">
+    <row r="26" spans="1:20" ht="174" hidden="1">
       <c r="A26" s="20">
         <v>352</v>
       </c>
@@ -8369,7 +8357,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="203">
+    <row r="27" spans="1:20" ht="203" hidden="1">
       <c r="A27" s="20">
         <v>353</v>
       </c>
@@ -8403,7 +8391,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="174">
+    <row r="28" spans="1:20" ht="174" hidden="1">
       <c r="A28" s="20">
         <v>354</v>
       </c>
@@ -8437,7 +8425,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="203">
+    <row r="29" spans="1:20" ht="203" hidden="1">
       <c r="A29" s="20">
         <v>355</v>
       </c>
@@ -8539,7 +8527,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="174">
+    <row r="32" spans="1:20" ht="174" hidden="1">
       <c r="A32" s="20">
         <v>358</v>
       </c>
@@ -8573,7 +8561,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="203">
+    <row r="33" spans="1:20" ht="203" hidden="1">
       <c r="A33" s="20">
         <v>359</v>
       </c>
@@ -8607,7 +8595,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="174">
+    <row r="34" spans="1:20" ht="174" hidden="1">
       <c r="A34" s="20">
         <v>360</v>
       </c>
@@ -8641,7 +8629,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="203">
+    <row r="35" spans="1:20" ht="203" hidden="1">
       <c r="A35" s="20">
         <v>361</v>
       </c>
@@ -8675,7 +8663,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="174">
+    <row r="36" spans="1:20" ht="174" hidden="1">
       <c r="A36" s="20">
         <v>362</v>
       </c>
@@ -8709,7 +8697,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="203">
+    <row r="37" spans="1:20" ht="203" hidden="1">
       <c r="A37" s="20">
         <v>363</v>
       </c>
@@ -8743,7 +8731,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="174">
+    <row r="38" spans="1:20" ht="174" hidden="1">
       <c r="A38" s="20">
         <v>364</v>
       </c>
@@ -8777,7 +8765,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="203">
+    <row r="39" spans="1:20" ht="203" hidden="1">
       <c r="A39" s="20">
         <v>365</v>
       </c>
@@ -8811,7 +8799,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="174">
+    <row r="40" spans="1:20" ht="174" hidden="1">
       <c r="A40" s="20">
         <v>366</v>
       </c>
@@ -8845,7 +8833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="203">
+    <row r="41" spans="1:20" ht="203" hidden="1">
       <c r="A41" s="20">
         <v>367</v>
       </c>
@@ -8879,7 +8867,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="145">
+    <row r="42" spans="1:20" ht="145" hidden="1">
       <c r="A42" s="20">
         <v>195</v>
       </c>
@@ -8913,7 +8901,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="116">
+    <row r="43" spans="1:20" ht="116" hidden="1">
       <c r="A43" s="20">
         <v>204</v>
       </c>
@@ -8947,7 +8935,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="145">
+    <row r="44" spans="1:20" ht="145" hidden="1">
       <c r="A44" s="20">
         <v>211</v>
       </c>
@@ -8981,7 +8969,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="116">
+    <row r="45" spans="1:20" ht="116" hidden="1">
       <c r="A45" s="20">
         <v>220</v>
       </c>
@@ -9083,7 +9071,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="145">
+    <row r="48" spans="1:20" ht="145" hidden="1">
       <c r="A48" s="20">
         <v>243</v>
       </c>
@@ -9117,7 +9105,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="116">
+    <row r="49" spans="1:20" ht="116" hidden="1">
       <c r="A49" s="20">
         <v>252</v>
       </c>
@@ -9151,7 +9139,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="145">
+    <row r="50" spans="1:20" ht="145" hidden="1">
       <c r="A50" s="20">
         <v>259</v>
       </c>
@@ -9185,7 +9173,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="116">
+    <row r="51" spans="1:20" ht="116" hidden="1">
       <c r="A51" s="20">
         <v>268</v>
       </c>
@@ -9219,7 +9207,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="145">
+    <row r="52" spans="1:20" ht="145" hidden="1">
       <c r="A52" s="20">
         <v>275</v>
       </c>
@@ -9253,7 +9241,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="116">
+    <row r="53" spans="1:20" ht="116" hidden="1">
       <c r="A53" s="20">
         <v>284</v>
       </c>
@@ -9287,7 +9275,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="145">
+    <row r="54" spans="1:20" ht="145" hidden="1">
       <c r="A54" s="20">
         <v>291</v>
       </c>
@@ -9321,7 +9309,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="116">
+    <row r="55" spans="1:20" ht="116" hidden="1">
       <c r="A55" s="20">
         <v>300</v>
       </c>
@@ -9355,7 +9343,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="145">
+    <row r="56" spans="1:20" ht="145" hidden="1">
       <c r="A56" s="20">
         <v>307</v>
       </c>
@@ -9389,7 +9377,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="116">
+    <row r="57" spans="1:20" ht="116" hidden="1">
       <c r="A57" s="20">
         <v>316</v>
       </c>
@@ -9423,7 +9411,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="232">
+    <row r="58" spans="1:20" ht="232" hidden="1">
       <c r="A58" s="20">
         <v>196</v>
       </c>
@@ -9457,7 +9445,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="217.5">
+    <row r="59" spans="1:20" ht="217.5" hidden="1">
       <c r="A59" s="20">
         <v>207</v>
       </c>
@@ -9491,7 +9479,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="232">
+    <row r="60" spans="1:20" ht="232" hidden="1">
       <c r="A60" s="20">
         <v>212</v>
       </c>
@@ -9525,7 +9513,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="217.5">
+    <row r="61" spans="1:20" ht="217.5" hidden="1">
       <c r="A61" s="20">
         <v>223</v>
       </c>
@@ -9627,7 +9615,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="261">
+    <row r="64" spans="1:20" ht="261" hidden="1">
       <c r="A64" s="20">
         <v>244</v>
       </c>
@@ -9661,7 +9649,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="232">
+    <row r="65" spans="1:20" ht="232" hidden="1">
       <c r="A65" s="20">
         <v>255</v>
       </c>
@@ -9695,7 +9683,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="261">
+    <row r="66" spans="1:20" ht="261" hidden="1">
       <c r="A66" s="20">
         <v>260</v>
       </c>
@@ -9729,7 +9717,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="232">
+    <row r="67" spans="1:20" ht="232" hidden="1">
       <c r="A67" s="20">
         <v>271</v>
       </c>
@@ -9763,7 +9751,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="232">
+    <row r="68" spans="1:20" ht="232" hidden="1">
       <c r="A68" s="20">
         <v>276</v>
       </c>
@@ -9797,7 +9785,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="217.5">
+    <row r="69" spans="1:20" ht="217.5" hidden="1">
       <c r="A69" s="20">
         <v>287</v>
       </c>
@@ -9831,7 +9819,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="232">
+    <row r="70" spans="1:20" ht="232" hidden="1">
       <c r="A70" s="20">
         <v>292</v>
       </c>
@@ -9865,7 +9853,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="217.5">
+    <row r="71" spans="1:20" ht="217.5" hidden="1">
       <c r="A71" s="20">
         <v>303</v>
       </c>
@@ -9899,7 +9887,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="232">
+    <row r="72" spans="1:20" ht="232" hidden="1">
       <c r="A72" s="20">
         <v>308</v>
       </c>
@@ -9933,7 +9921,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="217.5">
+    <row r="73" spans="1:20" ht="217.5" hidden="1">
       <c r="A73" s="20">
         <v>319</v>
       </c>
@@ -9967,7 +9955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="159.5">
+    <row r="74" spans="1:20" ht="159.5" hidden="1">
       <c r="A74" s="20">
         <v>192</v>
       </c>
@@ -10001,7 +9989,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="174">
+    <row r="75" spans="1:20" ht="174" hidden="1">
       <c r="A75" s="20">
         <v>197</v>
       </c>
@@ -10035,7 +10023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="188.5">
+    <row r="76" spans="1:20" ht="188.5" hidden="1">
       <c r="A76" s="20">
         <v>198</v>
       </c>
@@ -10069,7 +10057,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="203">
+    <row r="77" spans="1:20" ht="203" hidden="1">
       <c r="A77" s="20">
         <v>199</v>
       </c>
@@ -10103,7 +10091,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="188.5">
+    <row r="78" spans="1:20" ht="188.5" hidden="1">
       <c r="A78" s="20">
         <v>200</v>
       </c>
@@ -10137,7 +10125,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="188.5">
+    <row r="79" spans="1:20" ht="188.5" hidden="1">
       <c r="A79" s="20">
         <v>201</v>
       </c>
@@ -10171,7 +10159,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="188.5">
+    <row r="80" spans="1:20" ht="188.5" hidden="1">
       <c r="A80" s="20">
         <v>202</v>
       </c>
@@ -10205,7 +10193,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="203">
+    <row r="81" spans="1:20" ht="203" hidden="1">
       <c r="A81" s="20">
         <v>203</v>
       </c>
@@ -10239,7 +10227,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="159.5">
+    <row r="82" spans="1:20" ht="159.5" hidden="1">
       <c r="A82" s="20">
         <v>208</v>
       </c>
@@ -10273,7 +10261,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="174">
+    <row r="83" spans="1:20" ht="174" hidden="1">
       <c r="A83" s="20">
         <v>213</v>
       </c>
@@ -10307,7 +10295,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="188.5">
+    <row r="84" spans="1:20" ht="188.5" hidden="1">
       <c r="A84" s="20">
         <v>214</v>
       </c>
@@ -10341,7 +10329,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="203">
+    <row r="85" spans="1:20" ht="203" hidden="1">
       <c r="A85" s="20">
         <v>215</v>
       </c>
@@ -10375,7 +10363,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="188.5">
+    <row r="86" spans="1:20" ht="188.5" hidden="1">
       <c r="A86" s="20">
         <v>216</v>
       </c>
@@ -10409,7 +10397,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="188.5">
+    <row r="87" spans="1:20" ht="188.5" hidden="1">
       <c r="A87" s="20">
         <v>217</v>
       </c>
@@ -10443,7 +10431,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="188.5">
+    <row r="88" spans="1:20" ht="188.5" hidden="1">
       <c r="A88" s="20">
         <v>218</v>
       </c>
@@ -10477,7 +10465,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="203">
+    <row r="89" spans="1:20" ht="203" hidden="1">
       <c r="A89" s="20">
         <v>219</v>
       </c>
@@ -10783,7 +10771,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="174">
+    <row r="98" spans="1:20" ht="174" hidden="1">
       <c r="A98" s="20">
         <v>240</v>
       </c>
@@ -10817,7 +10805,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="188.5">
+    <row r="99" spans="1:20" ht="188.5" hidden="1">
       <c r="A99" s="20">
         <v>245</v>
       </c>
@@ -10851,7 +10839,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="203">
+    <row r="100" spans="1:20" ht="203" hidden="1">
       <c r="A100" s="20">
         <v>246</v>
       </c>
@@ -10885,7 +10873,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="217.5">
+    <row r="101" spans="1:20" ht="217.5" hidden="1">
       <c r="A101" s="20">
         <v>247</v>
       </c>
@@ -10919,7 +10907,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="203">
+    <row r="102" spans="1:20" ht="203" hidden="1">
       <c r="A102" s="20">
         <v>248</v>
       </c>
@@ -10953,7 +10941,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="203">
+    <row r="103" spans="1:20" ht="203" hidden="1">
       <c r="A103" s="20">
         <v>249</v>
       </c>
@@ -10987,7 +10975,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="203">
+    <row r="104" spans="1:20" ht="203" hidden="1">
       <c r="A104" s="20">
         <v>250</v>
       </c>
@@ -11021,7 +11009,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="217.5">
+    <row r="105" spans="1:20" ht="217.5" hidden="1">
       <c r="A105" s="20">
         <v>251</v>
       </c>
@@ -11055,7 +11043,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="174">
+    <row r="106" spans="1:20" ht="174" hidden="1">
       <c r="A106" s="20">
         <v>256</v>
       </c>
@@ -11089,7 +11077,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="188.5">
+    <row r="107" spans="1:20" ht="188.5" hidden="1">
       <c r="A107" s="20">
         <v>261</v>
       </c>
@@ -11123,7 +11111,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="203">
+    <row r="108" spans="1:20" ht="203" hidden="1">
       <c r="A108" s="20">
         <v>262</v>
       </c>
@@ -11157,7 +11145,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="217.5">
+    <row r="109" spans="1:20" ht="217.5" hidden="1">
       <c r="A109" s="20">
         <v>263</v>
       </c>
@@ -11191,7 +11179,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="203">
+    <row r="110" spans="1:20" ht="203" hidden="1">
       <c r="A110" s="20">
         <v>264</v>
       </c>
@@ -11225,7 +11213,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="203">
+    <row r="111" spans="1:20" ht="203" hidden="1">
       <c r="A111" s="20">
         <v>265</v>
       </c>
@@ -11259,7 +11247,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="203">
+    <row r="112" spans="1:20" ht="203" hidden="1">
       <c r="A112" s="20">
         <v>266</v>
       </c>
@@ -11293,7 +11281,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="217.5">
+    <row r="113" spans="1:20" ht="217.5" hidden="1">
       <c r="A113" s="20">
         <v>267</v>
       </c>
@@ -11327,7 +11315,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="159.5">
+    <row r="114" spans="1:20" ht="159.5" hidden="1">
       <c r="A114" s="20">
         <v>272</v>
       </c>
@@ -11361,7 +11349,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="174">
+    <row r="115" spans="1:20" ht="174" hidden="1">
       <c r="A115" s="20">
         <v>277</v>
       </c>
@@ -11395,7 +11383,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="188.5">
+    <row r="116" spans="1:20" ht="188.5" hidden="1">
       <c r="A116" s="20">
         <v>278</v>
       </c>
@@ -11429,7 +11417,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="203">
+    <row r="117" spans="1:20" ht="203" hidden="1">
       <c r="A117" s="20">
         <v>279</v>
       </c>
@@ -11463,7 +11451,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="188.5">
+    <row r="118" spans="1:20" ht="188.5" hidden="1">
       <c r="A118" s="20">
         <v>280</v>
       </c>
@@ -11497,7 +11485,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="188.5">
+    <row r="119" spans="1:20" ht="188.5" hidden="1">
       <c r="A119" s="20">
         <v>281</v>
       </c>
@@ -11531,7 +11519,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="188.5">
+    <row r="120" spans="1:20" ht="188.5" hidden="1">
       <c r="A120" s="20">
         <v>282</v>
       </c>
@@ -11565,7 +11553,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="203">
+    <row r="121" spans="1:20" ht="203" hidden="1">
       <c r="A121" s="20">
         <v>283</v>
       </c>
@@ -11599,7 +11587,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="159.5">
+    <row r="122" spans="1:20" ht="159.5" hidden="1">
       <c r="A122" s="20">
         <v>288</v>
       </c>
@@ -11633,7 +11621,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="174">
+    <row r="123" spans="1:20" ht="174" hidden="1">
       <c r="A123" s="20">
         <v>293</v>
       </c>
@@ -11667,7 +11655,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="188.5">
+    <row r="124" spans="1:20" ht="188.5" hidden="1">
       <c r="A124" s="20">
         <v>294</v>
       </c>
@@ -11701,7 +11689,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="203">
+    <row r="125" spans="1:20" ht="203" hidden="1">
       <c r="A125" s="20">
         <v>295</v>
       </c>
@@ -11735,7 +11723,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="188.5">
+    <row r="126" spans="1:20" ht="188.5" hidden="1">
       <c r="A126" s="20">
         <v>296</v>
       </c>
@@ -11769,7 +11757,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="188.5">
+    <row r="127" spans="1:20" ht="188.5" hidden="1">
       <c r="A127" s="20">
         <v>297</v>
       </c>
@@ -11803,7 +11791,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="188.5">
+    <row r="128" spans="1:20" ht="188.5" hidden="1">
       <c r="A128" s="20">
         <v>298</v>
       </c>
@@ -11837,7 +11825,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="203">
+    <row r="129" spans="1:20" ht="203" hidden="1">
       <c r="A129" s="20">
         <v>299</v>
       </c>
@@ -11871,7 +11859,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="159.5">
+    <row r="130" spans="1:20" ht="159.5" hidden="1">
       <c r="A130" s="20">
         <v>304</v>
       </c>
@@ -11905,7 +11893,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="174">
+    <row r="131" spans="1:20" ht="174" hidden="1">
       <c r="A131" s="20">
         <v>309</v>
       </c>
@@ -11939,7 +11927,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="188.5">
+    <row r="132" spans="1:20" ht="188.5" hidden="1">
       <c r="A132" s="20">
         <v>310</v>
       </c>
@@ -11973,7 +11961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="203">
+    <row r="133" spans="1:20" ht="203" hidden="1">
       <c r="A133" s="20">
         <v>311</v>
       </c>
@@ -12007,7 +11995,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="188.5">
+    <row r="134" spans="1:20" ht="188.5" hidden="1">
       <c r="A134" s="20">
         <v>312</v>
       </c>
@@ -12041,7 +12029,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="188.5">
+    <row r="135" spans="1:20" ht="188.5" hidden="1">
       <c r="A135" s="20">
         <v>313</v>
       </c>
@@ -12075,7 +12063,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="188.5">
+    <row r="136" spans="1:20" ht="188.5" hidden="1">
       <c r="A136" s="20">
         <v>314</v>
       </c>
@@ -12109,7 +12097,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="203">
+    <row r="137" spans="1:20" ht="203" hidden="1">
       <c r="A137" s="20">
         <v>315</v>
       </c>
@@ -12143,7 +12131,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="246.5">
+    <row r="138" spans="1:20" ht="246.5" hidden="1">
       <c r="A138" s="20">
         <v>320</v>
       </c>
@@ -12177,7 +12165,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="217.5">
+    <row r="139" spans="1:20" ht="217.5" hidden="1">
       <c r="A139" s="20">
         <v>321</v>
       </c>
@@ -12211,7 +12199,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="246.5">
+    <row r="140" spans="1:20" ht="246.5" hidden="1">
       <c r="A140" s="20">
         <v>324</v>
       </c>
@@ -12245,7 +12233,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="203">
+    <row r="141" spans="1:20" ht="203" hidden="1">
       <c r="A141" s="20">
         <v>325</v>
       </c>
@@ -12347,7 +12335,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="261">
+    <row r="144" spans="1:20" ht="261" hidden="1">
       <c r="A144" s="20">
         <v>332</v>
       </c>
@@ -12381,7 +12369,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="217.5">
+    <row r="145" spans="1:20" ht="217.5" hidden="1">
       <c r="A145" s="20">
         <v>333</v>
       </c>
@@ -12415,7 +12403,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="261">
+    <row r="146" spans="1:20" ht="261" hidden="1">
       <c r="A146" s="20">
         <v>336</v>
       </c>
@@ -12449,7 +12437,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="232">
+    <row r="147" spans="1:20" ht="232" hidden="1">
       <c r="A147" s="20">
         <v>337</v>
       </c>
@@ -12483,7 +12471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="246.5">
+    <row r="148" spans="1:20" ht="246.5" hidden="1">
       <c r="A148" s="20">
         <v>340</v>
       </c>
@@ -12517,7 +12505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="217.5">
+    <row r="149" spans="1:20" ht="217.5" hidden="1">
       <c r="A149" s="20">
         <v>341</v>
       </c>
@@ -12551,7 +12539,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="246.5">
+    <row r="150" spans="1:20" ht="246.5" hidden="1">
       <c r="A150" s="20">
         <v>344</v>
       </c>
@@ -12585,7 +12573,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="203">
+    <row r="151" spans="1:20" ht="203" hidden="1">
       <c r="A151" s="20">
         <v>345</v>
       </c>
@@ -12619,7 +12607,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="246.5">
+    <row r="152" spans="1:20" ht="246.5" hidden="1">
       <c r="A152" s="20">
         <v>348</v>
       </c>
@@ -12653,7 +12641,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="217.5">
+    <row r="153" spans="1:20" ht="217.5" hidden="1">
       <c r="A153" s="20">
         <v>349</v>
       </c>
@@ -12687,7 +12675,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="246.5">
+    <row r="154" spans="1:20" ht="246.5" hidden="1">
       <c r="A154" s="20">
         <v>193</v>
       </c>
@@ -12721,7 +12709,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="246.5">
+    <row r="155" spans="1:20" ht="246.5" hidden="1">
       <c r="A155" s="20">
         <v>206</v>
       </c>
@@ -12755,7 +12743,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="246.5">
+    <row r="156" spans="1:20" ht="246.5" hidden="1">
       <c r="A156" s="20">
         <v>209</v>
       </c>
@@ -12789,7 +12777,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="232">
+    <row r="157" spans="1:20" ht="232" hidden="1">
       <c r="A157" s="20">
         <v>222</v>
       </c>
@@ -12891,7 +12879,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="261">
+    <row r="160" spans="1:20" ht="261" hidden="1">
       <c r="A160" s="20">
         <v>241</v>
       </c>
@@ -12925,7 +12913,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="246.5">
+    <row r="161" spans="1:20" ht="246.5" hidden="1">
       <c r="A161" s="20">
         <v>254</v>
       </c>
@@ -12959,7 +12947,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="261">
+    <row r="162" spans="1:20" ht="261" hidden="1">
       <c r="A162" s="20">
         <v>257</v>
       </c>
@@ -12993,7 +12981,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="246.5">
+    <row r="163" spans="1:20" ht="246.5" hidden="1">
       <c r="A163" s="20">
         <v>270</v>
       </c>
@@ -13027,7 +13015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="246.5">
+    <row r="164" spans="1:20" ht="246.5" hidden="1">
       <c r="A164" s="20">
         <v>273</v>
       </c>
@@ -13061,7 +13049,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="232">
+    <row r="165" spans="1:20" ht="232" hidden="1">
       <c r="A165" s="20">
         <v>286</v>
       </c>
@@ -13095,7 +13083,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="246.5">
+    <row r="166" spans="1:20" ht="246.5" hidden="1">
       <c r="A166" s="20">
         <v>289</v>
       </c>
@@ -13129,7 +13117,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="232">
+    <row r="167" spans="1:20" ht="232" hidden="1">
       <c r="A167" s="20">
         <v>302</v>
       </c>
@@ -13163,7 +13151,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="246.5">
+    <row r="168" spans="1:20" ht="246.5" hidden="1">
       <c r="A168" s="20">
         <v>305</v>
       </c>
@@ -13197,7 +13185,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="232">
+    <row r="169" spans="1:20" ht="232" hidden="1">
       <c r="A169" s="20">
         <v>318</v>
       </c>
@@ -13231,7 +13219,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="188.5">
+    <row r="170" spans="1:20" ht="188.5" hidden="1">
       <c r="A170" s="20">
         <v>322</v>
       </c>
@@ -13265,7 +13253,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="217.5">
+    <row r="171" spans="1:20" ht="217.5" hidden="1">
       <c r="A171" s="20">
         <v>323</v>
       </c>
@@ -13299,7 +13287,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="188.5">
+    <row r="172" spans="1:20" ht="188.5" hidden="1">
       <c r="A172" s="20">
         <v>326</v>
       </c>
@@ -13333,7 +13321,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="217.5">
+    <row r="173" spans="1:20" ht="217.5" hidden="1">
       <c r="A173" s="20">
         <v>327</v>
       </c>
@@ -13435,7 +13423,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="188.5">
+    <row r="176" spans="1:20" ht="188.5" hidden="1">
       <c r="A176" s="20">
         <v>334</v>
       </c>
@@ -13469,7 +13457,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="232">
+    <row r="177" spans="1:20" ht="232" hidden="1">
       <c r="A177" s="20">
         <v>335</v>
       </c>
@@ -13503,7 +13491,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="203">
+    <row r="178" spans="1:20" ht="203" hidden="1">
       <c r="A178" s="20">
         <v>338</v>
       </c>
@@ -13537,7 +13525,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="232">
+    <row r="179" spans="1:20" ht="232" hidden="1">
       <c r="A179" s="20">
         <v>339</v>
       </c>
@@ -13571,7 +13559,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="188.5">
+    <row r="180" spans="1:20" ht="188.5" hidden="1">
       <c r="A180" s="20">
         <v>342</v>
       </c>
@@ -13605,7 +13593,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="217.5">
+    <row r="181" spans="1:20" ht="217.5" hidden="1">
       <c r="A181" s="20">
         <v>343</v>
       </c>
@@ -13639,7 +13627,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="174">
+    <row r="182" spans="1:20" ht="174" hidden="1">
       <c r="A182" s="20">
         <v>346</v>
       </c>
@@ -13673,7 +13661,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="217.5">
+    <row r="183" spans="1:20" ht="217.5" hidden="1">
       <c r="A183" s="20">
         <v>347</v>
       </c>
@@ -13707,7 +13695,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="188.5">
+    <row r="184" spans="1:20" ht="188.5" hidden="1">
       <c r="A184" s="20">
         <v>350</v>
       </c>
@@ -13741,7 +13729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="217.5">
+    <row r="185" spans="1:20" ht="217.5" hidden="1">
       <c r="A185" s="20">
         <v>351</v>
       </c>
@@ -13775,7 +13763,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="145">
+    <row r="186" spans="1:20" ht="145" hidden="1">
       <c r="A186" s="20">
         <v>1</v>
       </c>
@@ -13809,7 +13797,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="145">
+    <row r="187" spans="1:20" ht="145" hidden="1">
       <c r="A187" s="20">
         <v>2</v>
       </c>
@@ -13843,7 +13831,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="145">
+    <row r="188" spans="1:20" ht="145" hidden="1">
       <c r="A188" s="20">
         <v>3</v>
       </c>
@@ -13877,7 +13865,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="145">
+    <row r="189" spans="1:20" ht="145" hidden="1">
       <c r="A189" s="20">
         <v>4</v>
       </c>
@@ -13911,7 +13899,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="145">
+    <row r="190" spans="1:20" ht="145" hidden="1">
       <c r="A190" s="20">
         <v>5</v>
       </c>
@@ -13945,7 +13933,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="130.5">
+    <row r="191" spans="1:20" ht="130.5" hidden="1">
       <c r="A191" s="20">
         <v>6</v>
       </c>
@@ -13979,7 +13967,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="130.5">
+    <row r="192" spans="1:20" ht="130.5" hidden="1">
       <c r="A192" s="20">
         <v>7</v>
       </c>
@@ -14013,7 +14001,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="130.5">
+    <row r="193" spans="1:20" ht="130.5" hidden="1">
       <c r="A193" s="20">
         <v>8</v>
       </c>
@@ -14047,7 +14035,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="130.5">
+    <row r="194" spans="1:20" ht="130.5" hidden="1">
       <c r="A194" s="20">
         <v>9</v>
       </c>
@@ -14241,7 +14229,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="130.5">
+    <row r="199" spans="1:20" ht="130.5" hidden="1">
       <c r="A199" s="20">
         <v>16</v>
       </c>
@@ -14275,7 +14263,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="130.5">
+    <row r="200" spans="1:20" ht="130.5" hidden="1">
       <c r="A200" s="20">
         <v>17</v>
       </c>
@@ -14309,7 +14297,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="130.5">
+    <row r="201" spans="1:20" ht="130.5" hidden="1">
       <c r="A201" s="20">
         <v>18</v>
       </c>
@@ -14343,7 +14331,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="130.5">
+    <row r="202" spans="1:20" ht="130.5" hidden="1">
       <c r="A202" s="20">
         <v>19</v>
       </c>
@@ -14377,7 +14365,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="130.5">
+    <row r="203" spans="1:20" ht="130.5" hidden="1">
       <c r="A203" s="20">
         <v>20</v>
       </c>
@@ -14411,7 +14399,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="130.5">
+    <row r="204" spans="1:20" ht="130.5" hidden="1">
       <c r="A204" s="20">
         <v>21</v>
       </c>
@@ -14445,7 +14433,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="130.5">
+    <row r="205" spans="1:20" ht="130.5" hidden="1">
       <c r="A205" s="20">
         <v>22</v>
       </c>
@@ -14479,7 +14467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="130.5">
+    <row r="206" spans="1:20" ht="130.5" hidden="1">
       <c r="A206" s="20">
         <v>23</v>
       </c>
@@ -14513,7 +14501,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="130.5">
+    <row r="207" spans="1:20" ht="130.5" hidden="1">
       <c r="A207" s="20">
         <v>24</v>
       </c>
@@ -14547,7 +14535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="130.5">
+    <row r="208" spans="1:20" ht="130.5" hidden="1">
       <c r="A208" s="20">
         <v>25</v>
       </c>
@@ -14581,7 +14569,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="130.5">
+    <row r="209" spans="1:20" ht="130.5" hidden="1">
       <c r="A209" s="20">
         <v>26</v>
       </c>
@@ -14615,7 +14603,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="130.5">
+    <row r="210" spans="1:20" ht="130.5" hidden="1">
       <c r="A210" s="20">
         <v>27</v>
       </c>
@@ -14649,7 +14637,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="145">
+    <row r="211" spans="1:20" ht="145" hidden="1">
       <c r="A211" s="20">
         <v>28</v>
       </c>
@@ -14683,7 +14671,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="145">
+    <row r="212" spans="1:20" ht="145" hidden="1">
       <c r="A212" s="20">
         <v>29</v>
       </c>
@@ -14717,7 +14705,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="145">
+    <row r="213" spans="1:20" ht="145" hidden="1">
       <c r="A213" s="20">
         <v>30</v>
       </c>
@@ -14809,7 +14797,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="145">
+    <row r="215" spans="1:20" ht="145" hidden="1">
       <c r="A215" s="20">
         <v>32</v>
       </c>
@@ -14843,7 +14831,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="145">
+    <row r="216" spans="1:20" ht="145" hidden="1">
       <c r="A216" s="20">
         <v>33</v>
       </c>
@@ -14877,7 +14865,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="145">
+    <row r="217" spans="1:20" ht="145" hidden="1">
       <c r="A217" s="20">
         <v>34</v>
       </c>
@@ -14911,7 +14899,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="145">
+    <row r="218" spans="1:20" ht="145" hidden="1">
       <c r="A218" s="20">
         <v>35</v>
       </c>
@@ -14945,7 +14933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="145">
+    <row r="219" spans="1:20" ht="145" hidden="1">
       <c r="A219" s="20">
         <v>36</v>
       </c>
@@ -14979,7 +14967,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="145">
+    <row r="220" spans="1:20" ht="145" hidden="1">
       <c r="A220" s="20">
         <v>37</v>
       </c>
@@ -15013,7 +15001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="145">
+    <row r="221" spans="1:20" ht="145" hidden="1">
       <c r="A221" s="20">
         <v>38</v>
       </c>
@@ -15085,7 +15073,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="145">
+    <row r="223" spans="1:20" ht="145" hidden="1">
       <c r="A223" s="20">
         <v>40</v>
       </c>
@@ -15119,7 +15107,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="145">
+    <row r="224" spans="1:20" ht="145" hidden="1">
       <c r="A224" s="20">
         <v>41</v>
       </c>
@@ -15153,7 +15141,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="145">
+    <row r="225" spans="1:20" ht="145" hidden="1">
       <c r="A225" s="20">
         <v>42</v>
       </c>
@@ -15187,7 +15175,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="145">
+    <row r="226" spans="1:20" ht="145" hidden="1">
       <c r="A226" s="20">
         <v>43</v>
       </c>
@@ -15221,7 +15209,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="43.5">
+    <row r="227" spans="1:20" ht="43.5" hidden="1">
       <c r="A227" s="20">
         <v>44</v>
       </c>
@@ -15257,7 +15245,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="43.5">
+    <row r="228" spans="1:20" ht="43.5" hidden="1">
       <c r="A228" s="20">
         <v>45</v>
       </c>
@@ -15293,7 +15281,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="43.5">
+    <row r="229" spans="1:20" ht="43.5" hidden="1">
       <c r="A229" s="20">
         <v>46</v>
       </c>
@@ -15375,7 +15363,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="43.5">
+    <row r="231" spans="1:20" ht="43.5" hidden="1">
       <c r="A231" s="20">
         <v>48</v>
       </c>
@@ -15411,7 +15399,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="43.5">
+    <row r="232" spans="1:20" ht="43.5" hidden="1">
       <c r="A232" s="20">
         <v>49</v>
       </c>
@@ -15447,7 +15435,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="43.5">
+    <row r="233" spans="1:20" ht="43.5" hidden="1">
       <c r="A233" s="20">
         <v>50</v>
       </c>
@@ -15483,7 +15471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="43.5">
+    <row r="234" spans="1:20" ht="43.5" hidden="1">
       <c r="A234" s="20">
         <v>51</v>
       </c>
@@ -15519,7 +15507,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="116">
+    <row r="235" spans="1:20" ht="116" hidden="1">
       <c r="A235" s="20">
         <v>52</v>
       </c>
@@ -15553,7 +15541,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="116">
+    <row r="236" spans="1:20" ht="116" hidden="1">
       <c r="A236" s="20">
         <v>53</v>
       </c>
@@ -15587,7 +15575,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="116">
+    <row r="237" spans="1:20" ht="116" hidden="1">
       <c r="A237" s="20">
         <v>54</v>
       </c>
@@ -15621,7 +15609,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="116">
+    <row r="238" spans="1:20" ht="116" hidden="1">
       <c r="A238" s="20">
         <v>55</v>
       </c>
@@ -15655,7 +15643,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="116">
+    <row r="239" spans="1:20" ht="116" hidden="1">
       <c r="A239" s="20">
         <v>56</v>
       </c>
@@ -15689,7 +15677,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="116">
+    <row r="240" spans="1:20" ht="116" hidden="1">
       <c r="A240" s="20">
         <v>57</v>
       </c>
@@ -15723,7 +15711,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="116">
+    <row r="241" spans="1:20" ht="116" hidden="1">
       <c r="A241" s="20">
         <v>58</v>
       </c>
@@ -15757,7 +15745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="116">
+    <row r="242" spans="1:20" ht="116" hidden="1">
       <c r="A242" s="20">
         <v>59</v>
       </c>
@@ -15791,7 +15779,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="116">
+    <row r="243" spans="1:20" ht="116" hidden="1">
       <c r="A243" s="20">
         <v>60</v>
       </c>
@@ -15825,7 +15813,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="116">
+    <row r="244" spans="1:20" ht="116" hidden="1">
       <c r="A244" s="20">
         <v>61</v>
       </c>
@@ -15859,7 +15847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="116">
+    <row r="245" spans="1:20" ht="116" hidden="1">
       <c r="A245" s="20">
         <v>62</v>
       </c>
@@ -15893,7 +15881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="116">
+    <row r="246" spans="1:20" ht="116" hidden="1">
       <c r="A246" s="20">
         <v>63</v>
       </c>
@@ -15927,7 +15915,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="116">
+    <row r="247" spans="1:20" ht="116" hidden="1">
       <c r="A247" s="20">
         <v>64</v>
       </c>
@@ -15961,7 +15949,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="116">
+    <row r="248" spans="1:20" ht="116" hidden="1">
       <c r="A248" s="20">
         <v>65</v>
       </c>
@@ -15995,7 +15983,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="116">
+    <row r="249" spans="1:20" ht="116" hidden="1">
       <c r="A249" s="20">
         <v>66</v>
       </c>
@@ -16029,7 +16017,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="116">
+    <row r="250" spans="1:20" ht="116" hidden="1">
       <c r="A250" s="20">
         <v>67</v>
       </c>
@@ -16063,7 +16051,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="116">
+    <row r="251" spans="1:20" ht="116" hidden="1">
       <c r="A251" s="20">
         <v>68</v>
       </c>
@@ -16097,7 +16085,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="116">
+    <row r="252" spans="1:20" ht="116" hidden="1">
       <c r="A252" s="20">
         <v>69</v>
       </c>
@@ -16131,7 +16119,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="116">
+    <row r="253" spans="1:20" ht="116" hidden="1">
       <c r="A253" s="20">
         <v>70</v>
       </c>
@@ -16165,7 +16153,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="116">
+    <row r="254" spans="1:20" ht="116" hidden="1">
       <c r="A254" s="20">
         <v>71</v>
       </c>
@@ -16199,7 +16187,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="116">
+    <row r="255" spans="1:20" ht="116" hidden="1">
       <c r="A255" s="20">
         <v>72</v>
       </c>
@@ -16233,7 +16221,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="116">
+    <row r="256" spans="1:20" ht="116" hidden="1">
       <c r="A256" s="20">
         <v>73</v>
       </c>
@@ -16267,7 +16255,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="116">
+    <row r="257" spans="1:20" ht="116" hidden="1">
       <c r="A257" s="20">
         <v>74</v>
       </c>
@@ -16489,38 +16477,22 @@
       <c r="E262" s="22" t="s">
         <v>552</v>
       </c>
-      <c r="F262" s="33">
-        <v>45063</v>
-      </c>
-      <c r="G262" s="34" t="s">
-        <v>858</v>
-      </c>
-      <c r="H262" s="34" t="s">
-        <v>859</v>
-      </c>
-      <c r="I262" s="34" t="s">
-        <v>860</v>
-      </c>
+      <c r="F262" s="33"/>
+      <c r="G262" s="34"/>
+      <c r="H262" s="34"/>
+      <c r="I262" s="34"/>
       <c r="J262" s="35" t="s">
-        <v>489</v>
-      </c>
-      <c r="K262" s="35"/>
-      <c r="L262" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="M262" s="35" t="s">
-        <v>843</v>
-      </c>
+      <c r="K262" s="35" t="s">
+        <v>878</v>
+      </c>
+      <c r="L262" s="35"/>
+      <c r="M262" s="35"/>
       <c r="N262" s="35"/>
-      <c r="O262" s="35" t="s">
-        <v>489</v>
-      </c>
-      <c r="P262" s="35" t="s">
-        <v>845</v>
-      </c>
-      <c r="Q262" s="35" t="s">
-        <v>827</v>
-      </c>
+      <c r="O262" s="35"/>
+      <c r="P262" s="35"/>
+      <c r="Q262" s="35"/>
       <c r="R262" s="36"/>
       <c r="S262" s="37"/>
       <c r="T262" s="28" t="s">
@@ -16547,13 +16519,13 @@
         <v>45063</v>
       </c>
       <c r="G263" s="34" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="H263" s="34" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="I263" s="34" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="J263" s="35" t="s">
         <v>489</v>
@@ -16566,7 +16538,7 @@
         <v>843</v>
       </c>
       <c r="N263" s="35" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="O263" s="35" t="s">
         <v>489</v>
@@ -16579,7 +16551,7 @@
       </c>
       <c r="R263" s="36"/>
       <c r="S263" s="37" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="T263" s="28" t="s">
         <v>51</v>
@@ -16609,7 +16581,7 @@
         <v>829</v>
       </c>
       <c r="K264" s="35" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="L264" s="35"/>
       <c r="M264" s="35"/>
@@ -16643,13 +16615,13 @@
         <v>45064</v>
       </c>
       <c r="G265" s="34" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="H265" s="38" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="I265" s="34" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="J265" s="35" t="s">
         <v>489</v>
@@ -16662,7 +16634,7 @@
         <v>843</v>
       </c>
       <c r="N265" s="35" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="O265" s="35" t="s">
         <v>489</v>
@@ -16697,40 +16669,22 @@
       <c r="E266" s="22" t="s">
         <v>560</v>
       </c>
-      <c r="F266" s="33">
-        <v>45064</v>
-      </c>
-      <c r="G266" s="34" t="s">
-        <v>871</v>
-      </c>
-      <c r="H266" s="34" t="s">
-        <v>872</v>
-      </c>
-      <c r="I266" s="34" t="s">
-        <v>873</v>
-      </c>
+      <c r="F266" s="33"/>
+      <c r="G266" s="34"/>
+      <c r="H266" s="34"/>
+      <c r="I266" s="34"/>
       <c r="J266" s="35" t="s">
-        <v>489</v>
-      </c>
-      <c r="K266" s="35"/>
-      <c r="L266" s="35" t="s">
         <v>829</v>
       </c>
-      <c r="M266" s="35" t="s">
-        <v>829</v>
-      </c>
-      <c r="N266" s="35" t="s">
-        <v>884</v>
-      </c>
-      <c r="O266" s="35" t="s">
-        <v>489</v>
-      </c>
-      <c r="P266" s="35" t="s">
-        <v>845</v>
-      </c>
-      <c r="Q266" s="35" t="s">
-        <v>827</v>
-      </c>
+      <c r="K266" s="35" t="s">
+        <v>879</v>
+      </c>
+      <c r="L266" s="35"/>
+      <c r="M266" s="35"/>
+      <c r="N266" s="35"/>
+      <c r="O266" s="35"/>
+      <c r="P266" s="35"/>
+      <c r="Q266" s="35"/>
       <c r="R266" s="36"/>
       <c r="S266" s="37"/>
       <c r="T266" s="28" t="s">
@@ -16757,13 +16711,13 @@
         <v>45064</v>
       </c>
       <c r="G267" s="34" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="H267" s="34" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="I267" s="34" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="J267" s="35" t="s">
         <v>489</v>
@@ -16776,7 +16730,7 @@
         <v>843</v>
       </c>
       <c r="N267" s="35" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="O267" s="35" t="s">
         <v>489</v>
@@ -16817,7 +16771,7 @@
         <v>829</v>
       </c>
       <c r="K268" s="35" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
       <c r="L268" s="35"/>
       <c r="M268" s="35"/>
@@ -16855,7 +16809,7 @@
         <v>829</v>
       </c>
       <c r="K269" s="35" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="L269" s="35"/>
       <c r="M269" s="35"/>
@@ -16893,7 +16847,7 @@
         <v>829</v>
       </c>
       <c r="K270" s="35" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="L270" s="35"/>
       <c r="M270" s="35"/>
@@ -16931,7 +16885,7 @@
         <v>829</v>
       </c>
       <c r="K271" s="35" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="L271" s="35"/>
       <c r="M271" s="35"/>
@@ -16969,7 +16923,7 @@
         <v>829</v>
       </c>
       <c r="K272" s="35" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="L272" s="35"/>
       <c r="M272" s="35"/>
@@ -17007,7 +16961,7 @@
         <v>829</v>
       </c>
       <c r="K273" s="35" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="L273" s="35"/>
       <c r="M273" s="35"/>
@@ -17045,7 +16999,7 @@
         <v>829</v>
       </c>
       <c r="K274" s="35" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="L274" s="35"/>
       <c r="M274" s="35"/>
@@ -17083,7 +17037,7 @@
         <v>829</v>
       </c>
       <c r="K275" s="35" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="L275" s="35"/>
       <c r="M275" s="35"/>
@@ -17121,7 +17075,7 @@
         <v>829</v>
       </c>
       <c r="K276" s="35" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="L276" s="35"/>
       <c r="M276" s="35"/>
@@ -17135,7 +17089,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="130.5">
+    <row r="277" spans="1:20" ht="130.5" hidden="1">
       <c r="A277" s="20">
         <v>94</v>
       </c>
@@ -17169,7 +17123,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="130.5">
+    <row r="278" spans="1:20" ht="130.5" hidden="1">
       <c r="A278" s="20">
         <v>95</v>
       </c>
@@ -17203,7 +17157,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="101.5">
+    <row r="279" spans="1:20" ht="101.5" hidden="1">
       <c r="A279" s="20">
         <v>96</v>
       </c>
@@ -17237,7 +17191,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="116">
+    <row r="280" spans="1:20" ht="116" hidden="1">
       <c r="A280" s="20">
         <v>97</v>
       </c>
@@ -17271,7 +17225,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="130.5">
+    <row r="281" spans="1:20" ht="130.5" hidden="1">
       <c r="A281" s="20">
         <v>98</v>
       </c>
@@ -17305,7 +17259,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="130.5">
+    <row r="282" spans="1:20" ht="130.5" hidden="1">
       <c r="A282" s="20">
         <v>99</v>
       </c>
@@ -17339,7 +17293,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="101.5">
+    <row r="283" spans="1:20" ht="101.5" hidden="1">
       <c r="A283" s="20">
         <v>100</v>
       </c>
@@ -17373,7 +17327,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="116">
+    <row r="284" spans="1:20" ht="116" hidden="1">
       <c r="A284" s="20">
         <v>101</v>
       </c>
@@ -17407,7 +17361,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="130.5">
+    <row r="285" spans="1:20" ht="130.5" hidden="1">
       <c r="A285" s="20">
         <v>102</v>
       </c>
@@ -17441,7 +17395,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="130.5">
+    <row r="286" spans="1:20" ht="130.5" hidden="1">
       <c r="A286" s="20">
         <v>103</v>
       </c>
@@ -17475,7 +17429,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="101.5">
+    <row r="287" spans="1:20" ht="101.5" hidden="1">
       <c r="A287" s="20">
         <v>104</v>
       </c>
@@ -17509,7 +17463,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="130.5">
+    <row r="288" spans="1:20" ht="130.5" hidden="1">
       <c r="A288" s="20">
         <v>105</v>
       </c>
@@ -17543,7 +17497,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="130.5">
+    <row r="289" spans="1:20" ht="130.5" hidden="1">
       <c r="A289" s="20">
         <v>106</v>
       </c>
@@ -17577,7 +17531,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="116">
+    <row r="290" spans="1:20" ht="116" hidden="1">
       <c r="A290" s="20">
         <v>107</v>
       </c>
@@ -17611,7 +17565,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="116">
+    <row r="291" spans="1:20" ht="116" hidden="1">
       <c r="A291" s="20">
         <v>108</v>
       </c>
@@ -17645,7 +17599,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="116">
+    <row r="292" spans="1:20" ht="116" hidden="1">
       <c r="A292" s="20">
         <v>109</v>
       </c>
@@ -17679,7 +17633,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="101.5">
+    <row r="293" spans="1:20" ht="101.5" hidden="1">
       <c r="A293" s="20">
         <v>110</v>
       </c>
@@ -17713,7 +17667,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="116">
+    <row r="294" spans="1:20" ht="116" hidden="1">
       <c r="A294" s="20">
         <v>111</v>
       </c>
@@ -17747,7 +17701,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="116">
+    <row r="295" spans="1:20" ht="116" hidden="1">
       <c r="A295" s="20">
         <v>112</v>
       </c>
@@ -17781,7 +17735,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="116">
+    <row r="296" spans="1:20" ht="116" hidden="1">
       <c r="A296" s="20">
         <v>113</v>
       </c>
@@ -17815,7 +17769,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="116">
+    <row r="297" spans="1:20" ht="116" hidden="1">
       <c r="A297" s="20">
         <v>114</v>
       </c>
@@ -17849,7 +17803,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="116">
+    <row r="298" spans="1:20" ht="116" hidden="1">
       <c r="A298" s="20">
         <v>115</v>
       </c>
@@ -17883,7 +17837,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="116">
+    <row r="299" spans="1:20" ht="116" hidden="1">
       <c r="A299" s="20">
         <v>116</v>
       </c>
@@ -17917,7 +17871,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="116">
+    <row r="300" spans="1:20" ht="116" hidden="1">
       <c r="A300" s="20">
         <v>117</v>
       </c>
@@ -17951,7 +17905,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="116">
+    <row r="301" spans="1:20" ht="116" hidden="1">
       <c r="A301" s="20">
         <v>118</v>
       </c>
@@ -17985,7 +17939,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="116">
+    <row r="302" spans="1:20" ht="116" hidden="1">
       <c r="A302" s="20">
         <v>119</v>
       </c>
@@ -18019,7 +17973,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="116">
+    <row r="303" spans="1:20" ht="116" hidden="1">
       <c r="A303" s="20">
         <v>120</v>
       </c>
@@ -18053,7 +18007,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="116">
+    <row r="304" spans="1:20" ht="116" hidden="1">
       <c r="A304" s="20">
         <v>121</v>
       </c>
@@ -18087,7 +18041,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="101.5">
+    <row r="305" spans="1:20" ht="101.5" hidden="1">
       <c r="A305" s="20">
         <v>122</v>
       </c>
@@ -18121,7 +18075,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="101.5">
+    <row r="306" spans="1:20" ht="101.5" hidden="1">
       <c r="A306" s="20">
         <v>123</v>
       </c>
@@ -18155,7 +18109,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="101.5">
+    <row r="307" spans="1:20" ht="101.5" hidden="1">
       <c r="A307" s="20">
         <v>124</v>
       </c>
@@ -18189,7 +18143,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="116">
+    <row r="308" spans="1:20" ht="116" hidden="1">
       <c r="A308" s="20">
         <v>125</v>
       </c>
@@ -18223,7 +18177,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="101.5">
+    <row r="309" spans="1:20" ht="101.5" hidden="1">
       <c r="A309" s="20">
         <v>126</v>
       </c>
@@ -18257,7 +18211,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="101.5">
+    <row r="310" spans="1:20" ht="101.5" hidden="1">
       <c r="A310" s="20">
         <v>127</v>
       </c>
@@ -18291,7 +18245,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="101.5">
+    <row r="311" spans="1:20" ht="101.5" hidden="1">
       <c r="A311" s="20">
         <v>128</v>
       </c>
@@ -18325,7 +18279,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="116">
+    <row r="312" spans="1:20" ht="116" hidden="1">
       <c r="A312" s="20">
         <v>129</v>
       </c>
@@ -18359,7 +18313,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="101.5">
+    <row r="313" spans="1:20" ht="101.5" hidden="1">
       <c r="A313" s="20">
         <v>130</v>
       </c>
@@ -18393,7 +18347,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="101.5">
+    <row r="314" spans="1:20" ht="101.5" hidden="1">
       <c r="A314" s="20">
         <v>131</v>
       </c>
@@ -18427,7 +18381,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="101.5">
+    <row r="315" spans="1:20" ht="101.5" hidden="1">
       <c r="A315" s="20">
         <v>132</v>
       </c>
@@ -18461,7 +18415,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="116">
+    <row r="316" spans="1:20" ht="116" hidden="1">
       <c r="A316" s="20">
         <v>133</v>
       </c>
@@ -18495,7 +18449,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="101.5">
+    <row r="317" spans="1:20" ht="101.5" hidden="1">
       <c r="A317" s="20">
         <v>134</v>
       </c>
@@ -18529,7 +18483,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="101.5">
+    <row r="318" spans="1:20" ht="101.5" hidden="1">
       <c r="A318" s="20">
         <v>135</v>
       </c>
@@ -18563,7 +18517,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="101.5">
+    <row r="319" spans="1:20" ht="101.5" hidden="1">
       <c r="A319" s="20">
         <v>136</v>
       </c>
@@ -18597,7 +18551,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="116">
+    <row r="320" spans="1:20" ht="116" hidden="1">
       <c r="A320" s="20">
         <v>137</v>
       </c>
@@ -18631,7 +18585,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="101.5">
+    <row r="321" spans="1:20" ht="101.5" hidden="1">
       <c r="A321" s="20">
         <v>138</v>
       </c>
@@ -18665,7 +18619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="101.5">
+    <row r="322" spans="1:20" ht="101.5" hidden="1">
       <c r="A322" s="20">
         <v>139</v>
       </c>
@@ -18699,7 +18653,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="101.5">
+    <row r="323" spans="1:20" ht="101.5" hidden="1">
       <c r="A323" s="20">
         <v>140</v>
       </c>
@@ -18733,7 +18687,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="116">
+    <row r="324" spans="1:20" ht="116" hidden="1">
       <c r="A324" s="20">
         <v>141</v>
       </c>
@@ -18767,7 +18721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="101.5">
+    <row r="325" spans="1:20" ht="101.5" hidden="1">
       <c r="A325" s="20">
         <v>142</v>
       </c>
@@ -18801,7 +18755,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="101.5">
+    <row r="326" spans="1:20" ht="101.5" hidden="1">
       <c r="A326" s="20">
         <v>143</v>
       </c>
@@ -18835,7 +18789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="101.5">
+    <row r="327" spans="1:20" ht="101.5" hidden="1">
       <c r="A327" s="20">
         <v>144</v>
       </c>
@@ -18869,7 +18823,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="116">
+    <row r="328" spans="1:20" ht="116" hidden="1">
       <c r="A328" s="20">
         <v>145</v>
       </c>
@@ -18903,7 +18857,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="329" spans="1:20" ht="116">
+    <row r="329" spans="1:20" ht="116" hidden="1">
       <c r="A329" s="20">
         <v>146</v>
       </c>
@@ -18937,7 +18891,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="159.5">
+    <row r="330" spans="1:20" ht="159.5" hidden="1">
       <c r="A330" s="20">
         <v>147</v>
       </c>
@@ -18971,7 +18925,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="159.5">
+    <row r="331" spans="1:20" ht="159.5" hidden="1">
       <c r="A331" s="20">
         <v>148</v>
       </c>
@@ -19005,7 +18959,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="159.5">
+    <row r="332" spans="1:20" ht="159.5" hidden="1">
       <c r="A332" s="20">
         <v>149</v>
       </c>
@@ -19039,7 +18993,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="159.5">
+    <row r="333" spans="1:20" ht="159.5" hidden="1">
       <c r="A333" s="20">
         <v>150</v>
       </c>
@@ -19073,7 +19027,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="101.5">
+    <row r="334" spans="1:20" ht="101.5" hidden="1">
       <c r="A334" s="20">
         <v>151</v>
       </c>
@@ -19107,7 +19061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="116">
+    <row r="335" spans="1:20" ht="116" hidden="1">
       <c r="A335" s="20">
         <v>152</v>
       </c>
@@ -19141,7 +19095,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="116">
+    <row r="336" spans="1:20" ht="116" hidden="1">
       <c r="A336" s="20">
         <v>153</v>
       </c>
@@ -19175,7 +19129,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="116">
+    <row r="337" spans="1:20" ht="116" hidden="1">
       <c r="A337" s="20">
         <v>154</v>
       </c>
@@ -19209,7 +19163,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="116">
+    <row r="338" spans="1:20" ht="116" hidden="1">
       <c r="A338" s="20">
         <v>155</v>
       </c>
@@ -19243,7 +19197,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="116">
+    <row r="339" spans="1:20" ht="116" hidden="1">
       <c r="A339" s="20">
         <v>156</v>
       </c>
@@ -19277,7 +19231,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="116">
+    <row r="340" spans="1:20" ht="116" hidden="1">
       <c r="A340" s="20">
         <v>157</v>
       </c>
@@ -19311,7 +19265,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="116">
+    <row r="341" spans="1:20" ht="116" hidden="1">
       <c r="A341" s="20">
         <v>158</v>
       </c>
@@ -19345,7 +19299,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="101.5">
+    <row r="342" spans="1:20" ht="101.5" hidden="1">
       <c r="A342" s="20">
         <v>159</v>
       </c>
@@ -19379,7 +19333,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="101.5">
+    <row r="343" spans="1:20" ht="101.5" hidden="1">
       <c r="A343" s="20">
         <v>160</v>
       </c>
@@ -19413,7 +19367,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="116">
+    <row r="344" spans="1:20" ht="116" hidden="1">
       <c r="A344" s="20">
         <v>161</v>
       </c>
@@ -19447,7 +19401,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="116">
+    <row r="345" spans="1:20" ht="116" hidden="1">
       <c r="A345" s="20">
         <v>162</v>
       </c>
@@ -19481,7 +19435,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="116">
+    <row r="346" spans="1:20" ht="116" hidden="1">
       <c r="A346" s="20">
         <v>163</v>
       </c>
@@ -19515,7 +19469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="116">
+    <row r="347" spans="1:20" ht="116" hidden="1">
       <c r="A347" s="20">
         <v>164</v>
       </c>
@@ -19549,7 +19503,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="116">
+    <row r="348" spans="1:20" ht="116" hidden="1">
       <c r="A348" s="20">
         <v>165</v>
       </c>
@@ -19583,7 +19537,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="116">
+    <row r="349" spans="1:20" ht="116" hidden="1">
       <c r="A349" s="20">
         <v>166</v>
       </c>
@@ -19617,7 +19571,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="116">
+    <row r="350" spans="1:20" ht="116" hidden="1">
       <c r="A350" s="20">
         <v>167</v>
       </c>
@@ -19651,7 +19605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="116">
+    <row r="351" spans="1:20" ht="116" hidden="1">
       <c r="A351" s="20">
         <v>168</v>
       </c>
@@ -19685,7 +19639,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="116">
+    <row r="352" spans="1:20" ht="116" hidden="1">
       <c r="A352" s="20">
         <v>169</v>
       </c>
@@ -19719,7 +19673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="145">
+    <row r="353" spans="1:20" ht="145" hidden="1">
       <c r="A353" s="20">
         <v>170</v>
       </c>
@@ -19753,7 +19707,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="145">
+    <row r="354" spans="1:20" ht="145" hidden="1">
       <c r="A354" s="20">
         <v>171</v>
       </c>
@@ -19787,7 +19741,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="145">
+    <row r="355" spans="1:20" ht="145" hidden="1">
       <c r="A355" s="20">
         <v>172</v>
       </c>
@@ -19821,7 +19775,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="145">
+    <row r="356" spans="1:20" ht="145" hidden="1">
       <c r="A356" s="20">
         <v>173</v>
       </c>
@@ -19855,7 +19809,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="101.5">
+    <row r="357" spans="1:20" ht="101.5" hidden="1">
       <c r="A357" s="20">
         <v>174</v>
       </c>
@@ -19889,7 +19843,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="116">
+    <row r="358" spans="1:20" ht="116" hidden="1">
       <c r="A358" s="20">
         <v>175</v>
       </c>
@@ -19923,7 +19877,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="116">
+    <row r="359" spans="1:20" ht="116" hidden="1">
       <c r="A359" s="20">
         <v>176</v>
       </c>
@@ -19957,7 +19911,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="360" spans="1:20" ht="116">
+    <row r="360" spans="1:20" ht="116" hidden="1">
       <c r="A360" s="20">
         <v>177</v>
       </c>
@@ -19991,7 +19945,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="116">
+    <row r="361" spans="1:20" ht="116" hidden="1">
       <c r="A361" s="20">
         <v>178</v>
       </c>
@@ -20025,7 +19979,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="116">
+    <row r="362" spans="1:20" ht="116" hidden="1">
       <c r="A362" s="20">
         <v>179</v>
       </c>
@@ -20059,7 +20013,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="116">
+    <row r="363" spans="1:20" ht="116" hidden="1">
       <c r="A363" s="20">
         <v>180</v>
       </c>
@@ -20093,7 +20047,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="101.5">
+    <row r="364" spans="1:20" ht="101.5" hidden="1">
       <c r="A364" s="20">
         <v>181</v>
       </c>
@@ -20127,7 +20081,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="116">
+    <row r="365" spans="1:20" ht="116" hidden="1">
       <c r="A365" s="20">
         <v>182</v>
       </c>
@@ -20161,7 +20115,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="116">
+    <row r="366" spans="1:20" ht="116" hidden="1">
       <c r="A366" s="20">
         <v>183</v>
       </c>
@@ -20195,7 +20149,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="116">
+    <row r="367" spans="1:20" ht="116" hidden="1">
       <c r="A367" s="20">
         <v>184</v>
       </c>
@@ -20229,7 +20183,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="116">
+    <row r="368" spans="1:20" ht="116" hidden="1">
       <c r="A368" s="20">
         <v>185</v>
       </c>
@@ -20263,7 +20217,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="116">
+    <row r="369" spans="1:20" ht="116" hidden="1">
       <c r="A369" s="20">
         <v>186</v>
       </c>
@@ -20297,7 +20251,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="116">
+    <row r="370" spans="1:20" ht="116" hidden="1">
       <c r="A370" s="20">
         <v>187</v>
       </c>
@@ -20331,7 +20285,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="116">
+    <row r="371" spans="1:20" ht="116" hidden="1">
       <c r="A371" s="20">
         <v>188</v>
       </c>
@@ -20365,7 +20319,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="116">
+    <row r="372" spans="1:20" ht="116" hidden="1">
       <c r="A372" s="20">
         <v>189</v>
       </c>
@@ -20399,7 +20353,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="116">
+    <row r="373" spans="1:20" ht="116" hidden="1">
       <c r="A373" s="20">
         <v>190</v>
       </c>
@@ -20433,7 +20387,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="145">
+    <row r="374" spans="1:20" ht="145" hidden="1">
       <c r="A374" s="20">
         <v>191</v>
       </c>
@@ -30065,6 +30019,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T374" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="RAD"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:T374">
       <sortCondition ref="B9:B374"/>
     </sortState>
@@ -32823,8 +32782,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A052E4B0CBFBEE42A9BE94735C648D6A" ma:contentTypeVersion="15" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="46c42a7787fc2c2b7e7cfe1959215247">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xmlns:ns3="bb0bfb2d-9415-422c-9311-cf5d9d9d5142" xmlns:ns4="49919dca-d9c1-492f-bd36-8a887e31a6e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e12afe9cdb5af13725bc2bdd4e9733a" ns2:_="" ns3:_="" ns4:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="49919dca-d9c1-492f-bd36-8a887e31a6e3" xsi:nil="true"/>
+    <Tag xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A052E4B0CBFBEE42A9BE94735C648D6A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4e5f9d650d253b7a3d6ed53057f6e63e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xmlns:ns3="bb0bfb2d-9415-422c-9311-cf5d9d9d5142" xmlns:ns4="49919dca-d9c1-492f-bd36-8a887e31a6e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d80d0c74ac61bb9026b243c0c584c36" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
     <xsd:import namespace="bb0bfb2d-9415-422c-9311-cf5d9d9d5142"/>
     <xsd:import namespace="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
@@ -32914,7 +32899,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Tag immagine" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -32925,7 +32910,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bb0bfb2d-9415-422c-9311-cf5d9d9d5142" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Condiviso con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -32944,7 +32929,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Condiviso con dettagli" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -32976,8 +32961,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo di contenuto"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titolo"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -33066,34 +33051,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="49919dca-d9c1-492f-bd36-8a887e31a6e3" xsi:nil="true"/>
-    <Tag xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2850EEF4-EC69-4F2E-B0CE-8034B61489F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
+    <ds:schemaRef ds:uri="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ContentTypeId="0x01" PreviousValue="false"/>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C0D72B-6AAC-4529-B934-502AA3EA2A0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12D86236-EAFC-48DB-B351-E7598A8B8AB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{330C73C0-97BE-4E44-9B85-0CBBC432A409}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C73319A0-5C18-48A7-95DC-DC52937F884B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -33110,31 +33096,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2850EEF4-EC69-4F2E-B0CE-8034B61489F3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
-    <ds:schemaRef ds:uri="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C0D72B-6AAC-4529-B934-502AA3EA2A0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12D86236-EAFC-48DB-B351-E7598A8B8AB2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
All the validation tests have been done again
Added attribute ID to the XML nodes "component\structuredBody\component\section"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111PHILIPSXXXX/Philips/VuePACS-SignPlugin/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111PHILIPSXXXX/Philips/VuePACS-SignPlugin/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.philips.com/sites/HCISIntegration260/Integration Project Docs/EAMER/Italy/FSE 2.0/Accreditamento/file da sottomettere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9530529-A5B9-422E-8FC5-8A415B4E4272}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F65A2B2-A164-4272-B991-C03B9C417839}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4461,15 +4461,6 @@
     <t>Philips S.p.A.</t>
   </si>
   <si>
-    <t>2023-05-17T15:24:43.639Z</t>
-  </si>
-  <si>
-    <t>66296585b66b6b4e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.f7690455e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il sistema non gestisce la sezione opzionale "Conclusioni"</t>
   </si>
   <si>
@@ -4515,18 +4506,6 @@
     <t>Il sistema non prevede che il campo confidentialityCode/code sia vuoto</t>
   </si>
   <si>
-    <t>2023-05-17T17:49:18.061Z</t>
-  </si>
-  <si>
-    <t>58a7d1def3a620d8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.9321860ea510f21ed9d48c4459656e023041ce3dba23733394ffa5d9191d4d3a.3eef5e58c5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>title:"Errore semantico.","detail":"[Errore-46| codice fiscale 'tstcfs91h67h501f' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]","status":422,"instance":"/validation/error"</t>
-  </si>
-  <si>
     <t>Casistica gestita a livello di sistema. Normalmente questa situazione non si presenterà mai, in quanto impedita dalle regole implementate a livello di integrazione.</t>
   </si>
   <si>
@@ -4536,48 +4515,12 @@
     <t>Il sistema non prevede il campo opzionale indirizzo del paziente</t>
   </si>
   <si>
-    <t>2023-05-17T16:21:54.999Z</t>
-  </si>
-  <si>
-    <t>47111035032ae366</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.e5827c19fb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>title:"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: C]","status":400,"instance":"/validation/error"</t>
-  </si>
-  <si>
     <t>Casistica gestita a livello di sistema. Normalmente questa situazione non si presenterà mai, in quanto impedita dalle regole implementate a livello di integrazione (nel caso di valore diverso da M o F viene assegnato il valore di default "U").</t>
   </si>
   <si>
     <t>Il sistema non prevede il campo opzionale documentationOf</t>
   </si>
   <si>
-    <t>2023-05-18T09:30:18.195Z</t>
-  </si>
-  <si>
-    <t>1558e411e15285fe</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.e26ae1ef855d1a17087cd17b682ed6e932cff5d3dac28db235038885d766c28d.0577af3456^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>title:"Errore semantico.","detail":"[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ]","status":422,"instance":"/validation/error"</t>
-  </si>
-  <si>
-    <t>2023-05-18T09:40:43.581Z</t>
-  </si>
-  <si>
-    <t>47d04cd9413216a9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.ea8bb1101a26b96e8e4ddcc7563556243c103b50426ae3e3cff28c1bebb0d832.88cd0293a6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>title:"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.","status":400,"instance":"/validation/error"</t>
-  </si>
-  <si>
     <t>Il sistema non prevede che i campi della sezione "Referto" possano essere vuoti</t>
   </si>
   <si>
@@ -4600,6 +4543,69 @@
   </si>
   <si>
     <t xml:space="preserve">Il sistema genera sempre almeno un tag inFulfillmentOf/order/id, in quanto l'accession number è un prerequisito necessario e obbligatorio per la firma digitale. </t>
+  </si>
+  <si>
+    <t>2023-06-08T14:57:13.202Z</t>
+  </si>
+  <si>
+    <t>9fcca2520ba6ac7f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.367902f3ca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-08T15:29:26.708Z</t>
+  </si>
+  <si>
+    <t>2edab2b83fc894c0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.1573d3ffcd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>"title": "Errore semantico.",
+	"detail": "[Errore-46| codice fiscale 'tstpnt91h67h501a' cittadino ed operatore: 16 cifre[A-Z0-9]{16}]",
+	"status": 422,
+	"instance": "/validation/error"</t>
+  </si>
+  <si>
+    <t>2023-06-08T15:41:49.944Z</t>
+  </si>
+  <si>
+    <t>bf20c022cfa208dc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.adebda258e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>"title": "Errore vocabolario.",
+	"detail": "Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0,Codes:C]",
+	"status": 400,
+	"instance": "/validation/error"</t>
+  </si>
+  <si>
+    <t>2023-06-08T15:56:52.847Z</t>
+  </si>
+  <si>
+    <t>45694240b7c56567</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.e26ae1ef855d1a17087cd17b682ed6e932cff5d3dac28db235038885d766c28d.e4209f28df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>"title":"Errore semantico.","detail":"[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM']","status":422,"instance":"/validation/error"</t>
+  </si>
+  <si>
+    <t>2023-06-08T16:08:07.975Z</t>
+  </si>
+  <si>
+    <t>9258e79e6686c6ef</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.ea8bb1101a26b96e8e4ddcc7563556243c103b50426ae3e3cff28c1bebb0d832.b64930af7d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>"title":"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.","status":400,"instance":"/validation/error"</t>
   </si>
 </sst>
 </file>
@@ -5139,6 +5145,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:A3">
   <tableColumns count="1">
@@ -5361,10 +5371,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="149.1796875" customWidth="1"/>
-    <col min="2" max="26" width="8.90625" customWidth="1"/>
+    <col min="1" max="1" width="149.21875" customWidth="1"/>
+    <col min="2" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14.25" customHeight="1">
@@ -5372,32 +5382,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="87">
+    <row r="2" spans="1:1" ht="86.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.5">
+    <row r="3" spans="1:1" ht="14.4">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="174">
+    <row r="4" spans="1:1" ht="172.8">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="29">
+    <row r="5" spans="1:1" ht="28.8">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="29">
+    <row r="6" spans="1:1" ht="28.8">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.5">
+    <row r="7" spans="1:1" ht="14.4">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -6425,11 +6435,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.08984375" customWidth="1"/>
-    <col min="2" max="2" width="194.08984375" customWidth="1"/>
-    <col min="3" max="26" width="8.90625" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="194.109375" customWidth="1"/>
+    <col min="3" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -6501,7 +6511,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="43.5">
+    <row r="11" spans="1:2" ht="43.2">
       <c r="A11" s="10">
         <v>8</v>
       </c>
@@ -7522,27 +7532,27 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B264" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="E265" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A266" sqref="A266"/>
+      <selection pane="bottomRight" activeCell="I267" sqref="I267"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="46.90625" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" customWidth="1"/>
-    <col min="4" max="4" width="63.90625" customWidth="1"/>
-    <col min="5" max="5" width="104.90625" customWidth="1"/>
-    <col min="6" max="9" width="33.08984375" customWidth="1"/>
-    <col min="10" max="10" width="27.08984375" customWidth="1"/>
-    <col min="11" max="15" width="36.453125" customWidth="1"/>
-    <col min="16" max="16" width="27.08984375" customWidth="1"/>
-    <col min="17" max="17" width="33.08984375" customWidth="1"/>
-    <col min="18" max="18" width="36.453125" customWidth="1"/>
-    <col min="19" max="20" width="31.90625" customWidth="1"/>
-    <col min="21" max="26" width="8.90625" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="63.88671875" customWidth="1"/>
+    <col min="5" max="5" width="104.88671875" customWidth="1"/>
+    <col min="6" max="9" width="33.109375" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" customWidth="1"/>
+    <col min="11" max="15" width="36.44140625" customWidth="1"/>
+    <col min="16" max="16" width="27.109375" customWidth="1"/>
+    <col min="17" max="17" width="33.109375" customWidth="1"/>
+    <col min="18" max="18" width="36.44140625" customWidth="1"/>
+    <col min="19" max="20" width="31.88671875" customWidth="1"/>
+    <col min="21" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1">
@@ -7717,7 +7727,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="14.25" customHeight="1">
+    <row r="9" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -7779,7 +7789,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="232" hidden="1">
+    <row r="10" spans="1:20" ht="230.4" hidden="1">
       <c r="A10" s="20">
         <v>194</v>
       </c>
@@ -7813,7 +7823,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="217.5" hidden="1">
+    <row r="11" spans="1:20" ht="216" hidden="1">
       <c r="A11" s="20">
         <v>205</v>
       </c>
@@ -7847,7 +7857,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="232" hidden="1">
+    <row r="12" spans="1:20" ht="230.4" hidden="1">
       <c r="A12" s="20">
         <v>210</v>
       </c>
@@ -7881,7 +7891,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="217.5" hidden="1">
+    <row r="13" spans="1:20" ht="216" hidden="1">
       <c r="A13" s="20">
         <v>221</v>
       </c>
@@ -7915,7 +7925,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="232">
+    <row r="14" spans="1:20" ht="231" thickBot="1">
       <c r="A14" s="20">
         <v>226</v>
       </c>
@@ -7949,7 +7959,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="217.5">
+    <row r="15" spans="1:20" ht="216.6" thickBot="1">
       <c r="A15" s="20">
         <v>237</v>
       </c>
@@ -7983,7 +7993,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="232" hidden="1">
+    <row r="16" spans="1:20" ht="230.4" hidden="1">
       <c r="A16" s="20">
         <v>242</v>
       </c>
@@ -8017,7 +8027,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="217.5" hidden="1">
+    <row r="17" spans="1:20" ht="216" hidden="1">
       <c r="A17" s="20">
         <v>253</v>
       </c>
@@ -8051,7 +8061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="232" hidden="1">
+    <row r="18" spans="1:20" ht="230.4" hidden="1">
       <c r="A18" s="20">
         <v>258</v>
       </c>
@@ -8085,7 +8095,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="217.5" hidden="1">
+    <row r="19" spans="1:20" ht="216" hidden="1">
       <c r="A19" s="20">
         <v>269</v>
       </c>
@@ -8119,7 +8129,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="232" hidden="1">
+    <row r="20" spans="1:20" ht="230.4" hidden="1">
       <c r="A20" s="20">
         <v>274</v>
       </c>
@@ -8153,7 +8163,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="217.5" hidden="1">
+    <row r="21" spans="1:20" ht="216" hidden="1">
       <c r="A21" s="20">
         <v>285</v>
       </c>
@@ -8187,7 +8197,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="232" hidden="1">
+    <row r="22" spans="1:20" ht="230.4" hidden="1">
       <c r="A22" s="20">
         <v>290</v>
       </c>
@@ -8221,7 +8231,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="217.5" hidden="1">
+    <row r="23" spans="1:20" ht="216" hidden="1">
       <c r="A23" s="20">
         <v>301</v>
       </c>
@@ -8255,7 +8265,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="232" hidden="1">
+    <row r="24" spans="1:20" ht="230.4" hidden="1">
       <c r="A24" s="20">
         <v>306</v>
       </c>
@@ -8289,7 +8299,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="217.5" hidden="1">
+    <row r="25" spans="1:20" ht="216" hidden="1">
       <c r="A25" s="20">
         <v>317</v>
       </c>
@@ -8323,7 +8333,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="174" hidden="1">
+    <row r="26" spans="1:20" ht="172.8" hidden="1">
       <c r="A26" s="20">
         <v>352</v>
       </c>
@@ -8357,7 +8367,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="203" hidden="1">
+    <row r="27" spans="1:20" ht="201.6" hidden="1">
       <c r="A27" s="20">
         <v>353</v>
       </c>
@@ -8391,7 +8401,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="174" hidden="1">
+    <row r="28" spans="1:20" ht="172.8" hidden="1">
       <c r="A28" s="20">
         <v>354</v>
       </c>
@@ -8425,7 +8435,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="203" hidden="1">
+    <row r="29" spans="1:20" ht="201.6" hidden="1">
       <c r="A29" s="20">
         <v>355</v>
       </c>
@@ -8459,7 +8469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="174">
+    <row r="30" spans="1:20" ht="173.4" thickBot="1">
       <c r="A30" s="20">
         <v>356</v>
       </c>
@@ -8493,7 +8503,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="203">
+    <row r="31" spans="1:20" ht="202.2" thickBot="1">
       <c r="A31" s="20">
         <v>357</v>
       </c>
@@ -8527,7 +8537,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="174" hidden="1">
+    <row r="32" spans="1:20" ht="172.8" hidden="1">
       <c r="A32" s="20">
         <v>358</v>
       </c>
@@ -8561,7 +8571,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="203" hidden="1">
+    <row r="33" spans="1:20" ht="201.6" hidden="1">
       <c r="A33" s="20">
         <v>359</v>
       </c>
@@ -8595,7 +8605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="174" hidden="1">
+    <row r="34" spans="1:20" ht="172.8" hidden="1">
       <c r="A34" s="20">
         <v>360</v>
       </c>
@@ -8629,7 +8639,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="203" hidden="1">
+    <row r="35" spans="1:20" ht="201.6" hidden="1">
       <c r="A35" s="20">
         <v>361</v>
       </c>
@@ -8663,7 +8673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="174" hidden="1">
+    <row r="36" spans="1:20" ht="172.8" hidden="1">
       <c r="A36" s="20">
         <v>362</v>
       </c>
@@ -8697,7 +8707,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="203" hidden="1">
+    <row r="37" spans="1:20" ht="201.6" hidden="1">
       <c r="A37" s="20">
         <v>363</v>
       </c>
@@ -8731,7 +8741,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="174" hidden="1">
+    <row r="38" spans="1:20" ht="172.8" hidden="1">
       <c r="A38" s="20">
         <v>364</v>
       </c>
@@ -8765,7 +8775,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="203" hidden="1">
+    <row r="39" spans="1:20" ht="201.6" hidden="1">
       <c r="A39" s="20">
         <v>365</v>
       </c>
@@ -8799,7 +8809,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="174" hidden="1">
+    <row r="40" spans="1:20" ht="172.8" hidden="1">
       <c r="A40" s="20">
         <v>366</v>
       </c>
@@ -8833,7 +8843,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="203" hidden="1">
+    <row r="41" spans="1:20" ht="201.6" hidden="1">
       <c r="A41" s="20">
         <v>367</v>
       </c>
@@ -8867,7 +8877,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="145" hidden="1">
+    <row r="42" spans="1:20" ht="144" hidden="1">
       <c r="A42" s="20">
         <v>195</v>
       </c>
@@ -8901,7 +8911,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="116" hidden="1">
+    <row r="43" spans="1:20" ht="115.2" hidden="1">
       <c r="A43" s="20">
         <v>204</v>
       </c>
@@ -8935,7 +8945,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="145" hidden="1">
+    <row r="44" spans="1:20" ht="144" hidden="1">
       <c r="A44" s="20">
         <v>211</v>
       </c>
@@ -8969,7 +8979,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="116" hidden="1">
+    <row r="45" spans="1:20" ht="115.2" hidden="1">
       <c r="A45" s="20">
         <v>220</v>
       </c>
@@ -9003,7 +9013,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="145">
+    <row r="46" spans="1:20" ht="144.6" thickBot="1">
       <c r="A46" s="20">
         <v>227</v>
       </c>
@@ -9037,7 +9047,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="116">
+    <row r="47" spans="1:20" ht="115.8" thickBot="1">
       <c r="A47" s="20">
         <v>236</v>
       </c>
@@ -9071,7 +9081,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="145" hidden="1">
+    <row r="48" spans="1:20" ht="144" hidden="1">
       <c r="A48" s="20">
         <v>243</v>
       </c>
@@ -9105,7 +9115,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="116" hidden="1">
+    <row r="49" spans="1:20" ht="115.2" hidden="1">
       <c r="A49" s="20">
         <v>252</v>
       </c>
@@ -9139,7 +9149,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="145" hidden="1">
+    <row r="50" spans="1:20" ht="144" hidden="1">
       <c r="A50" s="20">
         <v>259</v>
       </c>
@@ -9173,7 +9183,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="116" hidden="1">
+    <row r="51" spans="1:20" ht="115.2" hidden="1">
       <c r="A51" s="20">
         <v>268</v>
       </c>
@@ -9207,7 +9217,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="145" hidden="1">
+    <row r="52" spans="1:20" ht="144" hidden="1">
       <c r="A52" s="20">
         <v>275</v>
       </c>
@@ -9241,7 +9251,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="116" hidden="1">
+    <row r="53" spans="1:20" ht="115.2" hidden="1">
       <c r="A53" s="20">
         <v>284</v>
       </c>
@@ -9275,7 +9285,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="145" hidden="1">
+    <row r="54" spans="1:20" ht="144" hidden="1">
       <c r="A54" s="20">
         <v>291</v>
       </c>
@@ -9309,7 +9319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="116" hidden="1">
+    <row r="55" spans="1:20" ht="115.2" hidden="1">
       <c r="A55" s="20">
         <v>300</v>
       </c>
@@ -9343,7 +9353,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="145" hidden="1">
+    <row r="56" spans="1:20" ht="144" hidden="1">
       <c r="A56" s="20">
         <v>307</v>
       </c>
@@ -9377,7 +9387,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="116" hidden="1">
+    <row r="57" spans="1:20" ht="115.2" hidden="1">
       <c r="A57" s="20">
         <v>316</v>
       </c>
@@ -9411,7 +9421,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="232" hidden="1">
+    <row r="58" spans="1:20" ht="230.4" hidden="1">
       <c r="A58" s="20">
         <v>196</v>
       </c>
@@ -9445,7 +9455,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="217.5" hidden="1">
+    <row r="59" spans="1:20" ht="216" hidden="1">
       <c r="A59" s="20">
         <v>207</v>
       </c>
@@ -9479,7 +9489,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="232" hidden="1">
+    <row r="60" spans="1:20" ht="230.4" hidden="1">
       <c r="A60" s="20">
         <v>212</v>
       </c>
@@ -9513,7 +9523,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="217.5" hidden="1">
+    <row r="61" spans="1:20" ht="216" hidden="1">
       <c r="A61" s="20">
         <v>223</v>
       </c>
@@ -9547,7 +9557,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="232">
+    <row r="62" spans="1:20" ht="231" thickBot="1">
       <c r="A62" s="20">
         <v>228</v>
       </c>
@@ -9581,7 +9591,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="217.5">
+    <row r="63" spans="1:20" ht="216.6" thickBot="1">
       <c r="A63" s="20">
         <v>239</v>
       </c>
@@ -9615,7 +9625,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="261" hidden="1">
+    <row r="64" spans="1:20" ht="259.2" hidden="1">
       <c r="A64" s="20">
         <v>244</v>
       </c>
@@ -9649,7 +9659,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="232" hidden="1">
+    <row r="65" spans="1:20" ht="230.4" hidden="1">
       <c r="A65" s="20">
         <v>255</v>
       </c>
@@ -9683,7 +9693,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="261" hidden="1">
+    <row r="66" spans="1:20" ht="259.2" hidden="1">
       <c r="A66" s="20">
         <v>260</v>
       </c>
@@ -9717,7 +9727,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="232" hidden="1">
+    <row r="67" spans="1:20" ht="230.4" hidden="1">
       <c r="A67" s="20">
         <v>271</v>
       </c>
@@ -9751,7 +9761,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="232" hidden="1">
+    <row r="68" spans="1:20" ht="230.4" hidden="1">
       <c r="A68" s="20">
         <v>276</v>
       </c>
@@ -9785,7 +9795,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="217.5" hidden="1">
+    <row r="69" spans="1:20" ht="216" hidden="1">
       <c r="A69" s="20">
         <v>287</v>
       </c>
@@ -9819,7 +9829,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="232" hidden="1">
+    <row r="70" spans="1:20" ht="230.4" hidden="1">
       <c r="A70" s="20">
         <v>292</v>
       </c>
@@ -9853,7 +9863,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="217.5" hidden="1">
+    <row r="71" spans="1:20" ht="216" hidden="1">
       <c r="A71" s="20">
         <v>303</v>
       </c>
@@ -9887,7 +9897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="232" hidden="1">
+    <row r="72" spans="1:20" ht="230.4" hidden="1">
       <c r="A72" s="20">
         <v>308</v>
       </c>
@@ -9921,7 +9931,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="217.5" hidden="1">
+    <row r="73" spans="1:20" ht="216" hidden="1">
       <c r="A73" s="20">
         <v>319</v>
       </c>
@@ -9955,7 +9965,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="159.5" hidden="1">
+    <row r="74" spans="1:20" ht="158.4" hidden="1">
       <c r="A74" s="20">
         <v>192</v>
       </c>
@@ -9989,7 +9999,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="174" hidden="1">
+    <row r="75" spans="1:20" ht="172.8" hidden="1">
       <c r="A75" s="20">
         <v>197</v>
       </c>
@@ -10023,7 +10033,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="188.5" hidden="1">
+    <row r="76" spans="1:20" ht="172.8" hidden="1">
       <c r="A76" s="20">
         <v>198</v>
       </c>
@@ -10057,7 +10067,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="203" hidden="1">
+    <row r="77" spans="1:20" ht="201.6" hidden="1">
       <c r="A77" s="20">
         <v>199</v>
       </c>
@@ -10091,7 +10101,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="188.5" hidden="1">
+    <row r="78" spans="1:20" ht="187.2" hidden="1">
       <c r="A78" s="20">
         <v>200</v>
       </c>
@@ -10125,7 +10135,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="188.5" hidden="1">
+    <row r="79" spans="1:20" ht="187.2" hidden="1">
       <c r="A79" s="20">
         <v>201</v>
       </c>
@@ -10159,7 +10169,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="188.5" hidden="1">
+    <row r="80" spans="1:20" ht="187.2" hidden="1">
       <c r="A80" s="20">
         <v>202</v>
       </c>
@@ -10193,7 +10203,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="203" hidden="1">
+    <row r="81" spans="1:20" ht="201.6" hidden="1">
       <c r="A81" s="20">
         <v>203</v>
       </c>
@@ -10227,7 +10237,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="159.5" hidden="1">
+    <row r="82" spans="1:20" ht="158.4" hidden="1">
       <c r="A82" s="20">
         <v>208</v>
       </c>
@@ -10261,7 +10271,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="174" hidden="1">
+    <row r="83" spans="1:20" ht="172.8" hidden="1">
       <c r="A83" s="20">
         <v>213</v>
       </c>
@@ -10295,7 +10305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="188.5" hidden="1">
+    <row r="84" spans="1:20" ht="172.8" hidden="1">
       <c r="A84" s="20">
         <v>214</v>
       </c>
@@ -10329,7 +10339,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="203" hidden="1">
+    <row r="85" spans="1:20" ht="201.6" hidden="1">
       <c r="A85" s="20">
         <v>215</v>
       </c>
@@ -10363,7 +10373,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="188.5" hidden="1">
+    <row r="86" spans="1:20" ht="187.2" hidden="1">
       <c r="A86" s="20">
         <v>216</v>
       </c>
@@ -10397,7 +10407,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="188.5" hidden="1">
+    <row r="87" spans="1:20" ht="187.2" hidden="1">
       <c r="A87" s="20">
         <v>217</v>
       </c>
@@ -10431,7 +10441,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="188.5" hidden="1">
+    <row r="88" spans="1:20" ht="187.2" hidden="1">
       <c r="A88" s="20">
         <v>218</v>
       </c>
@@ -10465,7 +10475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="203" hidden="1">
+    <row r="89" spans="1:20" ht="201.6" hidden="1">
       <c r="A89" s="20">
         <v>219</v>
       </c>
@@ -10499,7 +10509,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="159.5">
+    <row r="90" spans="1:20" ht="159" thickBot="1">
       <c r="A90" s="20">
         <v>224</v>
       </c>
@@ -10533,7 +10543,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="174">
+    <row r="91" spans="1:20" ht="173.4" thickBot="1">
       <c r="A91" s="20">
         <v>229</v>
       </c>
@@ -10567,7 +10577,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="188.5">
+    <row r="92" spans="1:20" ht="172.8">
       <c r="A92" s="20">
         <v>230</v>
       </c>
@@ -10601,7 +10611,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="203">
+    <row r="93" spans="1:20" ht="201.6">
       <c r="A93" s="20">
         <v>231</v>
       </c>
@@ -10635,7 +10645,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="188.5">
+    <row r="94" spans="1:20" ht="187.2">
       <c r="A94" s="20">
         <v>232</v>
       </c>
@@ -10669,7 +10679,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="188.5">
+    <row r="95" spans="1:20" ht="187.2">
       <c r="A95" s="20">
         <v>233</v>
       </c>
@@ -10703,7 +10713,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="188.5">
+    <row r="96" spans="1:20" ht="187.2">
       <c r="A96" s="20">
         <v>234</v>
       </c>
@@ -10737,7 +10747,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="203">
+    <row r="97" spans="1:20" ht="202.2" thickBot="1">
       <c r="A97" s="20">
         <v>235</v>
       </c>
@@ -10771,7 +10781,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="174" hidden="1">
+    <row r="98" spans="1:20" ht="172.8" hidden="1">
       <c r="A98" s="20">
         <v>240</v>
       </c>
@@ -10805,7 +10815,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="188.5" hidden="1">
+    <row r="99" spans="1:20" ht="187.2" hidden="1">
       <c r="A99" s="20">
         <v>245</v>
       </c>
@@ -10839,7 +10849,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="203" hidden="1">
+    <row r="100" spans="1:20" ht="187.2" hidden="1">
       <c r="A100" s="20">
         <v>246</v>
       </c>
@@ -10873,7 +10883,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="217.5" hidden="1">
+    <row r="101" spans="1:20" ht="216" hidden="1">
       <c r="A101" s="20">
         <v>247</v>
       </c>
@@ -10907,7 +10917,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="203" hidden="1">
+    <row r="102" spans="1:20" ht="201.6" hidden="1">
       <c r="A102" s="20">
         <v>248</v>
       </c>
@@ -10941,7 +10951,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="203" hidden="1">
+    <row r="103" spans="1:20" ht="201.6" hidden="1">
       <c r="A103" s="20">
         <v>249</v>
       </c>
@@ -10975,7 +10985,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="203" hidden="1">
+    <row r="104" spans="1:20" ht="201.6" hidden="1">
       <c r="A104" s="20">
         <v>250</v>
       </c>
@@ -11009,7 +11019,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="217.5" hidden="1">
+    <row r="105" spans="1:20" ht="216" hidden="1">
       <c r="A105" s="20">
         <v>251</v>
       </c>
@@ -11043,7 +11053,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="174" hidden="1">
+    <row r="106" spans="1:20" ht="172.8" hidden="1">
       <c r="A106" s="20">
         <v>256</v>
       </c>
@@ -11077,7 +11087,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="188.5" hidden="1">
+    <row r="107" spans="1:20" ht="187.2" hidden="1">
       <c r="A107" s="20">
         <v>261</v>
       </c>
@@ -11111,7 +11121,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="203" hidden="1">
+    <row r="108" spans="1:20" ht="187.2" hidden="1">
       <c r="A108" s="20">
         <v>262</v>
       </c>
@@ -11145,7 +11155,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="217.5" hidden="1">
+    <row r="109" spans="1:20" ht="216" hidden="1">
       <c r="A109" s="20">
         <v>263</v>
       </c>
@@ -11179,7 +11189,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="203" hidden="1">
+    <row r="110" spans="1:20" ht="201.6" hidden="1">
       <c r="A110" s="20">
         <v>264</v>
       </c>
@@ -11213,7 +11223,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="203" hidden="1">
+    <row r="111" spans="1:20" ht="201.6" hidden="1">
       <c r="A111" s="20">
         <v>265</v>
       </c>
@@ -11247,7 +11257,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="203" hidden="1">
+    <row r="112" spans="1:20" ht="201.6" hidden="1">
       <c r="A112" s="20">
         <v>266</v>
       </c>
@@ -11281,7 +11291,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="217.5" hidden="1">
+    <row r="113" spans="1:20" ht="216" hidden="1">
       <c r="A113" s="20">
         <v>267</v>
       </c>
@@ -11315,7 +11325,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="159.5" hidden="1">
+    <row r="114" spans="1:20" ht="158.4" hidden="1">
       <c r="A114" s="20">
         <v>272</v>
       </c>
@@ -11349,7 +11359,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="174" hidden="1">
+    <row r="115" spans="1:20" ht="172.8" hidden="1">
       <c r="A115" s="20">
         <v>277</v>
       </c>
@@ -11383,7 +11393,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="188.5" hidden="1">
+    <row r="116" spans="1:20" ht="172.8" hidden="1">
       <c r="A116" s="20">
         <v>278</v>
       </c>
@@ -11417,7 +11427,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="203" hidden="1">
+    <row r="117" spans="1:20" ht="201.6" hidden="1">
       <c r="A117" s="20">
         <v>279</v>
       </c>
@@ -11451,7 +11461,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="188.5" hidden="1">
+    <row r="118" spans="1:20" ht="187.2" hidden="1">
       <c r="A118" s="20">
         <v>280</v>
       </c>
@@ -11485,7 +11495,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="188.5" hidden="1">
+    <row r="119" spans="1:20" ht="187.2" hidden="1">
       <c r="A119" s="20">
         <v>281</v>
       </c>
@@ -11519,7 +11529,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="188.5" hidden="1">
+    <row r="120" spans="1:20" ht="187.2" hidden="1">
       <c r="A120" s="20">
         <v>282</v>
       </c>
@@ -11553,7 +11563,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="203" hidden="1">
+    <row r="121" spans="1:20" ht="201.6" hidden="1">
       <c r="A121" s="20">
         <v>283</v>
       </c>
@@ -11587,7 +11597,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="159.5" hidden="1">
+    <row r="122" spans="1:20" ht="158.4" hidden="1">
       <c r="A122" s="20">
         <v>288</v>
       </c>
@@ -11621,7 +11631,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="174" hidden="1">
+    <row r="123" spans="1:20" ht="172.8" hidden="1">
       <c r="A123" s="20">
         <v>293</v>
       </c>
@@ -11655,7 +11665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="188.5" hidden="1">
+    <row r="124" spans="1:20" ht="172.8" hidden="1">
       <c r="A124" s="20">
         <v>294</v>
       </c>
@@ -11689,7 +11699,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="203" hidden="1">
+    <row r="125" spans="1:20" ht="201.6" hidden="1">
       <c r="A125" s="20">
         <v>295</v>
       </c>
@@ -11723,7 +11733,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="188.5" hidden="1">
+    <row r="126" spans="1:20" ht="187.2" hidden="1">
       <c r="A126" s="20">
         <v>296</v>
       </c>
@@ -11757,7 +11767,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="188.5" hidden="1">
+    <row r="127" spans="1:20" ht="187.2" hidden="1">
       <c r="A127" s="20">
         <v>297</v>
       </c>
@@ -11791,7 +11801,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="188.5" hidden="1">
+    <row r="128" spans="1:20" ht="187.2" hidden="1">
       <c r="A128" s="20">
         <v>298</v>
       </c>
@@ -11825,7 +11835,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="203" hidden="1">
+    <row r="129" spans="1:20" ht="201.6" hidden="1">
       <c r="A129" s="20">
         <v>299</v>
       </c>
@@ -11859,7 +11869,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="159.5" hidden="1">
+    <row r="130" spans="1:20" ht="158.4" hidden="1">
       <c r="A130" s="20">
         <v>304</v>
       </c>
@@ -11893,7 +11903,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="174" hidden="1">
+    <row r="131" spans="1:20" ht="172.8" hidden="1">
       <c r="A131" s="20">
         <v>309</v>
       </c>
@@ -11927,7 +11937,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="188.5" hidden="1">
+    <row r="132" spans="1:20" ht="172.8" hidden="1">
       <c r="A132" s="20">
         <v>310</v>
       </c>
@@ -11961,7 +11971,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="203" hidden="1">
+    <row r="133" spans="1:20" ht="201.6" hidden="1">
       <c r="A133" s="20">
         <v>311</v>
       </c>
@@ -11995,7 +12005,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="188.5" hidden="1">
+    <row r="134" spans="1:20" ht="187.2" hidden="1">
       <c r="A134" s="20">
         <v>312</v>
       </c>
@@ -12029,7 +12039,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="188.5" hidden="1">
+    <row r="135" spans="1:20" ht="187.2" hidden="1">
       <c r="A135" s="20">
         <v>313</v>
       </c>
@@ -12063,7 +12073,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="188.5" hidden="1">
+    <row r="136" spans="1:20" ht="187.2" hidden="1">
       <c r="A136" s="20">
         <v>314</v>
       </c>
@@ -12097,7 +12107,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="203" hidden="1">
+    <row r="137" spans="1:20" ht="201.6" hidden="1">
       <c r="A137" s="20">
         <v>315</v>
       </c>
@@ -12131,7 +12141,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="246.5" hidden="1">
+    <row r="138" spans="1:20" ht="244.8" hidden="1">
       <c r="A138" s="20">
         <v>320</v>
       </c>
@@ -12165,7 +12175,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="217.5" hidden="1">
+    <row r="139" spans="1:20" ht="216" hidden="1">
       <c r="A139" s="20">
         <v>321</v>
       </c>
@@ -12199,7 +12209,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="246.5" hidden="1">
+    <row r="140" spans="1:20" ht="244.8" hidden="1">
       <c r="A140" s="20">
         <v>324</v>
       </c>
@@ -12233,7 +12243,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="203" hidden="1">
+    <row r="141" spans="1:20" ht="201.6" hidden="1">
       <c r="A141" s="20">
         <v>325</v>
       </c>
@@ -12267,7 +12277,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="246.5">
+    <row r="142" spans="1:20" ht="245.4" thickBot="1">
       <c r="A142" s="20">
         <v>328</v>
       </c>
@@ -12301,7 +12311,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="203">
+    <row r="143" spans="1:20" ht="202.2" thickBot="1">
       <c r="A143" s="20">
         <v>329</v>
       </c>
@@ -12335,7 +12345,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="261" hidden="1">
+    <row r="144" spans="1:20" ht="259.2" hidden="1">
       <c r="A144" s="20">
         <v>332</v>
       </c>
@@ -12369,7 +12379,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="217.5" hidden="1">
+    <row r="145" spans="1:20" ht="216" hidden="1">
       <c r="A145" s="20">
         <v>333</v>
       </c>
@@ -12403,7 +12413,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="261" hidden="1">
+    <row r="146" spans="1:20" ht="259.2" hidden="1">
       <c r="A146" s="20">
         <v>336</v>
       </c>
@@ -12437,7 +12447,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="232" hidden="1">
+    <row r="147" spans="1:20" ht="230.4" hidden="1">
       <c r="A147" s="20">
         <v>337</v>
       </c>
@@ -12471,7 +12481,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="246.5" hidden="1">
+    <row r="148" spans="1:20" ht="244.8" hidden="1">
       <c r="A148" s="20">
         <v>340</v>
       </c>
@@ -12505,7 +12515,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="217.5" hidden="1">
+    <row r="149" spans="1:20" ht="216" hidden="1">
       <c r="A149" s="20">
         <v>341</v>
       </c>
@@ -12539,7 +12549,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="246.5" hidden="1">
+    <row r="150" spans="1:20" ht="244.8" hidden="1">
       <c r="A150" s="20">
         <v>344</v>
       </c>
@@ -12573,7 +12583,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="203" hidden="1">
+    <row r="151" spans="1:20" ht="201.6" hidden="1">
       <c r="A151" s="20">
         <v>345</v>
       </c>
@@ -12607,7 +12617,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="246.5" hidden="1">
+    <row r="152" spans="1:20" ht="244.8" hidden="1">
       <c r="A152" s="20">
         <v>348</v>
       </c>
@@ -12641,7 +12651,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="217.5" hidden="1">
+    <row r="153" spans="1:20" ht="216" hidden="1">
       <c r="A153" s="20">
         <v>349</v>
       </c>
@@ -12675,7 +12685,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="246.5" hidden="1">
+    <row r="154" spans="1:20" ht="244.8" hidden="1">
       <c r="A154" s="20">
         <v>193</v>
       </c>
@@ -12709,7 +12719,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="246.5" hidden="1">
+    <row r="155" spans="1:20" ht="244.8" hidden="1">
       <c r="A155" s="20">
         <v>206</v>
       </c>
@@ -12743,7 +12753,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="246.5" hidden="1">
+    <row r="156" spans="1:20" ht="244.8" hidden="1">
       <c r="A156" s="20">
         <v>209</v>
       </c>
@@ -12777,7 +12787,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="232" hidden="1">
+    <row r="157" spans="1:20" ht="230.4" hidden="1">
       <c r="A157" s="20">
         <v>222</v>
       </c>
@@ -12811,7 +12821,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="246.5">
+    <row r="158" spans="1:20" ht="245.4" thickBot="1">
       <c r="A158" s="20">
         <v>225</v>
       </c>
@@ -12845,7 +12855,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="232">
+    <row r="159" spans="1:20" ht="231" thickBot="1">
       <c r="A159" s="20">
         <v>238</v>
       </c>
@@ -12879,7 +12889,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="261" hidden="1">
+    <row r="160" spans="1:20" ht="259.2" hidden="1">
       <c r="A160" s="20">
         <v>241</v>
       </c>
@@ -12913,7 +12923,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="246.5" hidden="1">
+    <row r="161" spans="1:20" ht="244.8" hidden="1">
       <c r="A161" s="20">
         <v>254</v>
       </c>
@@ -12947,7 +12957,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="261" hidden="1">
+    <row r="162" spans="1:20" ht="259.2" hidden="1">
       <c r="A162" s="20">
         <v>257</v>
       </c>
@@ -12981,7 +12991,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="246.5" hidden="1">
+    <row r="163" spans="1:20" ht="244.8" hidden="1">
       <c r="A163" s="20">
         <v>270</v>
       </c>
@@ -13015,7 +13025,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="246.5" hidden="1">
+    <row r="164" spans="1:20" ht="244.8" hidden="1">
       <c r="A164" s="20">
         <v>273</v>
       </c>
@@ -13049,7 +13059,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="232" hidden="1">
+    <row r="165" spans="1:20" ht="230.4" hidden="1">
       <c r="A165" s="20">
         <v>286</v>
       </c>
@@ -13083,7 +13093,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="246.5" hidden="1">
+    <row r="166" spans="1:20" ht="244.8" hidden="1">
       <c r="A166" s="20">
         <v>289</v>
       </c>
@@ -13117,7 +13127,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="232" hidden="1">
+    <row r="167" spans="1:20" ht="230.4" hidden="1">
       <c r="A167" s="20">
         <v>302</v>
       </c>
@@ -13151,7 +13161,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="246.5" hidden="1">
+    <row r="168" spans="1:20" ht="244.8" hidden="1">
       <c r="A168" s="20">
         <v>305</v>
       </c>
@@ -13185,7 +13195,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="232" hidden="1">
+    <row r="169" spans="1:20" ht="230.4" hidden="1">
       <c r="A169" s="20">
         <v>318</v>
       </c>
@@ -13219,7 +13229,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="188.5" hidden="1">
+    <row r="170" spans="1:20" ht="187.2" hidden="1">
       <c r="A170" s="20">
         <v>322</v>
       </c>
@@ -13253,7 +13263,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="217.5" hidden="1">
+    <row r="171" spans="1:20" ht="216" hidden="1">
       <c r="A171" s="20">
         <v>323</v>
       </c>
@@ -13287,7 +13297,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="188.5" hidden="1">
+    <row r="172" spans="1:20" ht="187.2" hidden="1">
       <c r="A172" s="20">
         <v>326</v>
       </c>
@@ -13321,7 +13331,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="217.5" hidden="1">
+    <row r="173" spans="1:20" ht="216" hidden="1">
       <c r="A173" s="20">
         <v>327</v>
       </c>
@@ -13355,7 +13365,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="188.5">
+    <row r="174" spans="1:20" ht="187.8" thickBot="1">
       <c r="A174" s="20">
         <v>330</v>
       </c>
@@ -13389,7 +13399,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="217.5">
+    <row r="175" spans="1:20" ht="216.6" thickBot="1">
       <c r="A175" s="20">
         <v>331</v>
       </c>
@@ -13423,7 +13433,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="188.5" hidden="1">
+    <row r="176" spans="1:20" ht="187.2" hidden="1">
       <c r="A176" s="20">
         <v>334</v>
       </c>
@@ -13457,7 +13467,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="232" hidden="1">
+    <row r="177" spans="1:20" ht="230.4" hidden="1">
       <c r="A177" s="20">
         <v>335</v>
       </c>
@@ -13491,7 +13501,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="203" hidden="1">
+    <row r="178" spans="1:20" ht="201.6" hidden="1">
       <c r="A178" s="20">
         <v>338</v>
       </c>
@@ -13525,7 +13535,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="232" hidden="1">
+    <row r="179" spans="1:20" ht="230.4" hidden="1">
       <c r="A179" s="20">
         <v>339</v>
       </c>
@@ -13559,7 +13569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="188.5" hidden="1">
+    <row r="180" spans="1:20" ht="187.2" hidden="1">
       <c r="A180" s="20">
         <v>342</v>
       </c>
@@ -13593,7 +13603,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="217.5" hidden="1">
+    <row r="181" spans="1:20" ht="216" hidden="1">
       <c r="A181" s="20">
         <v>343</v>
       </c>
@@ -13627,7 +13637,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="174" hidden="1">
+    <row r="182" spans="1:20" ht="172.8" hidden="1">
       <c r="A182" s="20">
         <v>346</v>
       </c>
@@ -13661,7 +13671,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="217.5" hidden="1">
+    <row r="183" spans="1:20" ht="216" hidden="1">
       <c r="A183" s="20">
         <v>347</v>
       </c>
@@ -13695,7 +13705,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="188.5" hidden="1">
+    <row r="184" spans="1:20" ht="187.2" hidden="1">
       <c r="A184" s="20">
         <v>350</v>
       </c>
@@ -13729,7 +13739,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="217.5" hidden="1">
+    <row r="185" spans="1:20" ht="216" hidden="1">
       <c r="A185" s="20">
         <v>351</v>
       </c>
@@ -13763,7 +13773,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="145" hidden="1">
+    <row r="186" spans="1:20" ht="144" hidden="1">
       <c r="A186" s="20">
         <v>1</v>
       </c>
@@ -13797,7 +13807,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="145" hidden="1">
+    <row r="187" spans="1:20" ht="144" hidden="1">
       <c r="A187" s="20">
         <v>2</v>
       </c>
@@ -13831,7 +13841,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="145" hidden="1">
+    <row r="188" spans="1:20" ht="144" hidden="1">
       <c r="A188" s="20">
         <v>3</v>
       </c>
@@ -13865,7 +13875,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="145" hidden="1">
+    <row r="189" spans="1:20" ht="144" hidden="1">
       <c r="A189" s="20">
         <v>4</v>
       </c>
@@ -13899,7 +13909,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="145" hidden="1">
+    <row r="190" spans="1:20" ht="144" hidden="1">
       <c r="A190" s="20">
         <v>5</v>
       </c>
@@ -13933,7 +13943,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="130.5" hidden="1">
+    <row r="191" spans="1:20" ht="129.6" hidden="1">
       <c r="A191" s="20">
         <v>6</v>
       </c>
@@ -13967,7 +13977,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="130.5" hidden="1">
+    <row r="192" spans="1:20" ht="129.6" hidden="1">
       <c r="A192" s="20">
         <v>7</v>
       </c>
@@ -14001,7 +14011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="130.5" hidden="1">
+    <row r="193" spans="1:20" ht="129.6" hidden="1">
       <c r="A193" s="20">
         <v>8</v>
       </c>
@@ -14035,7 +14045,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="130.5" hidden="1">
+    <row r="194" spans="1:20" ht="129.6" hidden="1">
       <c r="A194" s="20">
         <v>9</v>
       </c>
@@ -14069,7 +14079,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="130.5">
+    <row r="195" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A195" s="20">
         <v>11</v>
       </c>
@@ -14086,16 +14096,16 @@
         <v>424</v>
       </c>
       <c r="F195" s="33">
-        <v>45063</v>
+        <v>45085</v>
       </c>
       <c r="G195" s="34" t="s">
-        <v>834</v>
+        <v>861</v>
       </c>
       <c r="H195" s="34" t="s">
-        <v>835</v>
+        <v>862</v>
       </c>
       <c r="I195" s="34" t="s">
-        <v>836</v>
+        <v>863</v>
       </c>
       <c r="J195" s="35" t="s">
         <v>489</v>
@@ -14115,7 +14125,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="130.5">
+    <row r="196" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A196" s="20">
         <v>12</v>
       </c>
@@ -14139,7 +14149,7 @@
         <v>829</v>
       </c>
       <c r="K196" s="35" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="L196" s="35"/>
       <c r="M196" s="35"/>
@@ -14153,7 +14163,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="130.5">
+    <row r="197" spans="1:20" ht="129.6">
       <c r="A197" s="20">
         <v>13</v>
       </c>
@@ -14177,7 +14187,7 @@
         <v>829</v>
       </c>
       <c r="K197" s="35" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="L197" s="35"/>
       <c r="M197" s="35"/>
@@ -14191,7 +14201,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="130.5">
+    <row r="198" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A198" s="20">
         <v>14</v>
       </c>
@@ -14215,7 +14225,7 @@
         <v>829</v>
       </c>
       <c r="K198" s="35" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="L198" s="35"/>
       <c r="M198" s="35"/>
@@ -14229,7 +14239,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="130.5" hidden="1">
+    <row r="199" spans="1:20" ht="129.6" hidden="1">
       <c r="A199" s="20">
         <v>16</v>
       </c>
@@ -14263,7 +14273,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="130.5" hidden="1">
+    <row r="200" spans="1:20" ht="129.6" hidden="1">
       <c r="A200" s="20">
         <v>17</v>
       </c>
@@ -14297,7 +14307,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="130.5" hidden="1">
+    <row r="201" spans="1:20" ht="129.6" hidden="1">
       <c r="A201" s="20">
         <v>18</v>
       </c>
@@ -14331,7 +14341,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="130.5" hidden="1">
+    <row r="202" spans="1:20" ht="129.6" hidden="1">
       <c r="A202" s="20">
         <v>19</v>
       </c>
@@ -14365,7 +14375,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="130.5" hidden="1">
+    <row r="203" spans="1:20" ht="129.6" hidden="1">
       <c r="A203" s="20">
         <v>20</v>
       </c>
@@ -14399,7 +14409,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="130.5" hidden="1">
+    <row r="204" spans="1:20" ht="129.6" hidden="1">
       <c r="A204" s="20">
         <v>21</v>
       </c>
@@ -14433,7 +14443,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="130.5" hidden="1">
+    <row r="205" spans="1:20" ht="129.6" hidden="1">
       <c r="A205" s="20">
         <v>22</v>
       </c>
@@ -14467,7 +14477,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="130.5" hidden="1">
+    <row r="206" spans="1:20" ht="129.6" hidden="1">
       <c r="A206" s="20">
         <v>23</v>
       </c>
@@ -14501,7 +14511,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="130.5" hidden="1">
+    <row r="207" spans="1:20" ht="129.6" hidden="1">
       <c r="A207" s="20">
         <v>24</v>
       </c>
@@ -14535,7 +14545,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="130.5" hidden="1">
+    <row r="208" spans="1:20" ht="129.6" hidden="1">
       <c r="A208" s="20">
         <v>25</v>
       </c>
@@ -14569,7 +14579,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="130.5" hidden="1">
+    <row r="209" spans="1:20" ht="129.6" hidden="1">
       <c r="A209" s="20">
         <v>26</v>
       </c>
@@ -14603,7 +14613,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="130.5" hidden="1">
+    <row r="210" spans="1:20" ht="129.6" hidden="1">
       <c r="A210" s="20">
         <v>27</v>
       </c>
@@ -14637,7 +14647,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="145" hidden="1">
+    <row r="211" spans="1:20" ht="129.6" hidden="1">
       <c r="A211" s="20">
         <v>28</v>
       </c>
@@ -14671,7 +14681,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="145" hidden="1">
+    <row r="212" spans="1:20" ht="129.6" hidden="1">
       <c r="A212" s="20">
         <v>29</v>
       </c>
@@ -14705,7 +14715,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="145" hidden="1">
+    <row r="213" spans="1:20" ht="129.6" hidden="1">
       <c r="A213" s="20">
         <v>30</v>
       </c>
@@ -14739,7 +14749,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="145">
+    <row r="214" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A214" s="20">
         <v>31</v>
       </c>
@@ -14759,13 +14769,13 @@
         <v>45063</v>
       </c>
       <c r="G214" s="34" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="H214" s="34" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="I214" s="34" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="J214" s="35" t="s">
         <v>489</v>
@@ -14775,29 +14785,29 @@
         <v>829</v>
       </c>
       <c r="M214" s="35" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="N214" s="35" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="O214" s="35" t="s">
         <v>489</v>
       </c>
       <c r="P214" s="35" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="Q214" s="35" t="s">
         <v>827</v>
       </c>
       <c r="R214" s="36"/>
       <c r="S214" s="37" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="T214" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="145" hidden="1">
+    <row r="215" spans="1:20" ht="129.6" hidden="1">
       <c r="A215" s="20">
         <v>32</v>
       </c>
@@ -14831,7 +14841,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="145" hidden="1">
+    <row r="216" spans="1:20" ht="129.6" hidden="1">
       <c r="A216" s="20">
         <v>33</v>
       </c>
@@ -14865,7 +14875,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="145" hidden="1">
+    <row r="217" spans="1:20" ht="129.6" hidden="1">
       <c r="A217" s="20">
         <v>34</v>
       </c>
@@ -14899,7 +14909,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="145" hidden="1">
+    <row r="218" spans="1:20" ht="129.6" hidden="1">
       <c r="A218" s="20">
         <v>35</v>
       </c>
@@ -14933,7 +14943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="145" hidden="1">
+    <row r="219" spans="1:20" ht="144" hidden="1">
       <c r="A219" s="20">
         <v>36</v>
       </c>
@@ -14967,7 +14977,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="145" hidden="1">
+    <row r="220" spans="1:20" ht="144" hidden="1">
       <c r="A220" s="20">
         <v>37</v>
       </c>
@@ -15001,7 +15011,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="145" hidden="1">
+    <row r="221" spans="1:20" ht="144" hidden="1">
       <c r="A221" s="20">
         <v>38</v>
       </c>
@@ -15035,7 +15045,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="145">
+    <row r="222" spans="1:20" ht="144.6" thickBot="1">
       <c r="A222" s="20">
         <v>39</v>
       </c>
@@ -15059,7 +15069,7 @@
         <v>829</v>
       </c>
       <c r="K222" s="35" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="L222" s="35"/>
       <c r="M222" s="35"/>
@@ -15073,7 +15083,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="145" hidden="1">
+    <row r="223" spans="1:20" ht="144" hidden="1">
       <c r="A223" s="20">
         <v>40</v>
       </c>
@@ -15107,7 +15117,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="145" hidden="1">
+    <row r="224" spans="1:20" ht="144" hidden="1">
       <c r="A224" s="20">
         <v>41</v>
       </c>
@@ -15141,7 +15151,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="145" hidden="1">
+    <row r="225" spans="1:20" ht="144" hidden="1">
       <c r="A225" s="20">
         <v>42</v>
       </c>
@@ -15175,7 +15185,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="145" hidden="1">
+    <row r="226" spans="1:20" ht="144" hidden="1">
       <c r="A226" s="20">
         <v>43</v>
       </c>
@@ -15209,7 +15219,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="43.5" hidden="1">
+    <row r="227" spans="1:20" ht="43.2" hidden="1">
       <c r="A227" s="20">
         <v>44</v>
       </c>
@@ -15245,7 +15255,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="43.5" hidden="1">
+    <row r="228" spans="1:20" ht="43.2" hidden="1">
       <c r="A228" s="20">
         <v>45</v>
       </c>
@@ -15281,7 +15291,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="43.5" hidden="1">
+    <row r="229" spans="1:20" ht="43.2" hidden="1">
       <c r="A229" s="20">
         <v>46</v>
       </c>
@@ -15317,7 +15327,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="319">
+    <row r="230" spans="1:20" ht="303" thickBot="1">
       <c r="A230" s="20">
         <v>47</v>
       </c>
@@ -15337,7 +15347,7 @@
         <v>45063</v>
       </c>
       <c r="G230" s="34" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="H230" s="34"/>
       <c r="I230" s="34"/>
@@ -15352,7 +15362,7 @@
         <v>829</v>
       </c>
       <c r="P230" s="35" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="Q230" s="35" t="s">
         <v>827</v>
@@ -15363,7 +15373,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="43.5" hidden="1">
+    <row r="231" spans="1:20" ht="43.2" hidden="1">
       <c r="A231" s="20">
         <v>48</v>
       </c>
@@ -15399,7 +15409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="43.5" hidden="1">
+    <row r="232" spans="1:20" ht="43.2" hidden="1">
       <c r="A232" s="20">
         <v>49</v>
       </c>
@@ -15435,7 +15445,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="43.5" hidden="1">
+    <row r="233" spans="1:20" ht="43.2" hidden="1">
       <c r="A233" s="20">
         <v>50</v>
       </c>
@@ -15471,7 +15481,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="43.5" hidden="1">
+    <row r="234" spans="1:20" ht="43.2" hidden="1">
       <c r="A234" s="20">
         <v>51</v>
       </c>
@@ -15507,7 +15517,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="116" hidden="1">
+    <row r="235" spans="1:20" ht="115.2" hidden="1">
       <c r="A235" s="20">
         <v>52</v>
       </c>
@@ -15541,7 +15551,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="116" hidden="1">
+    <row r="236" spans="1:20" ht="115.2" hidden="1">
       <c r="A236" s="20">
         <v>53</v>
       </c>
@@ -15575,7 +15585,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="116" hidden="1">
+    <row r="237" spans="1:20" ht="115.2" hidden="1">
       <c r="A237" s="20">
         <v>54</v>
       </c>
@@ -15609,7 +15619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="116" hidden="1">
+    <row r="238" spans="1:20" ht="115.2" hidden="1">
       <c r="A238" s="20">
         <v>55</v>
       </c>
@@ -15643,7 +15653,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="116" hidden="1">
+    <row r="239" spans="1:20" ht="115.2" hidden="1">
       <c r="A239" s="20">
         <v>56</v>
       </c>
@@ -15677,7 +15687,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="116" hidden="1">
+    <row r="240" spans="1:20" ht="115.2" hidden="1">
       <c r="A240" s="20">
         <v>57</v>
       </c>
@@ -15711,7 +15721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="116" hidden="1">
+    <row r="241" spans="1:20" ht="115.2" hidden="1">
       <c r="A241" s="20">
         <v>58</v>
       </c>
@@ -15745,7 +15755,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="116" hidden="1">
+    <row r="242" spans="1:20" ht="115.2" hidden="1">
       <c r="A242" s="20">
         <v>59</v>
       </c>
@@ -15779,7 +15789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="116" hidden="1">
+    <row r="243" spans="1:20" ht="115.2" hidden="1">
       <c r="A243" s="20">
         <v>60</v>
       </c>
@@ -15813,7 +15823,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="116" hidden="1">
+    <row r="244" spans="1:20" ht="115.2" hidden="1">
       <c r="A244" s="20">
         <v>61</v>
       </c>
@@ -15847,7 +15857,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="116" hidden="1">
+    <row r="245" spans="1:20" ht="115.2" hidden="1">
       <c r="A245" s="20">
         <v>62</v>
       </c>
@@ -15881,7 +15891,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="116" hidden="1">
+    <row r="246" spans="1:20" ht="115.2" hidden="1">
       <c r="A246" s="20">
         <v>63</v>
       </c>
@@ -15915,7 +15925,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="116" hidden="1">
+    <row r="247" spans="1:20" ht="115.2" hidden="1">
       <c r="A247" s="20">
         <v>64</v>
       </c>
@@ -15949,7 +15959,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="116" hidden="1">
+    <row r="248" spans="1:20" ht="115.2" hidden="1">
       <c r="A248" s="20">
         <v>65</v>
       </c>
@@ -15983,7 +15993,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="116" hidden="1">
+    <row r="249" spans="1:20" ht="115.2" hidden="1">
       <c r="A249" s="20">
         <v>66</v>
       </c>
@@ -16017,7 +16027,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="116" hidden="1">
+    <row r="250" spans="1:20" ht="115.2" hidden="1">
       <c r="A250" s="20">
         <v>67</v>
       </c>
@@ -16051,7 +16061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="116" hidden="1">
+    <row r="251" spans="1:20" ht="115.2" hidden="1">
       <c r="A251" s="20">
         <v>68</v>
       </c>
@@ -16085,7 +16095,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="116" hidden="1">
+    <row r="252" spans="1:20" ht="115.2" hidden="1">
       <c r="A252" s="20">
         <v>69</v>
       </c>
@@ -16119,7 +16129,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="116" hidden="1">
+    <row r="253" spans="1:20" ht="115.2" hidden="1">
       <c r="A253" s="20">
         <v>70</v>
       </c>
@@ -16153,7 +16163,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="116" hidden="1">
+    <row r="254" spans="1:20" ht="115.2" hidden="1">
       <c r="A254" s="20">
         <v>71</v>
       </c>
@@ -16187,7 +16197,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="116" hidden="1">
+    <row r="255" spans="1:20" ht="115.2" hidden="1">
       <c r="A255" s="20">
         <v>72</v>
       </c>
@@ -16221,7 +16231,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="116" hidden="1">
+    <row r="256" spans="1:20" ht="115.2" hidden="1">
       <c r="A256" s="20">
         <v>73</v>
       </c>
@@ -16255,7 +16265,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="116" hidden="1">
+    <row r="257" spans="1:20" ht="115.2" hidden="1">
       <c r="A257" s="20">
         <v>74</v>
       </c>
@@ -16289,7 +16299,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="130.5">
+    <row r="258" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A258" s="20">
         <v>75</v>
       </c>
@@ -16313,7 +16323,7 @@
         <v>829</v>
       </c>
       <c r="K258" s="35" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="L258" s="35"/>
       <c r="M258" s="35"/>
@@ -16327,7 +16337,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="116">
+    <row r="259" spans="1:20" ht="115.8" thickBot="1">
       <c r="A259" s="20">
         <v>76</v>
       </c>
@@ -16344,16 +16354,16 @@
         <v>546</v>
       </c>
       <c r="F259" s="33">
-        <v>45063</v>
+        <v>45085</v>
       </c>
       <c r="G259" s="34" t="s">
-        <v>851</v>
+        <v>864</v>
       </c>
       <c r="H259" s="34" t="s">
-        <v>852</v>
+        <v>865</v>
       </c>
       <c r="I259" s="34" t="s">
-        <v>853</v>
+        <v>866</v>
       </c>
       <c r="J259" s="35" t="s">
         <v>489</v>
@@ -16363,29 +16373,29 @@
         <v>829</v>
       </c>
       <c r="M259" s="35" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="N259" s="35" t="s">
-        <v>854</v>
+        <v>867</v>
       </c>
       <c r="O259" s="35" t="s">
         <v>489</v>
       </c>
       <c r="P259" s="35" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="Q259" s="35" t="s">
         <v>827</v>
       </c>
       <c r="R259" s="36"/>
       <c r="S259" s="37" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="T259" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="101.5">
+    <row r="260" spans="1:20" ht="101.4" thickBot="1">
       <c r="A260" s="20">
         <v>77</v>
       </c>
@@ -16409,7 +16419,7 @@
         <v>829</v>
       </c>
       <c r="K260" s="35" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="L260" s="35"/>
       <c r="M260" s="35"/>
@@ -16423,7 +16433,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="101.5">
+    <row r="261" spans="1:20" ht="100.8">
       <c r="A261" s="20">
         <v>78</v>
       </c>
@@ -16447,7 +16457,7 @@
         <v>829</v>
       </c>
       <c r="K261" s="35" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="L261" s="35"/>
       <c r="M261" s="35"/>
@@ -16461,7 +16471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="116">
+    <row r="262" spans="1:20" ht="115.2">
       <c r="A262" s="20">
         <v>79</v>
       </c>
@@ -16485,7 +16495,7 @@
         <v>829</v>
       </c>
       <c r="K262" s="35" t="s">
-        <v>878</v>
+        <v>859</v>
       </c>
       <c r="L262" s="35"/>
       <c r="M262" s="35"/>
@@ -16499,7 +16509,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="116">
+    <row r="263" spans="1:20" ht="115.2">
       <c r="A263" s="20">
         <v>80</v>
       </c>
@@ -16516,16 +16526,16 @@
         <v>554</v>
       </c>
       <c r="F263" s="33">
-        <v>45063</v>
+        <v>45085</v>
       </c>
       <c r="G263" s="34" t="s">
-        <v>858</v>
+        <v>868</v>
       </c>
       <c r="H263" s="34" t="s">
-        <v>859</v>
+        <v>869</v>
       </c>
       <c r="I263" s="34" t="s">
-        <v>860</v>
+        <v>870</v>
       </c>
       <c r="J263" s="35" t="s">
         <v>489</v>
@@ -16535,29 +16545,29 @@
         <v>829</v>
       </c>
       <c r="M263" s="35" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="N263" s="35" t="s">
-        <v>861</v>
+        <v>871</v>
       </c>
       <c r="O263" s="35" t="s">
         <v>489</v>
       </c>
       <c r="P263" s="35" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="Q263" s="35" t="s">
         <v>827</v>
       </c>
       <c r="R263" s="36"/>
       <c r="S263" s="37" t="s">
-        <v>862</v>
+        <v>851</v>
       </c>
       <c r="T263" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="116">
+    <row r="264" spans="1:20" ht="115.8" thickBot="1">
       <c r="A264" s="20">
         <v>81</v>
       </c>
@@ -16581,7 +16591,7 @@
         <v>829</v>
       </c>
       <c r="K264" s="35" t="s">
-        <v>863</v>
+        <v>852</v>
       </c>
       <c r="L264" s="35"/>
       <c r="M264" s="35"/>
@@ -16595,7 +16605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="130.5">
+    <row r="265" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A265" s="20">
         <v>82</v>
       </c>
@@ -16612,16 +16622,16 @@
         <v>558</v>
       </c>
       <c r="F265" s="33">
-        <v>45064</v>
+        <v>45085</v>
       </c>
       <c r="G265" s="34" t="s">
-        <v>864</v>
+        <v>872</v>
       </c>
       <c r="H265" s="38" t="s">
-        <v>865</v>
+        <v>873</v>
       </c>
       <c r="I265" s="34" t="s">
-        <v>866</v>
+        <v>874</v>
       </c>
       <c r="J265" s="35" t="s">
         <v>489</v>
@@ -16631,29 +16641,29 @@
         <v>829</v>
       </c>
       <c r="M265" s="35" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="N265" s="35" t="s">
-        <v>867</v>
+        <v>875</v>
       </c>
       <c r="O265" s="35" t="s">
         <v>489</v>
       </c>
       <c r="P265" s="35" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="Q265" s="35" t="s">
         <v>827</v>
       </c>
       <c r="R265" s="36"/>
       <c r="S265" s="37" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="T265" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="101.5">
+    <row r="266" spans="1:20" ht="101.4" thickBot="1">
       <c r="A266" s="20">
         <v>83</v>
       </c>
@@ -16677,7 +16687,7 @@
         <v>829</v>
       </c>
       <c r="K266" s="35" t="s">
-        <v>879</v>
+        <v>860</v>
       </c>
       <c r="L266" s="35"/>
       <c r="M266" s="35"/>
@@ -16691,7 +16701,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="116">
+    <row r="267" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A267" s="20">
         <v>84</v>
       </c>
@@ -16708,16 +16718,16 @@
         <v>562</v>
       </c>
       <c r="F267" s="33">
-        <v>45064</v>
+        <v>45085</v>
       </c>
       <c r="G267" s="34" t="s">
-        <v>868</v>
+        <v>876</v>
       </c>
       <c r="H267" s="34" t="s">
-        <v>869</v>
+        <v>877</v>
       </c>
       <c r="I267" s="34" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="J267" s="35" t="s">
         <v>489</v>
@@ -16727,16 +16737,16 @@
         <v>829</v>
       </c>
       <c r="M267" s="35" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="N267" s="35" t="s">
-        <v>871</v>
+        <v>879</v>
       </c>
       <c r="O267" s="35" t="s">
         <v>489</v>
       </c>
       <c r="P267" s="35" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="Q267" s="35" t="s">
         <v>827</v>
@@ -16747,7 +16757,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="116">
+    <row r="268" spans="1:20" ht="115.8" thickBot="1">
       <c r="A268" s="20">
         <v>85</v>
       </c>
@@ -16771,7 +16781,7 @@
         <v>829</v>
       </c>
       <c r="K268" s="35" t="s">
-        <v>872</v>
+        <v>853</v>
       </c>
       <c r="L268" s="35"/>
       <c r="M268" s="35"/>
@@ -16785,7 +16795,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="116">
+    <row r="269" spans="1:20" ht="115.2">
       <c r="A269" s="20">
         <v>86</v>
       </c>
@@ -16809,7 +16819,7 @@
         <v>829</v>
       </c>
       <c r="K269" s="35" t="s">
-        <v>873</v>
+        <v>854</v>
       </c>
       <c r="L269" s="35"/>
       <c r="M269" s="35"/>
@@ -16823,7 +16833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="130.5">
+    <row r="270" spans="1:20" ht="129.6">
       <c r="A270" s="20">
         <v>87</v>
       </c>
@@ -16847,7 +16857,7 @@
         <v>829</v>
       </c>
       <c r="K270" s="35" t="s">
-        <v>874</v>
+        <v>855</v>
       </c>
       <c r="L270" s="35"/>
       <c r="M270" s="35"/>
@@ -16861,7 +16871,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="116">
+    <row r="271" spans="1:20" ht="115.2">
       <c r="A271" s="20">
         <v>88</v>
       </c>
@@ -16885,7 +16895,7 @@
         <v>829</v>
       </c>
       <c r="K271" s="35" t="s">
-        <v>875</v>
+        <v>856</v>
       </c>
       <c r="L271" s="35"/>
       <c r="M271" s="35"/>
@@ -16899,7 +16909,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="101.5">
+    <row r="272" spans="1:20" ht="100.8">
       <c r="A272" s="20">
         <v>89</v>
       </c>
@@ -16923,7 +16933,7 @@
         <v>829</v>
       </c>
       <c r="K272" s="35" t="s">
-        <v>875</v>
+        <v>856</v>
       </c>
       <c r="L272" s="35"/>
       <c r="M272" s="35"/>
@@ -16937,7 +16947,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="101.5">
+    <row r="273" spans="1:20" ht="100.8">
       <c r="A273" s="20">
         <v>90</v>
       </c>
@@ -16961,7 +16971,7 @@
         <v>829</v>
       </c>
       <c r="K273" s="35" t="s">
-        <v>875</v>
+        <v>856</v>
       </c>
       <c r="L273" s="35"/>
       <c r="M273" s="35"/>
@@ -16975,7 +16985,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="116">
+    <row r="274" spans="1:20" ht="115.2">
       <c r="A274" s="20">
         <v>91</v>
       </c>
@@ -16999,7 +17009,7 @@
         <v>829</v>
       </c>
       <c r="K274" s="35" t="s">
-        <v>875</v>
+        <v>856</v>
       </c>
       <c r="L274" s="35"/>
       <c r="M274" s="35"/>
@@ -17013,7 +17023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="116">
+    <row r="275" spans="1:20" ht="115.2">
       <c r="A275" s="20">
         <v>92</v>
       </c>
@@ -17037,7 +17047,7 @@
         <v>829</v>
       </c>
       <c r="K275" s="35" t="s">
-        <v>876</v>
+        <v>857</v>
       </c>
       <c r="L275" s="35"/>
       <c r="M275" s="35"/>
@@ -17051,7 +17061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="116">
+    <row r="276" spans="1:20" ht="115.2">
       <c r="A276" s="20">
         <v>93</v>
       </c>
@@ -17075,7 +17085,7 @@
         <v>829</v>
       </c>
       <c r="K276" s="35" t="s">
-        <v>877</v>
+        <v>858</v>
       </c>
       <c r="L276" s="35"/>
       <c r="M276" s="35"/>
@@ -17089,7 +17099,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="130.5" hidden="1">
+    <row r="277" spans="1:20" ht="129.6" hidden="1">
       <c r="A277" s="20">
         <v>94</v>
       </c>
@@ -17123,7 +17133,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="130.5" hidden="1">
+    <row r="278" spans="1:20" ht="129.6" hidden="1">
       <c r="A278" s="20">
         <v>95</v>
       </c>
@@ -17157,7 +17167,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="101.5" hidden="1">
+    <row r="279" spans="1:20" ht="100.8" hidden="1">
       <c r="A279" s="20">
         <v>96</v>
       </c>
@@ -17191,7 +17201,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="116" hidden="1">
+    <row r="280" spans="1:20" ht="115.2" hidden="1">
       <c r="A280" s="20">
         <v>97</v>
       </c>
@@ -17225,7 +17235,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="130.5" hidden="1">
+    <row r="281" spans="1:20" ht="129.6" hidden="1">
       <c r="A281" s="20">
         <v>98</v>
       </c>
@@ -17259,7 +17269,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="130.5" hidden="1">
+    <row r="282" spans="1:20" ht="129.6" hidden="1">
       <c r="A282" s="20">
         <v>99</v>
       </c>
@@ -17293,7 +17303,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="101.5" hidden="1">
+    <row r="283" spans="1:20" ht="100.8" hidden="1">
       <c r="A283" s="20">
         <v>100</v>
       </c>
@@ -17327,7 +17337,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="116" hidden="1">
+    <row r="284" spans="1:20" ht="115.2" hidden="1">
       <c r="A284" s="20">
         <v>101</v>
       </c>
@@ -17361,7 +17371,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="130.5" hidden="1">
+    <row r="285" spans="1:20" ht="129.6" hidden="1">
       <c r="A285" s="20">
         <v>102</v>
       </c>
@@ -17395,7 +17405,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="130.5" hidden="1">
+    <row r="286" spans="1:20" ht="129.6" hidden="1">
       <c r="A286" s="20">
         <v>103</v>
       </c>
@@ -17429,7 +17439,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="101.5" hidden="1">
+    <row r="287" spans="1:20" ht="100.8" hidden="1">
       <c r="A287" s="20">
         <v>104</v>
       </c>
@@ -17463,7 +17473,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="130.5" hidden="1">
+    <row r="288" spans="1:20" ht="129.6" hidden="1">
       <c r="A288" s="20">
         <v>105</v>
       </c>
@@ -17497,7 +17507,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="130.5" hidden="1">
+    <row r="289" spans="1:20" ht="129.6" hidden="1">
       <c r="A289" s="20">
         <v>106</v>
       </c>
@@ -17531,7 +17541,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="116" hidden="1">
+    <row r="290" spans="1:20" ht="115.2" hidden="1">
       <c r="A290" s="20">
         <v>107</v>
       </c>
@@ -17565,7 +17575,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="116" hidden="1">
+    <row r="291" spans="1:20" ht="115.2" hidden="1">
       <c r="A291" s="20">
         <v>108</v>
       </c>
@@ -17599,7 +17609,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="116" hidden="1">
+    <row r="292" spans="1:20" ht="115.2" hidden="1">
       <c r="A292" s="20">
         <v>109</v>
       </c>
@@ -17633,7 +17643,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="101.5" hidden="1">
+    <row r="293" spans="1:20" ht="100.8" hidden="1">
       <c r="A293" s="20">
         <v>110</v>
       </c>
@@ -17667,7 +17677,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="116" hidden="1">
+    <row r="294" spans="1:20" ht="115.2" hidden="1">
       <c r="A294" s="20">
         <v>111</v>
       </c>
@@ -17701,7 +17711,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="116" hidden="1">
+    <row r="295" spans="1:20" ht="115.2" hidden="1">
       <c r="A295" s="20">
         <v>112</v>
       </c>
@@ -17735,7 +17745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="116" hidden="1">
+    <row r="296" spans="1:20" ht="115.2" hidden="1">
       <c r="A296" s="20">
         <v>113</v>
       </c>
@@ -17769,7 +17779,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="116" hidden="1">
+    <row r="297" spans="1:20" ht="115.2" hidden="1">
       <c r="A297" s="20">
         <v>114</v>
       </c>
@@ -17803,7 +17813,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="116" hidden="1">
+    <row r="298" spans="1:20" ht="115.2" hidden="1">
       <c r="A298" s="20">
         <v>115</v>
       </c>
@@ -17837,7 +17847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="116" hidden="1">
+    <row r="299" spans="1:20" ht="115.2" hidden="1">
       <c r="A299" s="20">
         <v>116</v>
       </c>
@@ -17871,7 +17881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="116" hidden="1">
+    <row r="300" spans="1:20" ht="115.2" hidden="1">
       <c r="A300" s="20">
         <v>117</v>
       </c>
@@ -17905,7 +17915,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="116" hidden="1">
+    <row r="301" spans="1:20" ht="115.2" hidden="1">
       <c r="A301" s="20">
         <v>118</v>
       </c>
@@ -17939,7 +17949,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="116" hidden="1">
+    <row r="302" spans="1:20" ht="115.2" hidden="1">
       <c r="A302" s="20">
         <v>119</v>
       </c>
@@ -17973,7 +17983,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="116" hidden="1">
+    <row r="303" spans="1:20" ht="115.2" hidden="1">
       <c r="A303" s="20">
         <v>120</v>
       </c>
@@ -18007,7 +18017,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="116" hidden="1">
+    <row r="304" spans="1:20" ht="115.2" hidden="1">
       <c r="A304" s="20">
         <v>121</v>
       </c>
@@ -18041,7 +18051,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="101.5" hidden="1">
+    <row r="305" spans="1:20" ht="100.8" hidden="1">
       <c r="A305" s="20">
         <v>122</v>
       </c>
@@ -18075,7 +18085,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="101.5" hidden="1">
+    <row r="306" spans="1:20" ht="100.8" hidden="1">
       <c r="A306" s="20">
         <v>123</v>
       </c>
@@ -18109,7 +18119,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="101.5" hidden="1">
+    <row r="307" spans="1:20" ht="100.8" hidden="1">
       <c r="A307" s="20">
         <v>124</v>
       </c>
@@ -18143,7 +18153,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="116" hidden="1">
+    <row r="308" spans="1:20" ht="115.2" hidden="1">
       <c r="A308" s="20">
         <v>125</v>
       </c>
@@ -18177,7 +18187,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="101.5" hidden="1">
+    <row r="309" spans="1:20" ht="100.8" hidden="1">
       <c r="A309" s="20">
         <v>126</v>
       </c>
@@ -18211,7 +18221,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="101.5" hidden="1">
+    <row r="310" spans="1:20" ht="100.8" hidden="1">
       <c r="A310" s="20">
         <v>127</v>
       </c>
@@ -18245,7 +18255,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="101.5" hidden="1">
+    <row r="311" spans="1:20" ht="100.8" hidden="1">
       <c r="A311" s="20">
         <v>128</v>
       </c>
@@ -18279,7 +18289,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="116" hidden="1">
+    <row r="312" spans="1:20" ht="115.2" hidden="1">
       <c r="A312" s="20">
         <v>129</v>
       </c>
@@ -18313,7 +18323,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="101.5" hidden="1">
+    <row r="313" spans="1:20" ht="100.8" hidden="1">
       <c r="A313" s="20">
         <v>130</v>
       </c>
@@ -18347,7 +18357,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="101.5" hidden="1">
+    <row r="314" spans="1:20" ht="100.8" hidden="1">
       <c r="A314" s="20">
         <v>131</v>
       </c>
@@ -18381,7 +18391,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="101.5" hidden="1">
+    <row r="315" spans="1:20" ht="100.8" hidden="1">
       <c r="A315" s="20">
         <v>132</v>
       </c>
@@ -18415,7 +18425,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="116" hidden="1">
+    <row r="316" spans="1:20" ht="115.2" hidden="1">
       <c r="A316" s="20">
         <v>133</v>
       </c>
@@ -18449,7 +18459,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="101.5" hidden="1">
+    <row r="317" spans="1:20" ht="100.8" hidden="1">
       <c r="A317" s="20">
         <v>134</v>
       </c>
@@ -18483,7 +18493,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="101.5" hidden="1">
+    <row r="318" spans="1:20" ht="100.8" hidden="1">
       <c r="A318" s="20">
         <v>135</v>
       </c>
@@ -18517,7 +18527,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="101.5" hidden="1">
+    <row r="319" spans="1:20" ht="100.8" hidden="1">
       <c r="A319" s="20">
         <v>136</v>
       </c>
@@ -18551,7 +18561,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="116" hidden="1">
+    <row r="320" spans="1:20" ht="115.2" hidden="1">
       <c r="A320" s="20">
         <v>137</v>
       </c>
@@ -18585,7 +18595,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="101.5" hidden="1">
+    <row r="321" spans="1:20" ht="100.8" hidden="1">
       <c r="A321" s="20">
         <v>138</v>
       </c>
@@ -18619,7 +18629,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="101.5" hidden="1">
+    <row r="322" spans="1:20" ht="100.8" hidden="1">
       <c r="A322" s="20">
         <v>139</v>
       </c>
@@ -18653,7 +18663,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="101.5" hidden="1">
+    <row r="323" spans="1:20" ht="100.8" hidden="1">
       <c r="A323" s="20">
         <v>140</v>
       </c>
@@ -18687,7 +18697,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="116" hidden="1">
+    <row r="324" spans="1:20" ht="115.2" hidden="1">
       <c r="A324" s="20">
         <v>141</v>
       </c>
@@ -18721,7 +18731,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="101.5" hidden="1">
+    <row r="325" spans="1:20" ht="100.8" hidden="1">
       <c r="A325" s="20">
         <v>142</v>
       </c>
@@ -18755,7 +18765,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="101.5" hidden="1">
+    <row r="326" spans="1:20" ht="100.8" hidden="1">
       <c r="A326" s="20">
         <v>143</v>
       </c>
@@ -18789,7 +18799,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="101.5" hidden="1">
+    <row r="327" spans="1:20" ht="100.8" hidden="1">
       <c r="A327" s="20">
         <v>144</v>
       </c>
@@ -18823,7 +18833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="116" hidden="1">
+    <row r="328" spans="1:20" ht="115.2" hidden="1">
       <c r="A328" s="20">
         <v>145</v>
       </c>
@@ -18857,7 +18867,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="329" spans="1:20" ht="116" hidden="1">
+    <row r="329" spans="1:20" ht="115.2" hidden="1">
       <c r="A329" s="20">
         <v>146</v>
       </c>
@@ -18891,7 +18901,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="159.5" hidden="1">
+    <row r="330" spans="1:20" ht="158.4" hidden="1">
       <c r="A330" s="20">
         <v>147</v>
       </c>
@@ -18925,7 +18935,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="159.5" hidden="1">
+    <row r="331" spans="1:20" ht="158.4" hidden="1">
       <c r="A331" s="20">
         <v>148</v>
       </c>
@@ -18959,7 +18969,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="159.5" hidden="1">
+    <row r="332" spans="1:20" ht="158.4" hidden="1">
       <c r="A332" s="20">
         <v>149</v>
       </c>
@@ -18993,7 +19003,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="159.5" hidden="1">
+    <row r="333" spans="1:20" ht="158.4" hidden="1">
       <c r="A333" s="20">
         <v>150</v>
       </c>
@@ -19027,7 +19037,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="101.5" hidden="1">
+    <row r="334" spans="1:20" ht="100.8" hidden="1">
       <c r="A334" s="20">
         <v>151</v>
       </c>
@@ -19061,7 +19071,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="116" hidden="1">
+    <row r="335" spans="1:20" ht="115.2" hidden="1">
       <c r="A335" s="20">
         <v>152</v>
       </c>
@@ -19095,7 +19105,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="116" hidden="1">
+    <row r="336" spans="1:20" ht="115.2" hidden="1">
       <c r="A336" s="20">
         <v>153</v>
       </c>
@@ -19129,7 +19139,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="116" hidden="1">
+    <row r="337" spans="1:20" ht="115.2" hidden="1">
       <c r="A337" s="20">
         <v>154</v>
       </c>
@@ -19163,7 +19173,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="116" hidden="1">
+    <row r="338" spans="1:20" ht="115.2" hidden="1">
       <c r="A338" s="20">
         <v>155</v>
       </c>
@@ -19197,7 +19207,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="116" hidden="1">
+    <row r="339" spans="1:20" ht="115.2" hidden="1">
       <c r="A339" s="20">
         <v>156</v>
       </c>
@@ -19231,7 +19241,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="116" hidden="1">
+    <row r="340" spans="1:20" ht="115.2" hidden="1">
       <c r="A340" s="20">
         <v>157</v>
       </c>
@@ -19265,7 +19275,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="116" hidden="1">
+    <row r="341" spans="1:20" ht="115.2" hidden="1">
       <c r="A341" s="20">
         <v>158</v>
       </c>
@@ -19299,7 +19309,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="101.5" hidden="1">
+    <row r="342" spans="1:20" ht="100.8" hidden="1">
       <c r="A342" s="20">
         <v>159</v>
       </c>
@@ -19333,7 +19343,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="101.5" hidden="1">
+    <row r="343" spans="1:20" ht="100.8" hidden="1">
       <c r="A343" s="20">
         <v>160</v>
       </c>
@@ -19367,7 +19377,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="116" hidden="1">
+    <row r="344" spans="1:20" ht="115.2" hidden="1">
       <c r="A344" s="20">
         <v>161</v>
       </c>
@@ -19401,7 +19411,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="116" hidden="1">
+    <row r="345" spans="1:20" ht="115.2" hidden="1">
       <c r="A345" s="20">
         <v>162</v>
       </c>
@@ -19435,7 +19445,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="116" hidden="1">
+    <row r="346" spans="1:20" ht="115.2" hidden="1">
       <c r="A346" s="20">
         <v>163</v>
       </c>
@@ -19469,7 +19479,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="116" hidden="1">
+    <row r="347" spans="1:20" ht="115.2" hidden="1">
       <c r="A347" s="20">
         <v>164</v>
       </c>
@@ -19503,7 +19513,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="116" hidden="1">
+    <row r="348" spans="1:20" ht="115.2" hidden="1">
       <c r="A348" s="20">
         <v>165</v>
       </c>
@@ -19537,7 +19547,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="116" hidden="1">
+    <row r="349" spans="1:20" ht="115.2" hidden="1">
       <c r="A349" s="20">
         <v>166</v>
       </c>
@@ -19571,7 +19581,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="116" hidden="1">
+    <row r="350" spans="1:20" ht="115.2" hidden="1">
       <c r="A350" s="20">
         <v>167</v>
       </c>
@@ -19605,7 +19615,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="116" hidden="1">
+    <row r="351" spans="1:20" ht="115.2" hidden="1">
       <c r="A351" s="20">
         <v>168</v>
       </c>
@@ -19639,7 +19649,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="116" hidden="1">
+    <row r="352" spans="1:20" ht="115.2" hidden="1">
       <c r="A352" s="20">
         <v>169</v>
       </c>
@@ -19673,7 +19683,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="145" hidden="1">
+    <row r="353" spans="1:20" ht="144" hidden="1">
       <c r="A353" s="20">
         <v>170</v>
       </c>
@@ -19707,7 +19717,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="145" hidden="1">
+    <row r="354" spans="1:20" ht="144" hidden="1">
       <c r="A354" s="20">
         <v>171</v>
       </c>
@@ -19741,7 +19751,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="145" hidden="1">
+    <row r="355" spans="1:20" ht="144" hidden="1">
       <c r="A355" s="20">
         <v>172</v>
       </c>
@@ -19775,7 +19785,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="145" hidden="1">
+    <row r="356" spans="1:20" ht="144" hidden="1">
       <c r="A356" s="20">
         <v>173</v>
       </c>
@@ -19809,7 +19819,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="101.5" hidden="1">
+    <row r="357" spans="1:20" ht="100.8" hidden="1">
       <c r="A357" s="20">
         <v>174</v>
       </c>
@@ -19843,7 +19853,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="116" hidden="1">
+    <row r="358" spans="1:20" ht="115.2" hidden="1">
       <c r="A358" s="20">
         <v>175</v>
       </c>
@@ -19877,7 +19887,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="116" hidden="1">
+    <row r="359" spans="1:20" ht="115.2" hidden="1">
       <c r="A359" s="20">
         <v>176</v>
       </c>
@@ -19911,7 +19921,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="360" spans="1:20" ht="116" hidden="1">
+    <row r="360" spans="1:20" ht="115.2" hidden="1">
       <c r="A360" s="20">
         <v>177</v>
       </c>
@@ -19945,7 +19955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="116" hidden="1">
+    <row r="361" spans="1:20" ht="115.2" hidden="1">
       <c r="A361" s="20">
         <v>178</v>
       </c>
@@ -19979,7 +19989,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="116" hidden="1">
+    <row r="362" spans="1:20" ht="115.2" hidden="1">
       <c r="A362" s="20">
         <v>179</v>
       </c>
@@ -20013,7 +20023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="116" hidden="1">
+    <row r="363" spans="1:20" ht="115.2" hidden="1">
       <c r="A363" s="20">
         <v>180</v>
       </c>
@@ -20047,7 +20057,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="101.5" hidden="1">
+    <row r="364" spans="1:20" ht="100.8" hidden="1">
       <c r="A364" s="20">
         <v>181</v>
       </c>
@@ -20081,7 +20091,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="116" hidden="1">
+    <row r="365" spans="1:20" ht="115.2" hidden="1">
       <c r="A365" s="20">
         <v>182</v>
       </c>
@@ -20115,7 +20125,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="116" hidden="1">
+    <row r="366" spans="1:20" ht="115.2" hidden="1">
       <c r="A366" s="20">
         <v>183</v>
       </c>
@@ -20149,7 +20159,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="116" hidden="1">
+    <row r="367" spans="1:20" ht="115.2" hidden="1">
       <c r="A367" s="20">
         <v>184</v>
       </c>
@@ -20183,7 +20193,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="116" hidden="1">
+    <row r="368" spans="1:20" ht="115.2" hidden="1">
       <c r="A368" s="20">
         <v>185</v>
       </c>
@@ -20217,7 +20227,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="116" hidden="1">
+    <row r="369" spans="1:20" ht="115.2" hidden="1">
       <c r="A369" s="20">
         <v>186</v>
       </c>
@@ -20251,7 +20261,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="116" hidden="1">
+    <row r="370" spans="1:20" ht="115.2" hidden="1">
       <c r="A370" s="20">
         <v>187</v>
       </c>
@@ -20285,7 +20295,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="116" hidden="1">
+    <row r="371" spans="1:20" ht="115.2" hidden="1">
       <c r="A371" s="20">
         <v>188</v>
       </c>
@@ -20319,7 +20329,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="116" hidden="1">
+    <row r="372" spans="1:20" ht="115.2" hidden="1">
       <c r="A372" s="20">
         <v>189</v>
       </c>
@@ -20353,7 +20363,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="116" hidden="1">
+    <row r="373" spans="1:20" ht="115.2" hidden="1">
       <c r="A373" s="20">
         <v>190</v>
       </c>
@@ -20387,7 +20397,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="145" hidden="1">
+    <row r="374" spans="1:20" ht="144" hidden="1">
       <c r="A374" s="20">
         <v>191</v>
       </c>
@@ -30038,8 +30048,8 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -30070,15 +30080,15 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="23.90625" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
     <col min="4" max="4" width="102" customWidth="1"/>
-    <col min="5" max="6" width="8.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" customWidth="1"/>
-    <col min="8" max="26" width="8.90625" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
@@ -30165,7 +30175,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.5">
+    <row r="7" spans="1:4" ht="14.4">
       <c r="A7" s="11" t="s">
         <v>72</v>
       </c>
@@ -30179,7 +30189,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.5">
+    <row r="8" spans="1:4" ht="14.4">
       <c r="A8" s="11" t="s">
         <v>77</v>
       </c>
@@ -30193,7 +30203,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.5">
+    <row r="9" spans="1:4" ht="14.4">
       <c r="A9" s="11" t="s">
         <v>82</v>
       </c>
@@ -31740,11 +31750,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="26" width="8.90625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -32782,23 +32792,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="49919dca-d9c1-492f-bd36-8a887e31a6e3" xsi:nil="true"/>
-    <Tag xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ContentTypeId="0x01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -32807,9 +32800,9 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A052E4B0CBFBEE42A9BE94735C648D6A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4e5f9d650d253b7a3d6ed53057f6e63e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xmlns:ns3="bb0bfb2d-9415-422c-9311-cf5d9d9d5142" xmlns:ns4="49919dca-d9c1-492f-bd36-8a887e31a6e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d80d0c74ac61bb9026b243c0c584c36" ns2:_="" ns3:_="" ns4:_="">
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A052E4B0CBFBEE42A9BE94735C648D6A" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="06f94ea8854638265dc6ad431c5f7754">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xmlns:ns3="bb0bfb2d-9415-422c-9311-cf5d9d9d5142" xmlns:ns4="49919dca-d9c1-492f-bd36-8a887e31a6e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0729176c5d1fe4fe80f5b7b62f44ef90" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
     <xsd:import namespace="bb0bfb2d-9415-422c-9311-cf5d9d9d5142"/>
     <xsd:import namespace="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
@@ -32833,6 +32826,7 @@
                 <xsd:element ref="ns2:Tag" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -32905,6 +32899,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bb0bfb2d-9415-422c-9311-cf5d9d9d5142" elementFormDefault="qualified">
@@ -33051,26 +33050,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2850EEF4-EC69-4F2E-B0CE-8034B61489F3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
-    <ds:schemaRef ds:uri="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="49919dca-d9c1-492f-bd36-8a887e31a6e3" xsi:nil="true"/>
+    <Tag xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C0D72B-6AAC-4529-B934-502AA3EA2A0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ContentTypeId="0x01" PreviousValue="false"/>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12D86236-EAFC-48DB-B351-E7598A8B8AB2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -33078,8 +33075,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C73319A0-5C18-48A7-95DC-DC52937F884B}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{541AB99F-90C1-41B9-9D99-FB662A21B634}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -33096,4 +33093,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2850EEF4-EC69-4F2E-B0CE-8034B61489F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
+    <ds:schemaRef ds:uri="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C0D72B-6AAC-4529-B934-502AA3EA2A0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chiarimenti per i casi con ID [31, 76, 80, 82, 84]
chiarimenti per i casi con ID [31, 76, 80, 82, 84] - Gestione errori
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111PHILIPSXXXX/Philips/VuePACS-SignPlugin/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111PHILIPSXXXX/Philips/VuePACS-SignPlugin/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.philips.com/sites/HCISIntegration260/Integration Project Docs/EAMER/Italy/FSE 2.0/Accreditamento/file da sottomettere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F65A2B2-A164-4272-B991-C03B9C417839}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9884504A-E773-4C39-A618-70201580750E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2085" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4485,9 +4485,6 @@
     <t>title:"Campo token JWT non valido.","detail":"Il codice fiscale nel campo sub non è corretto","status":403,"instance":"/jwt-mandatory-field-malformed"</t>
   </si>
   <si>
-    <t>Il flusso radiologico (produzione referto e relativa firma digitale) può continuare.</t>
-  </si>
-  <si>
     <t>Non è stato utilizzato il campo purpose_of_use in quanto tale campo non può essere nullo (per come è stato implementato l'applicativo).
 Per il test si è quindi scelto di non valorizzare il codice fiscale.</t>
   </si>
@@ -4606,6 +4603,9 @@
   </si>
   <si>
     <t>"title":"Errore di sintassi.","detail":"ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.","status":400,"instance":"/validation/error"</t>
+  </si>
+  <si>
+    <t>A seguito dell'errore di validazione,lo studio viene marcato per una gestione della problematica in back office. Successivamente alla risoluzione del problema,una nuova firma digitale sarà necessaria per pubblicare il referto su Fascicolo. Il referto viene in ogni caso firmato digitalmente per non bloccare fondamentali flussi radiologici. All'utente non viene visualizzato alcun errore.</t>
   </si>
 </sst>
 </file>
@@ -5143,10 +5143,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7532,10 +7528,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E265" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="J198" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I267" sqref="I267"/>
+      <selection pane="bottomRight" activeCell="P268" sqref="P268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -14099,13 +14095,13 @@
         <v>45085</v>
       </c>
       <c r="G195" s="34" t="s">
+        <v>860</v>
+      </c>
+      <c r="H195" s="34" t="s">
         <v>861</v>
       </c>
-      <c r="H195" s="34" t="s">
+      <c r="I195" s="34" t="s">
         <v>862</v>
-      </c>
-      <c r="I195" s="34" t="s">
-        <v>863</v>
       </c>
       <c r="J195" s="35" t="s">
         <v>489</v>
@@ -14749,7 +14745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="214" spans="1:20" ht="202.2" thickBot="1">
       <c r="A214" s="20">
         <v>31</v>
       </c>
@@ -14794,14 +14790,14 @@
         <v>489</v>
       </c>
       <c r="P214" s="35" t="s">
-        <v>842</v>
+        <v>879</v>
       </c>
       <c r="Q214" s="35" t="s">
         <v>827</v>
       </c>
       <c r="R214" s="36"/>
       <c r="S214" s="37" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="T214" s="28" t="s">
         <v>51</v>
@@ -15069,7 +15065,7 @@
         <v>829</v>
       </c>
       <c r="K222" s="35" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="L222" s="35"/>
       <c r="M222" s="35"/>
@@ -15347,7 +15343,7 @@
         <v>45063</v>
       </c>
       <c r="G230" s="34" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H230" s="34"/>
       <c r="I230" s="34"/>
@@ -15362,7 +15358,7 @@
         <v>829</v>
       </c>
       <c r="P230" s="35" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="Q230" s="35" t="s">
         <v>827</v>
@@ -16323,7 +16319,7 @@
         <v>829</v>
       </c>
       <c r="K258" s="35" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="L258" s="35"/>
       <c r="M258" s="35"/>
@@ -16337,7 +16333,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="115.8" thickBot="1">
+    <row r="259" spans="1:20" ht="202.2" thickBot="1">
       <c r="A259" s="20">
         <v>76</v>
       </c>
@@ -16357,13 +16353,13 @@
         <v>45085</v>
       </c>
       <c r="G259" s="34" t="s">
+        <v>863</v>
+      </c>
+      <c r="H259" s="34" t="s">
         <v>864</v>
       </c>
-      <c r="H259" s="34" t="s">
+      <c r="I259" s="34" t="s">
         <v>865</v>
-      </c>
-      <c r="I259" s="34" t="s">
-        <v>866</v>
       </c>
       <c r="J259" s="35" t="s">
         <v>489</v>
@@ -16376,20 +16372,20 @@
         <v>840</v>
       </c>
       <c r="N259" s="35" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="O259" s="35" t="s">
         <v>489</v>
       </c>
       <c r="P259" s="35" t="s">
-        <v>842</v>
+        <v>879</v>
       </c>
       <c r="Q259" s="35" t="s">
         <v>827</v>
       </c>
       <c r="R259" s="36"/>
       <c r="S259" s="37" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="T259" s="28" t="s">
         <v>51</v>
@@ -16419,7 +16415,7 @@
         <v>829</v>
       </c>
       <c r="K260" s="35" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="L260" s="35"/>
       <c r="M260" s="35"/>
@@ -16457,7 +16453,7 @@
         <v>829</v>
       </c>
       <c r="K261" s="35" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="L261" s="35"/>
       <c r="M261" s="35"/>
@@ -16495,7 +16491,7 @@
         <v>829</v>
       </c>
       <c r="K262" s="35" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="L262" s="35"/>
       <c r="M262" s="35"/>
@@ -16509,7 +16505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="115.2">
+    <row r="263" spans="1:20" ht="201.6">
       <c r="A263" s="20">
         <v>80</v>
       </c>
@@ -16529,13 +16525,13 @@
         <v>45085</v>
       </c>
       <c r="G263" s="34" t="s">
+        <v>867</v>
+      </c>
+      <c r="H263" s="34" t="s">
         <v>868</v>
       </c>
-      <c r="H263" s="34" t="s">
+      <c r="I263" s="34" t="s">
         <v>869</v>
-      </c>
-      <c r="I263" s="34" t="s">
-        <v>870</v>
       </c>
       <c r="J263" s="35" t="s">
         <v>489</v>
@@ -16548,20 +16544,20 @@
         <v>840</v>
       </c>
       <c r="N263" s="35" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="O263" s="35" t="s">
         <v>489</v>
       </c>
       <c r="P263" s="35" t="s">
-        <v>842</v>
+        <v>879</v>
       </c>
       <c r="Q263" s="35" t="s">
         <v>827</v>
       </c>
       <c r="R263" s="36"/>
       <c r="S263" s="37" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="T263" s="28" t="s">
         <v>51</v>
@@ -16591,7 +16587,7 @@
         <v>829</v>
       </c>
       <c r="K264" s="35" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="L264" s="35"/>
       <c r="M264" s="35"/>
@@ -16605,7 +16601,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="265" spans="1:20" ht="202.2" thickBot="1">
       <c r="A265" s="20">
         <v>82</v>
       </c>
@@ -16625,13 +16621,13 @@
         <v>45085</v>
       </c>
       <c r="G265" s="34" t="s">
+        <v>871</v>
+      </c>
+      <c r="H265" s="38" t="s">
         <v>872</v>
       </c>
-      <c r="H265" s="38" t="s">
+      <c r="I265" s="34" t="s">
         <v>873</v>
-      </c>
-      <c r="I265" s="34" t="s">
-        <v>874</v>
       </c>
       <c r="J265" s="35" t="s">
         <v>489</v>
@@ -16644,20 +16640,20 @@
         <v>840</v>
       </c>
       <c r="N265" s="35" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="O265" s="35" t="s">
         <v>489</v>
       </c>
       <c r="P265" s="35" t="s">
-        <v>842</v>
+        <v>879</v>
       </c>
       <c r="Q265" s="35" t="s">
         <v>827</v>
       </c>
       <c r="R265" s="36"/>
       <c r="S265" s="37" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="T265" s="28" t="s">
         <v>51</v>
@@ -16687,7 +16683,7 @@
         <v>829</v>
       </c>
       <c r="K266" s="35" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="L266" s="35"/>
       <c r="M266" s="35"/>
@@ -16701,7 +16697,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="267" spans="1:20" ht="202.2" thickBot="1">
       <c r="A267" s="20">
         <v>84</v>
       </c>
@@ -16721,13 +16717,13 @@
         <v>45085</v>
       </c>
       <c r="G267" s="34" t="s">
+        <v>875</v>
+      </c>
+      <c r="H267" s="34" t="s">
         <v>876</v>
       </c>
-      <c r="H267" s="34" t="s">
+      <c r="I267" s="34" t="s">
         <v>877</v>
-      </c>
-      <c r="I267" s="34" t="s">
-        <v>878</v>
       </c>
       <c r="J267" s="35" t="s">
         <v>489</v>
@@ -16740,13 +16736,13 @@
         <v>840</v>
       </c>
       <c r="N267" s="35" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="O267" s="35" t="s">
         <v>489</v>
       </c>
       <c r="P267" s="35" t="s">
-        <v>842</v>
+        <v>879</v>
       </c>
       <c r="Q267" s="35" t="s">
         <v>827</v>
@@ -16781,7 +16777,7 @@
         <v>829</v>
       </c>
       <c r="K268" s="35" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="L268" s="35"/>
       <c r="M268" s="35"/>
@@ -16819,7 +16815,7 @@
         <v>829</v>
       </c>
       <c r="K269" s="35" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="L269" s="35"/>
       <c r="M269" s="35"/>
@@ -16857,7 +16853,7 @@
         <v>829</v>
       </c>
       <c r="K270" s="35" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="L270" s="35"/>
       <c r="M270" s="35"/>
@@ -16895,7 +16891,7 @@
         <v>829</v>
       </c>
       <c r="K271" s="35" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="L271" s="35"/>
       <c r="M271" s="35"/>
@@ -16933,7 +16929,7 @@
         <v>829</v>
       </c>
       <c r="K272" s="35" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="L272" s="35"/>
       <c r="M272" s="35"/>
@@ -16971,7 +16967,7 @@
         <v>829</v>
       </c>
       <c r="K273" s="35" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="L273" s="35"/>
       <c r="M273" s="35"/>
@@ -17009,7 +17005,7 @@
         <v>829</v>
       </c>
       <c r="K274" s="35" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="L274" s="35"/>
       <c r="M274" s="35"/>
@@ -17047,7 +17043,7 @@
         <v>829</v>
       </c>
       <c r="K275" s="35" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="L275" s="35"/>
       <c r="M275" s="35"/>
@@ -17085,7 +17081,7 @@
         <v>829</v>
       </c>
       <c r="K276" s="35" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="L276" s="35"/>
       <c r="M276" s="35"/>
@@ -32793,14 +32789,22 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ContentTypeId="0x01" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="49919dca-d9c1-492f-bd36-8a887e31a6e3" xsi:nil="true"/>
+    <Tag xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A052E4B0CBFBEE42A9BE94735C648D6A" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="06f94ea8854638265dc6ad431c5f7754">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xmlns:ns3="bb0bfb2d-9415-422c-9311-cf5d9d9d5142" xmlns:ns4="49919dca-d9c1-492f-bd36-8a887e31a6e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0729176c5d1fe4fe80f5b7b62f44ef90" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
@@ -33050,32 +33054,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="49919dca-d9c1-492f-bd36-8a887e31a6e3" xsi:nil="true"/>
-    <Tag xmlns="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="e40374fb-a6cc-4854-989f-c1d94a7967ee" ContentTypeId="0x01" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12D86236-EAFC-48DB-B351-E7598A8B8AB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C0D72B-6AAC-4529-B934-502AA3EA2A0C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2850EEF4-EC69-4F2E-B0CE-8034B61489F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
+    <ds:schemaRef ds:uri="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{541AB99F-90C1-41B9-9D99-FB662A21B634}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33095,21 +33102,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2850EEF4-EC69-4F2E-B0CE-8034B61489F3}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12D86236-EAFC-48DB-B351-E7598A8B8AB2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2fbb41f8-148e-47b2-8bb2-53dd0d6e062d"/>
-    <ds:schemaRef ds:uri="49919dca-d9c1-492f-bd36-8a887e31a6e3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C0D72B-6AAC-4529-B934-502AA3EA2A0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>